<commit_message>
SDLT RPM update code pushed
</commit_message>
<xml_diff>
--- a/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
+++ b/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Taylors\DocumentUnderstandingFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D18E77-04A9-4248-A438-2F387D95811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCA9BB-BA6A-4EFE-83DC-5C38EC011466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>Insight Ref</t>
   </si>
@@ -274,299 +274,71 @@
     <t>No</t>
   </si>
   <si>
-    <t>Leasehold</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Harrow</t>
-  </si>
-  <si>
-    <t>HA1 4BF</t>
-  </si>
-  <si>
-    <t>HARROW VIEW LLP</t>
-  </si>
-  <si>
-    <t>NBT1800</t>
-  </si>
-  <si>
-    <t>Parisa Baroudy</t>
-  </si>
-  <si>
-    <t>Schuurstraat 61 , Sint- Amandsberg Belgium 9040</t>
-  </si>
-  <si>
-    <t>Flat 8 Dodson House 13 Medawar Drive Mill Hill NW7 1WG</t>
-  </si>
-  <si>
-    <t>BDW TRADING LIMITED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barratt House, Cartwright Way, Forest Business Park, Bardon Hill, Coalville, Leicestershire LE67 1 UF </t>
-  </si>
-  <si>
-    <t>05/01/2018</t>
-  </si>
-  <si>
-    <t>04/30/3017</t>
-  </si>
-  <si>
-    <t>Parisa</t>
-  </si>
-  <si>
-    <t>Baroudy</t>
-  </si>
-  <si>
-    <t>Flat 8 Dodson House 13 Medawar Drive Mill Hill</t>
-  </si>
-  <si>
-    <t>NW7 1WG</t>
-  </si>
-  <si>
-    <t>SJ957962C</t>
-  </si>
-  <si>
-    <t>NBT1799</t>
-  </si>
-  <si>
-    <t>Flat 4 Dodson House 13 Medawar Drive Mill hill NW7 1WG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 4 Dodson House 13 Medawar Drive Mill hill </t>
-  </si>
-  <si>
-    <t>NBT1580</t>
-  </si>
-  <si>
-    <t>Rohan Bomle</t>
-  </si>
-  <si>
-    <t>Flat 22, Taro Apartments Henry Strong Road Harrow HA1 4BF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barratt House, Cartwright Way, Forest Business Park, Bardon Hill, Coalville, Leicestershire, LE67 1 UF </t>
-  </si>
-  <si>
-    <t>Rohan</t>
-  </si>
-  <si>
-    <t>Kashmira</t>
-  </si>
-  <si>
-    <t>Naresh</t>
-  </si>
-  <si>
-    <t>Bomle</t>
-  </si>
-  <si>
-    <t>Dawal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HARROW VIEW LLP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 22, Taro Apartments Henry Strong Road Harrow </t>
-  </si>
-  <si>
-    <t>Kashmira Naresh Dawal</t>
-  </si>
-  <si>
-    <t>SX247433B</t>
-  </si>
-  <si>
-    <t>SZ320421B</t>
-  </si>
-  <si>
-    <t>NBT1712</t>
-  </si>
-  <si>
-    <t>Vament Chan</t>
-  </si>
-  <si>
-    <t>Flat 63 Taro Apartments Henry Strong Road Harrow HA1 4BF</t>
-  </si>
-  <si>
-    <t>Vament</t>
-  </si>
-  <si>
-    <t>Ching</t>
-  </si>
-  <si>
-    <t>Yee</t>
-  </si>
-  <si>
-    <t>Chan</t>
-  </si>
-  <si>
-    <t>Ng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 63 Taro Apartments Henry Strong Road Harrow </t>
-  </si>
-  <si>
-    <t>Ching Yee Ng</t>
-  </si>
-  <si>
-    <t>NJ855536A</t>
-  </si>
-  <si>
-    <t>NJ862921B</t>
-  </si>
-  <si>
-    <t>NBT1794</t>
-  </si>
-  <si>
-    <t>Vizion Homes Ltd</t>
-  </si>
-  <si>
-    <t>Brentano Suite 390 Catalyst House 720 Centennial Court Centennial Park Elstree WD6 3SY</t>
-  </si>
-  <si>
-    <t>Flat 33 Dodson House, 13 Medawar Drive Mill hill NW7 1WG</t>
-  </si>
-  <si>
-    <t>Barratt House, Cartwright Way, Forest Business Park, Bardon Hill, Coalville, Leicestershire LE67 1UF</t>
-  </si>
-  <si>
-    <t>03/01/2018</t>
-  </si>
-  <si>
-    <t>02/28/3017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 33 Dodson House, 13 Medawar Drive Mill hill </t>
-  </si>
-  <si>
-    <t>NBT1339</t>
-  </si>
-  <si>
-    <t>Alexander Syal</t>
-  </si>
-  <si>
-    <t>3 Osborn Gardens Mill Hill London NW7 1DY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 52, Dodson House 13 Medawar Drive Mill Hill </t>
-  </si>
-  <si>
-    <t>Barnet</t>
-  </si>
-  <si>
-    <t>BOW TRADING LIMITED</t>
-  </si>
-  <si>
-    <t>Alexander</t>
-  </si>
-  <si>
-    <t>Syal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOW TRADING LIMITED </t>
-  </si>
-  <si>
-    <t>Flat 52, Dodson House 13 Medawar Drive Mill Hill</t>
-  </si>
-  <si>
-    <t>PW889479D</t>
-  </si>
-  <si>
-    <t>NBT896</t>
-  </si>
-  <si>
-    <t>Amir Ghani Properties Ltd</t>
-  </si>
-  <si>
-    <t>33 Malvern Gardens Harrow HA3 9PA</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Flat 67 Taro Aprtments Henry Strong Road Harrow United Kingdom</t>
-  </si>
-  <si>
-    <t>NBT1826</t>
-  </si>
-  <si>
-    <t>Benjamin Philip Laws</t>
-  </si>
-  <si>
-    <t>FLAT 54 Taro Apartments Henry Strong Road Harrow HA1 4BF</t>
-  </si>
-  <si>
-    <t>FLAT 54 Taro Apartments Henry Strong Road Harrow</t>
-  </si>
-  <si>
-    <t>04/20/3017</t>
-  </si>
-  <si>
-    <t>Benjamin</t>
-  </si>
-  <si>
-    <t>Sneha</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>Laws</t>
-  </si>
-  <si>
-    <t>Chattopadhyay</t>
-  </si>
-  <si>
-    <t>Sneha Chattopadhyay</t>
-  </si>
-  <si>
-    <t>PA175317B</t>
-  </si>
-  <si>
-    <t>SX119256A</t>
-  </si>
-  <si>
-    <t>NBT1744</t>
-  </si>
-  <si>
-    <t>Harbhajan Singh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">136 SANDWELL ROAD HANDSWORTH BIRMINGHAM B21 BPS </t>
-  </si>
-  <si>
-    <t>Flat 35 Taro Apartments Henry Strong Road Harrow</t>
-  </si>
-  <si>
-    <t>Harbhajan</t>
-  </si>
-  <si>
-    <t>Harvinder</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
-    <t>Sidhu</t>
-  </si>
-  <si>
-    <t>Harvinder Sidhu</t>
-  </si>
-  <si>
-    <t>24 High Street West Bromwich B70 6JX</t>
-  </si>
-  <si>
-    <t>JC631037B</t>
-  </si>
-  <si>
-    <t>PC127552A</t>
+    <t>Freehold</t>
+  </si>
+  <si>
+    <t>MRT1723</t>
+  </si>
+  <si>
+    <t>Katarzyna Maria Szczerba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17B Church Rise, London, </t>
+  </si>
+  <si>
+    <t>Lewisham</t>
+  </si>
+  <si>
+    <t>Michael Brian Wood</t>
+  </si>
+  <si>
+    <t>17b Church Rise, Forest Hill, London, SE23 2UD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Katarzyna Maria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pierre Mathieu </t>
+  </si>
+  <si>
+    <t>Szczerba</t>
+  </si>
+  <si>
+    <t>Blacque- Florentin</t>
+  </si>
+  <si>
+    <t>SGL507353</t>
+  </si>
+  <si>
+    <t>Michael Brian Wood and Claire Jessica Harding</t>
+  </si>
+  <si>
+    <t>17B Church Rise, London</t>
+  </si>
+  <si>
+    <t>SE23 2UD</t>
+  </si>
+  <si>
+    <t>Claire Jessica Harding</t>
+  </si>
+  <si>
+    <t>17B Church Rise, Forest Hill, London, SE23 2UD</t>
+  </si>
+  <si>
+    <t>Pierre Mathieu Blacque- Florentin</t>
+  </si>
+  <si>
+    <t>SN352872A</t>
+  </si>
+  <si>
+    <t>SN382090C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="96" x14ac:knownFonts="1">
+  <fonts count="99" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1237,6 +1009,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1256,13 +1048,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2329">
+  <cellStyleXfs count="2439">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
@@ -1288,6 +1092,8 @@
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
@@ -1329,6 +1135,8 @@
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
@@ -1400,6 +1208,7 @@
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
@@ -1408,6 +1217,10 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
@@ -1427,6 +1240,10 @@
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
@@ -1450,6 +1267,10 @@
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
@@ -1477,6 +1298,10 @@
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
@@ -1508,6 +1333,10 @@
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
@@ -1543,6 +1372,9 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
@@ -1642,6 +1474,8 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
@@ -1683,6 +1517,8 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
@@ -1748,6 +1584,8 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
@@ -1793,6 +1631,9 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
@@ -1840,6 +1681,11 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
@@ -2054,6 +1900,8 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
@@ -2109,6 +1957,8 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
@@ -2195,6 +2045,7 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
@@ -2224,6 +2075,10 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
@@ -2285,6 +2140,12 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
@@ -2351,6 +2212,13 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
@@ -2423,6 +2291,11 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
@@ -2502,6 +2375,9 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -2585,6 +2461,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
@@ -2670,6 +2549,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
@@ -2802,7 +2683,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
@@ -2847,6 +2727,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
@@ -3025,6 +2907,11 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -3118,6 +3005,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -3215,6 +3106,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -3371,6 +3269,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -3532,6 +3432,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -3587,14 +3489,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2329">
+  <cellStyles count="2439">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="159" xr:uid="{22378139-A9D0-4012-B7E1-FB95B8397E06}"/>
     <cellStyle name="Normal 10 10" xfId="276" xr:uid="{2FF1057A-C0FD-428A-B8F5-F70C6C4ED22C}"/>
@@ -3663,6 +3568,8 @@
     <cellStyle name="Normal 10 68" xfId="2229" xr:uid="{A8691793-BE7C-480D-83AD-19DF1C5D3EB0}"/>
     <cellStyle name="Normal 10 69" xfId="2283" xr:uid="{F58A0D10-DBA6-430C-AB4E-C6C36BF07EBF}"/>
     <cellStyle name="Normal 10 7" xfId="228" xr:uid="{267F1CFF-9F4B-436A-AEEC-36F3EF937E54}"/>
+    <cellStyle name="Normal 10 70" xfId="2337" xr:uid="{6AF9F2A8-BD6D-4090-98D2-C3FA834F8D6A}"/>
+    <cellStyle name="Normal 10 71" xfId="2392" xr:uid="{B54803D1-1FBD-49E8-A559-9E1C0366BC41}"/>
     <cellStyle name="Normal 10 8" xfId="243" xr:uid="{731BFDFC-42EF-40DB-B469-49423BAFDD34}"/>
     <cellStyle name="Normal 10 9" xfId="259" xr:uid="{C9BCE7F2-A0DC-424E-BD2A-3833A66918FA}"/>
     <cellStyle name="Normal 11" xfId="169" xr:uid="{24883276-07D4-417F-A269-AF8F8014D6B0}"/>
@@ -3730,7 +3637,9 @@
     <cellStyle name="Normal 11 66" xfId="2176" xr:uid="{4847EA09-468D-4049-B750-7B8B05C5BF8A}"/>
     <cellStyle name="Normal 11 67" xfId="2230" xr:uid="{99C40354-1D0A-432F-99AE-E64E96465C87}"/>
     <cellStyle name="Normal 11 68" xfId="2284" xr:uid="{16C8F53F-B88F-426E-800C-98B66BC5E71D}"/>
+    <cellStyle name="Normal 11 69" xfId="2338" xr:uid="{EC2E0160-8B90-4700-8AE5-F6F4DD62D0EF}"/>
     <cellStyle name="Normal 11 7" xfId="244" xr:uid="{3EAFC835-4A7D-45CE-AE77-990DDEAAFDC0}"/>
+    <cellStyle name="Normal 11 70" xfId="2393" xr:uid="{6D271227-DFD7-4B1C-AF1B-4F79A7D80EDB}"/>
     <cellStyle name="Normal 11 8" xfId="260" xr:uid="{F04D5FA1-BA3E-4D95-B369-72C9BC4A33B2}"/>
     <cellStyle name="Normal 11 9" xfId="277" xr:uid="{2BA3F0B3-DDFB-4ED8-8F9B-FB1DE74EA628}"/>
     <cellStyle name="Normal 12" xfId="180" xr:uid="{64C12A1D-7934-48F2-9578-4F1C04C3D62D}"/>
@@ -3797,6 +3706,8 @@
     <cellStyle name="Normal 12 65" xfId="2177" xr:uid="{D4B5BD42-1A0E-4ED5-8598-65707B796D24}"/>
     <cellStyle name="Normal 12 66" xfId="2231" xr:uid="{0BDE2C98-1E34-4841-B8D9-388E9CC85765}"/>
     <cellStyle name="Normal 12 67" xfId="2285" xr:uid="{6AD88E17-B684-40AE-89D0-D8410D5C8C33}"/>
+    <cellStyle name="Normal 12 68" xfId="2339" xr:uid="{B423458D-728F-44E9-9CAB-11D9C3A57F13}"/>
+    <cellStyle name="Normal 12 69" xfId="2394" xr:uid="{2B8431ED-EBFA-4D86-96A7-1791264F5ADE}"/>
     <cellStyle name="Normal 12 7" xfId="261" xr:uid="{83DDF630-CAFE-4366-8DB0-A3134118B594}"/>
     <cellStyle name="Normal 12 8" xfId="278" xr:uid="{F6B4CBEB-461D-400D-9C34-7FB47B2F92C3}"/>
     <cellStyle name="Normal 12 9" xfId="296" xr:uid="{030E8C75-BAB4-4848-8367-E74DEC184755}"/>
@@ -3863,6 +3774,8 @@
     <cellStyle name="Normal 13 64" xfId="2178" xr:uid="{EEEC9752-E906-4144-A0CD-70F7EC572E7D}"/>
     <cellStyle name="Normal 13 65" xfId="2232" xr:uid="{7B8DB9F5-50DF-4CE0-8886-50EF47757061}"/>
     <cellStyle name="Normal 13 66" xfId="2286" xr:uid="{383FAE42-0127-4E2D-B79E-9CCC5E40F900}"/>
+    <cellStyle name="Normal 13 67" xfId="2340" xr:uid="{20C31C95-B57F-4B02-B667-FB76C66C9674}"/>
+    <cellStyle name="Normal 13 68" xfId="2395" xr:uid="{47E0422F-177D-4FB0-B60C-0CBAE2D3DB26}"/>
     <cellStyle name="Normal 13 7" xfId="279" xr:uid="{2D9D628C-A27B-4B86-8C7E-7C9804E457BC}"/>
     <cellStyle name="Normal 13 8" xfId="297" xr:uid="{4A5D7C9D-C5C5-40A5-8715-701C74A7B825}"/>
     <cellStyle name="Normal 13 9" xfId="316" xr:uid="{62B80AA8-8706-4987-866E-1A4286CD93CB}"/>
@@ -3928,6 +3841,8 @@
     <cellStyle name="Normal 14 63" xfId="2179" xr:uid="{9E39D04D-92B3-4F8E-8282-34A8C294EA12}"/>
     <cellStyle name="Normal 14 64" xfId="2233" xr:uid="{56FC2D3F-27E3-42A3-B128-221EB4243A0E}"/>
     <cellStyle name="Normal 14 65" xfId="2287" xr:uid="{19D61C33-98A2-4173-AB9B-E40113E087DC}"/>
+    <cellStyle name="Normal 14 66" xfId="2341" xr:uid="{CC58DE51-6FC2-4826-BEEA-B6F7806042D4}"/>
+    <cellStyle name="Normal 14 67" xfId="2396" xr:uid="{9CBB6B57-ACBB-4988-A69F-89E2CF9EA0AB}"/>
     <cellStyle name="Normal 14 7" xfId="298" xr:uid="{CD68E702-2F82-4764-9927-11DABC2F5829}"/>
     <cellStyle name="Normal 14 8" xfId="317" xr:uid="{6DB7F330-9C64-4B26-AF4F-17A09E12CEC6}"/>
     <cellStyle name="Normal 14 9" xfId="337" xr:uid="{104D5C09-BA78-4885-AA2B-E347E11C3013}"/>
@@ -3992,6 +3907,8 @@
     <cellStyle name="Normal 15 62" xfId="2180" xr:uid="{242ECE3E-4955-450D-BB0B-3752A917D92A}"/>
     <cellStyle name="Normal 15 63" xfId="2234" xr:uid="{6D835B51-C84D-4ADA-A7F3-E876BB68D11D}"/>
     <cellStyle name="Normal 15 64" xfId="2288" xr:uid="{37E8890E-A66E-4B4F-8104-4017DE5D9878}"/>
+    <cellStyle name="Normal 15 65" xfId="2342" xr:uid="{B5581F79-5361-439D-8669-4102E08F839E}"/>
+    <cellStyle name="Normal 15 66" xfId="2397" xr:uid="{C97F2FF7-D326-4A21-9CE0-A21A9C68AE6F}"/>
     <cellStyle name="Normal 15 7" xfId="318" xr:uid="{BC74AE1A-9CA6-4EA4-BFD8-B522F63CB6FF}"/>
     <cellStyle name="Normal 15 8" xfId="338" xr:uid="{52CEAA3B-3AF8-4A6A-ADD3-4403D3D982ED}"/>
     <cellStyle name="Normal 15 9" xfId="358" xr:uid="{52621DB2-9BFC-4EF1-B2FF-A1D2EBD982F8}"/>
@@ -4055,6 +3972,8 @@
     <cellStyle name="Normal 16 61" xfId="2181" xr:uid="{34C06024-21E8-4C18-852F-08390CE4A66D}"/>
     <cellStyle name="Normal 16 62" xfId="2235" xr:uid="{9BC9B08A-3F2A-4FFB-B5F8-109236B0BDF5}"/>
     <cellStyle name="Normal 16 63" xfId="2289" xr:uid="{E5EDA437-73CB-4309-8F89-6D6C3CC00A52}"/>
+    <cellStyle name="Normal 16 64" xfId="2343" xr:uid="{554CC56B-E56F-4FC5-803A-F93332F5EFCF}"/>
+    <cellStyle name="Normal 16 65" xfId="2398" xr:uid="{2CCE9BA0-146A-44DC-9107-50616C3BCBDC}"/>
     <cellStyle name="Normal 16 7" xfId="339" xr:uid="{FAA81CF7-9E8B-4D43-8B87-FEA4DEA195A2}"/>
     <cellStyle name="Normal 16 8" xfId="359" xr:uid="{71945961-3DA4-41F9-B589-733CD154B56B}"/>
     <cellStyle name="Normal 16 9" xfId="379" xr:uid="{2D615019-0C6B-4533-BF0F-B9FB56006E3E}"/>
@@ -4117,6 +4036,8 @@
     <cellStyle name="Normal 17 60" xfId="2182" xr:uid="{681684EF-82D2-4704-B39F-F6A3521AF448}"/>
     <cellStyle name="Normal 17 61" xfId="2236" xr:uid="{27B19F62-0DFD-4876-9457-A41A71B966F6}"/>
     <cellStyle name="Normal 17 62" xfId="2290" xr:uid="{AA8020A6-90EC-45DD-AF0E-DCC2A23AF4C2}"/>
+    <cellStyle name="Normal 17 63" xfId="2344" xr:uid="{0C62EA86-D42E-48CE-ADC8-3297522089DB}"/>
+    <cellStyle name="Normal 17 64" xfId="2399" xr:uid="{99F82004-39D7-4B04-B53C-8B36B0136401}"/>
     <cellStyle name="Normal 17 7" xfId="360" xr:uid="{EF50DC9C-CCDF-49C3-BD04-EC1F385C2EB2}"/>
     <cellStyle name="Normal 17 8" xfId="380" xr:uid="{F7FF7910-81D8-41FE-87E6-74E265C4FE49}"/>
     <cellStyle name="Normal 17 9" xfId="400" xr:uid="{0131EC3E-0935-425F-A406-A9A4A62BE59C}"/>
@@ -4178,6 +4099,8 @@
     <cellStyle name="Normal 18 6" xfId="361" xr:uid="{DACBEFBE-7C6D-415D-817F-3E294365306F}"/>
     <cellStyle name="Normal 18 60" xfId="2237" xr:uid="{EDE31735-226F-433A-A0F5-607825952C61}"/>
     <cellStyle name="Normal 18 61" xfId="2291" xr:uid="{92331A33-9B7A-4686-95A9-FC3B065D72F4}"/>
+    <cellStyle name="Normal 18 62" xfId="2345" xr:uid="{1B5483A4-1DA1-4A8A-8066-EAD76FE37848}"/>
+    <cellStyle name="Normal 18 63" xfId="2400" xr:uid="{67645393-6B54-41BA-9ECD-63C645356B52}"/>
     <cellStyle name="Normal 18 7" xfId="381" xr:uid="{AA0AB4C2-AC98-4892-8993-9C51D645351A}"/>
     <cellStyle name="Normal 18 8" xfId="401" xr:uid="{97EBEF4A-C9B9-484A-A9B8-2BD6E9C715B6}"/>
     <cellStyle name="Normal 18 9" xfId="421" xr:uid="{E88C8D00-A684-4B81-9E3E-D25CD466C39D}"/>
@@ -4238,6 +4161,8 @@
     <cellStyle name="Normal 19 59" xfId="2238" xr:uid="{40123A8D-2D51-4FA1-A957-16D6CE66E800}"/>
     <cellStyle name="Normal 19 6" xfId="382" xr:uid="{0AB426E6-0EDB-41A8-9213-7F540BF567F0}"/>
     <cellStyle name="Normal 19 60" xfId="2292" xr:uid="{18D3992C-C8CC-45C4-B22A-DB4F56CC3651}"/>
+    <cellStyle name="Normal 19 61" xfId="2346" xr:uid="{4A485BF6-DB43-4F04-8375-658BA274D870}"/>
+    <cellStyle name="Normal 19 62" xfId="2401" xr:uid="{7978AFB6-E21D-4EF3-AAD4-EAA63A4D14AE}"/>
     <cellStyle name="Normal 19 7" xfId="402" xr:uid="{7C70AE42-3659-4E21-B1E7-5A2B14B05D2D}"/>
     <cellStyle name="Normal 19 8" xfId="422" xr:uid="{258ACE1C-8C37-43E9-8F9E-504F66369A2C}"/>
     <cellStyle name="Normal 19 9" xfId="443" xr:uid="{AED5C701-AD5D-4D29-BEA5-DC3E31B13CEA}"/>
@@ -4331,6 +4256,8 @@
     <cellStyle name="Normal 2 89" xfId="2221" xr:uid="{346AE234-3485-4E02-BA51-796A6E984CCB}"/>
     <cellStyle name="Normal 2 9" xfId="51" xr:uid="{6FE407A4-72E3-4095-A9DA-0F00979F500D}"/>
     <cellStyle name="Normal 2 90" xfId="2275" xr:uid="{26A141F5-DF12-4532-9EC1-5C4AA47F9FB1}"/>
+    <cellStyle name="Normal 2 91" xfId="2329" xr:uid="{2FB8B8B4-D88E-4A7E-B88B-02CDD96C20BA}"/>
+    <cellStyle name="Normal 2 92" xfId="2384" xr:uid="{5F89FF23-273B-4DAC-A8B3-C925288C6339}"/>
     <cellStyle name="Normal 20" xfId="304" xr:uid="{46E9EC2A-F4CD-4474-8F1F-128DC22F7FEE}"/>
     <cellStyle name="Normal 20 10" xfId="487" xr:uid="{7BB6CDCC-D9F1-4CB0-A7DC-4C2435A3C632}"/>
     <cellStyle name="Normal 20 11" xfId="509" xr:uid="{BC3D68B8-B4B0-466B-88F8-0FB74407A0D0}"/>
@@ -4387,6 +4314,8 @@
     <cellStyle name="Normal 20 58" xfId="2239" xr:uid="{666C5DA3-D976-45DD-B21E-1AB70EF26F0E}"/>
     <cellStyle name="Normal 20 59" xfId="2293" xr:uid="{057C4F56-4F26-4835-928F-56163FF4D8CE}"/>
     <cellStyle name="Normal 20 6" xfId="403" xr:uid="{EDE2DB7C-D6C6-4FFB-9944-879D931D902B}"/>
+    <cellStyle name="Normal 20 60" xfId="2347" xr:uid="{EC1B911F-0406-4638-8B43-775F966355F1}"/>
+    <cellStyle name="Normal 20 61" xfId="2402" xr:uid="{CE530E64-C64A-4892-89C0-F9E0D96226C8}"/>
     <cellStyle name="Normal 20 7" xfId="423" xr:uid="{086835B6-4345-4031-B11A-51B0C72CE8BF}"/>
     <cellStyle name="Normal 20 8" xfId="444" xr:uid="{AB563AA1-827B-4C23-99CE-81D8ACA1B263}"/>
     <cellStyle name="Normal 20 9" xfId="465" xr:uid="{8753642A-194D-4639-8E76-06C881170BFA}"/>
@@ -4444,7 +4373,9 @@
     <cellStyle name="Normal 21 56" xfId="2186" xr:uid="{AB0B689B-C3DA-4CD9-9EC6-2DC8F02A21FE}"/>
     <cellStyle name="Normal 21 57" xfId="2240" xr:uid="{D20DDAD8-28D7-49AB-BD7C-8481F04D3C24}"/>
     <cellStyle name="Normal 21 58" xfId="2294" xr:uid="{6AE3A907-88BE-4039-96CE-93386B7B6F2D}"/>
+    <cellStyle name="Normal 21 59" xfId="2348" xr:uid="{FB4B6430-E2E6-4FD6-9C08-27ED49C36461}"/>
     <cellStyle name="Normal 21 6" xfId="424" xr:uid="{697EF57E-FC1D-456D-A2E3-7187FCE63ED8}"/>
+    <cellStyle name="Normal 21 60" xfId="2403" xr:uid="{22F3B7FD-8FE5-46C7-9284-4283A3DE614A}"/>
     <cellStyle name="Normal 21 7" xfId="445" xr:uid="{1C2BB24F-B439-48A3-AEEA-D7AB69CCFDC1}"/>
     <cellStyle name="Normal 21 8" xfId="466" xr:uid="{5E3619D4-D275-4EB0-A165-F875F480DB0E}"/>
     <cellStyle name="Normal 21 9" xfId="488" xr:uid="{B9BF371B-ACB6-4682-B3CB-DE98962B0D2B}"/>
@@ -4497,6 +4428,8 @@
     <cellStyle name="Normal 22 51" xfId="2187" xr:uid="{A0D0D3E2-321B-4D39-954D-5CDA7EA8A427}"/>
     <cellStyle name="Normal 22 52" xfId="2241" xr:uid="{0A7C26B2-3E8A-4A5F-A47C-F049EEE95DBA}"/>
     <cellStyle name="Normal 22 53" xfId="2295" xr:uid="{17D870F7-133C-4111-AEC0-1C397AC42314}"/>
+    <cellStyle name="Normal 22 54" xfId="2349" xr:uid="{393FD145-9595-4778-81E4-0E7053058E53}"/>
+    <cellStyle name="Normal 22 55" xfId="2404" xr:uid="{6D9BDD54-182A-43EF-BF31-6BDF2EB6430B}"/>
     <cellStyle name="Normal 22 6" xfId="533" xr:uid="{6D06BD98-20DD-45B0-8C60-88A9912CEF28}"/>
     <cellStyle name="Normal 22 7" xfId="556" xr:uid="{C4538170-DB37-479E-96ED-6FC8842F1A26}"/>
     <cellStyle name="Normal 22 8" xfId="579" xr:uid="{E69F69A2-D4D9-4555-B390-12901B969277}"/>
@@ -4548,6 +4481,8 @@
     <cellStyle name="Normal 23 5" xfId="557" xr:uid="{668AE752-4D82-441D-AEC8-A1ED7694047B}"/>
     <cellStyle name="Normal 23 50" xfId="2242" xr:uid="{230CD466-1E5E-4141-ACAB-E49C853CF123}"/>
     <cellStyle name="Normal 23 51" xfId="2296" xr:uid="{D525B771-3269-4E6E-973E-351C3A8CD281}"/>
+    <cellStyle name="Normal 23 52" xfId="2350" xr:uid="{67833818-5129-42D8-818C-CE70B4C6E1F9}"/>
+    <cellStyle name="Normal 23 53" xfId="2405" xr:uid="{19CB0872-A789-4EEA-A697-B19375F4B6DF}"/>
     <cellStyle name="Normal 23 6" xfId="580" xr:uid="{AAB043AD-CE0D-40DF-9A63-8A4C5A6D4F58}"/>
     <cellStyle name="Normal 23 7" xfId="604" xr:uid="{34A3DB58-17AE-4BF6-9728-A09FFBA397E1}"/>
     <cellStyle name="Normal 23 8" xfId="629" xr:uid="{F434F633-2719-4E36-A0A3-945AC33697C3}"/>
@@ -4595,7 +4530,9 @@
     <cellStyle name="Normal 24 46" xfId="2189" xr:uid="{65A51C94-D0F4-4F09-8856-021709C6261F}"/>
     <cellStyle name="Normal 24 47" xfId="2243" xr:uid="{CD598F06-C5AF-455C-A602-1CB6343D677A}"/>
     <cellStyle name="Normal 24 48" xfId="2297" xr:uid="{2021A10B-7724-404E-807D-FEE3E8CD95CD}"/>
+    <cellStyle name="Normal 24 49" xfId="2351" xr:uid="{8BBBA13F-D5A6-4D17-A26B-5AC251374C5F}"/>
     <cellStyle name="Normal 24 5" xfId="630" xr:uid="{EF3257C5-660E-46BC-92EF-B371A268B966}"/>
+    <cellStyle name="Normal 24 50" xfId="2406" xr:uid="{FF89A4E2-CBB3-4CF1-820B-6D3AEC466467}"/>
     <cellStyle name="Normal 24 6" xfId="657" xr:uid="{32CD1B47-986E-462F-9668-4C8456D8C1B2}"/>
     <cellStyle name="Normal 24 7" xfId="684" xr:uid="{4CA8DE0A-B4AD-4241-8614-A270B05E4B04}"/>
     <cellStyle name="Normal 24 8" xfId="711" xr:uid="{C4B81C6D-EA33-4229-A72E-E576757A69AA}"/>
@@ -4641,6 +4578,8 @@
     <cellStyle name="Normal 25 44" xfId="2190" xr:uid="{BECA82AF-1D14-474A-8A70-7F47D45A973F}"/>
     <cellStyle name="Normal 25 45" xfId="2244" xr:uid="{8541398F-E3AD-461A-8420-7C414BA03FA7}"/>
     <cellStyle name="Normal 25 46" xfId="2298" xr:uid="{91170925-8CF6-4E16-8978-AF71AD52EB30}"/>
+    <cellStyle name="Normal 25 47" xfId="2352" xr:uid="{66108485-3E38-4511-BE80-6B3463342FD1}"/>
+    <cellStyle name="Normal 25 48" xfId="2407" xr:uid="{E0C0AFC1-4590-4240-9197-3F84798DD155}"/>
     <cellStyle name="Normal 25 5" xfId="685" xr:uid="{DD6998FF-E097-4F7D-A460-95B18DABE8A9}"/>
     <cellStyle name="Normal 25 6" xfId="712" xr:uid="{829BB221-C705-476D-A467-70C6FED9B8ED}"/>
     <cellStyle name="Normal 25 7" xfId="739" xr:uid="{B64EF1EB-9F92-4BEC-BEAD-2E23DE7EC71A}"/>
@@ -4686,6 +4625,8 @@
     <cellStyle name="Normal 26 43" xfId="2191" xr:uid="{831DB7A5-B0A3-4CC0-819E-5C8B3BDEE459}"/>
     <cellStyle name="Normal 26 44" xfId="2245" xr:uid="{D60F2113-32AC-4B3E-A11D-6B7BDAE44191}"/>
     <cellStyle name="Normal 26 45" xfId="2299" xr:uid="{36644ADC-8F18-4CD8-82F2-5F6EDFE8309E}"/>
+    <cellStyle name="Normal 26 46" xfId="2353" xr:uid="{8A495161-9B41-48C2-B731-E58D2D7FDF89}"/>
+    <cellStyle name="Normal 26 47" xfId="2408" xr:uid="{8E8831B9-C32D-4746-A6BD-1B89DC3538E7}"/>
     <cellStyle name="Normal 26 5" xfId="713" xr:uid="{D344AFEE-A03D-4DA9-BD02-29F7ABE09946}"/>
     <cellStyle name="Normal 26 6" xfId="740" xr:uid="{55099FE6-EF4A-4F80-A025-FC0681D4C856}"/>
     <cellStyle name="Normal 26 7" xfId="767" xr:uid="{E0D5D6CA-66CD-46E6-81F6-E5EF5A9B9699}"/>
@@ -4730,6 +4671,8 @@
     <cellStyle name="Normal 27 42" xfId="2192" xr:uid="{41EBAF67-CDED-4241-9231-0724FCE7EECB}"/>
     <cellStyle name="Normal 27 43" xfId="2246" xr:uid="{6AF8C49F-1A6F-405C-A5E5-1836AE60A24F}"/>
     <cellStyle name="Normal 27 44" xfId="2300" xr:uid="{7F64AC8D-D54B-4551-B7D6-FAC321FCFDE9}"/>
+    <cellStyle name="Normal 27 45" xfId="2354" xr:uid="{35ED50A4-119A-42DB-8B12-F81EECFB6985}"/>
+    <cellStyle name="Normal 27 46" xfId="2409" xr:uid="{921F6FEA-C33A-4779-920B-7DBA20603530}"/>
     <cellStyle name="Normal 27 5" xfId="741" xr:uid="{73F13B32-388D-4D89-9F01-E89AA863010F}"/>
     <cellStyle name="Normal 27 6" xfId="768" xr:uid="{C1FF1113-E4F1-409B-9342-01929F68ADCD}"/>
     <cellStyle name="Normal 27 7" xfId="795" xr:uid="{637C3645-B9B7-4559-9CFF-F3A6B8FF3C81}"/>
@@ -4774,6 +4717,8 @@
     <cellStyle name="Normal 28 42" xfId="2193" xr:uid="{52710BDA-008D-44A1-8B22-437D08E65F65}"/>
     <cellStyle name="Normal 28 43" xfId="2247" xr:uid="{9394D01C-E2EE-4ADF-AB85-7611AE355BAE}"/>
     <cellStyle name="Normal 28 44" xfId="2301" xr:uid="{5AB414CF-DD12-4AFC-A3F7-E4B94DEE0D7F}"/>
+    <cellStyle name="Normal 28 45" xfId="2355" xr:uid="{54B74C83-6C34-4A7D-9AD3-9A1EA78BECC5}"/>
+    <cellStyle name="Normal 28 46" xfId="2410" xr:uid="{F60F07C7-4DE0-49FD-9622-192482283209}"/>
     <cellStyle name="Normal 28 5" xfId="742" xr:uid="{0E873815-9144-409F-9560-E3292F714AD5}"/>
     <cellStyle name="Normal 28 6" xfId="769" xr:uid="{E1B9D957-F371-47A0-AEBA-EB4390991517}"/>
     <cellStyle name="Normal 28 7" xfId="796" xr:uid="{CE95D840-1DED-4550-9B45-79BB1A30B661}"/>
@@ -4809,6 +4754,8 @@
     <cellStyle name="Normal 29 34" xfId="2194" xr:uid="{BC1BE158-4343-477E-A3CD-6F4BC6216194}"/>
     <cellStyle name="Normal 29 35" xfId="2248" xr:uid="{DED7610A-0AE0-4426-A3DC-9243D6CF9EDC}"/>
     <cellStyle name="Normal 29 36" xfId="2302" xr:uid="{1AD7A340-A7DB-4D71-9501-31DCAF062C83}"/>
+    <cellStyle name="Normal 29 37" xfId="2356" xr:uid="{929283DC-4112-4FB7-BC9D-DF7DBF16E899}"/>
+    <cellStyle name="Normal 29 38" xfId="2411" xr:uid="{32B4EF5D-097A-4490-AB57-B12BF3203489}"/>
     <cellStyle name="Normal 29 4" xfId="936" xr:uid="{B0ED404B-A0BC-4005-9C07-3ADBBFE5F173}"/>
     <cellStyle name="Normal 29 5" xfId="965" xr:uid="{E4F2ED17-F04A-4AF1-A706-C14A73357E91}"/>
     <cellStyle name="Normal 29 6" xfId="994" xr:uid="{CAF38D46-8974-47D6-914C-330FB88EC9BB}"/>
@@ -4905,6 +4852,8 @@
     <cellStyle name="Normal 3 89" xfId="2222" xr:uid="{E91487DA-2C12-4FC1-87ED-6CFAAC0AC1B6}"/>
     <cellStyle name="Normal 3 9" xfId="52" xr:uid="{67EF2365-F906-488B-BF98-0B8A0C7AD397}"/>
     <cellStyle name="Normal 3 90" xfId="2276" xr:uid="{05D0FD9A-2C4D-4E67-B715-F48881962247}"/>
+    <cellStyle name="Normal 3 91" xfId="2330" xr:uid="{7C9CB010-F1E7-4EFD-804C-07FFFC147F7B}"/>
+    <cellStyle name="Normal 3 92" xfId="2385" xr:uid="{C802E603-F79D-484A-8796-D10DCC293D44}"/>
     <cellStyle name="Normal 30" xfId="908" xr:uid="{29060677-DDC7-44E4-9DB7-833832E2C2EF}"/>
     <cellStyle name="Normal 30 10" xfId="1194" xr:uid="{87CB8D63-90E2-489B-B2F1-CACD93DC026A}"/>
     <cellStyle name="Normal 30 11" xfId="1233" xr:uid="{BE9D1AC2-FA84-447C-980B-7C0F52813116}"/>
@@ -4933,6 +4882,8 @@
     <cellStyle name="Normal 30 32" xfId="2195" xr:uid="{7DA1B9D3-65C8-41DA-892E-7BB49962EE3C}"/>
     <cellStyle name="Normal 30 33" xfId="2249" xr:uid="{5AA52825-6ED6-4D22-96C8-7B35382EE0CF}"/>
     <cellStyle name="Normal 30 34" xfId="2303" xr:uid="{600E12BF-5A9C-4BD3-A3CA-2ABA40241DF6}"/>
+    <cellStyle name="Normal 30 35" xfId="2357" xr:uid="{ABD7D2C6-C14A-4E7C-98E4-7A6F126BC750}"/>
+    <cellStyle name="Normal 30 36" xfId="2412" xr:uid="{C360F1EF-5219-46D6-9B03-DCDF440403A4}"/>
     <cellStyle name="Normal 30 4" xfId="995" xr:uid="{8A471471-CC73-4677-8055-BF9B78704B15}"/>
     <cellStyle name="Normal 30 5" xfId="1025" xr:uid="{8A88A566-55ED-4197-B3EC-34A2D6F4693C}"/>
     <cellStyle name="Normal 30 6" xfId="1056" xr:uid="{C7E13848-0B37-42F9-92EF-9D5A7F8289AC}"/>
@@ -4964,6 +4915,8 @@
     <cellStyle name="Normal 31 3" xfId="1057" xr:uid="{BEEB650F-2862-40F3-8D59-DBB86C058CB6}"/>
     <cellStyle name="Normal 31 30" xfId="2250" xr:uid="{879AA462-BFAB-40DA-93F2-FAB1769126CA}"/>
     <cellStyle name="Normal 31 31" xfId="2304" xr:uid="{6902C0B4-6563-4408-9608-C6349C3F6E17}"/>
+    <cellStyle name="Normal 31 32" xfId="2358" xr:uid="{EF15EB66-4386-4230-A612-ED933C7471FB}"/>
+    <cellStyle name="Normal 31 33" xfId="2413" xr:uid="{89E2EA3F-47F5-47C0-A540-133C298E781A}"/>
     <cellStyle name="Normal 31 4" xfId="1089" xr:uid="{115B4DBC-0A4B-43C2-8D38-B8E1346CA496}"/>
     <cellStyle name="Normal 31 5" xfId="1123" xr:uid="{17785C55-2ED2-45EA-9422-1590CD144DCC}"/>
     <cellStyle name="Normal 31 6" xfId="1158" xr:uid="{5257BC80-708E-436F-B0A2-DE856F2C5DBA}"/>
@@ -4994,6 +4947,8 @@
     <cellStyle name="Normal 32 29" xfId="2251" xr:uid="{7BDF06E4-D5A8-4E9F-9256-774A85D5D645}"/>
     <cellStyle name="Normal 32 3" xfId="1090" xr:uid="{6B374505-EDC7-4D43-95D8-B665B15D29DA}"/>
     <cellStyle name="Normal 32 30" xfId="2305" xr:uid="{F9553DB4-A148-47E3-9FF7-0F065C20ED3F}"/>
+    <cellStyle name="Normal 32 31" xfId="2359" xr:uid="{3E9B7C91-4175-4E1E-A314-4613B40E6C7A}"/>
+    <cellStyle name="Normal 32 32" xfId="2414" xr:uid="{EEB684C7-4033-4182-BB34-C200845CF3B8}"/>
     <cellStyle name="Normal 32 4" xfId="1124" xr:uid="{02CC8B8D-088C-499C-99A0-F631BCDD8473}"/>
     <cellStyle name="Normal 32 5" xfId="1159" xr:uid="{D2F78B05-994A-4DB4-A496-D9328EBBE67B}"/>
     <cellStyle name="Normal 32 6" xfId="1196" xr:uid="{2DCB929C-297C-4C53-82E4-0403B87AF2B1}"/>
@@ -5023,6 +4978,8 @@
     <cellStyle name="Normal 33 28" xfId="2252" xr:uid="{5B996FB3-253D-4E93-8766-07AF7A04AFAB}"/>
     <cellStyle name="Normal 33 29" xfId="2306" xr:uid="{09EC3DDB-5998-43C1-A94B-B6EA893EA050}"/>
     <cellStyle name="Normal 33 3" xfId="1125" xr:uid="{DA4B6EED-C769-4BE0-BA7E-E741A1CD3FB3}"/>
+    <cellStyle name="Normal 33 30" xfId="2360" xr:uid="{6ECE6C43-8104-47B9-B117-B38271699D3A}"/>
+    <cellStyle name="Normal 33 31" xfId="2415" xr:uid="{52E82BF7-BDDE-4D85-BE3E-EF35E155C12A}"/>
     <cellStyle name="Normal 33 4" xfId="1160" xr:uid="{740C5F2E-4830-4E49-BDD6-9A5138A262C0}"/>
     <cellStyle name="Normal 33 5" xfId="1197" xr:uid="{63D7510F-076E-4560-907D-87441A3EC81D}"/>
     <cellStyle name="Normal 33 6" xfId="1236" xr:uid="{32588593-4A0B-46F3-8C61-023846E9132B}"/>
@@ -5050,7 +5007,9 @@
     <cellStyle name="Normal 34 26" xfId="2199" xr:uid="{68409217-F7CD-4BCC-82C3-470D3D903BA4}"/>
     <cellStyle name="Normal 34 27" xfId="2253" xr:uid="{3D5B7521-4F29-43B6-A5EF-B9B878A0CE08}"/>
     <cellStyle name="Normal 34 28" xfId="2307" xr:uid="{D8BB9877-8295-4B94-884E-ACB44929AA69}"/>
+    <cellStyle name="Normal 34 29" xfId="2361" xr:uid="{63FDA86C-8D93-4610-8F20-F59CA8ED1F80}"/>
     <cellStyle name="Normal 34 3" xfId="1161" xr:uid="{984471BB-698B-4FEC-BE51-290CAAFB126E}"/>
+    <cellStyle name="Normal 34 30" xfId="2416" xr:uid="{83F2861E-D22C-423E-BDA5-D7F16A77409B}"/>
     <cellStyle name="Normal 34 4" xfId="1198" xr:uid="{8F856BAA-2847-43FC-BEA2-D1DAFE5D5C08}"/>
     <cellStyle name="Normal 34 5" xfId="1237" xr:uid="{E8D324D6-0564-42C7-A347-F071F77AD38C}"/>
     <cellStyle name="Normal 34 6" xfId="1277" xr:uid="{78E23A18-BA39-450B-AF6F-829AB866D556}"/>
@@ -5078,7 +5037,9 @@
     <cellStyle name="Normal 35 26" xfId="2200" xr:uid="{C70615DF-CBF6-4B20-B0C2-1224BFF71B47}"/>
     <cellStyle name="Normal 35 27" xfId="2254" xr:uid="{1F6EE8FD-27B2-460A-A193-516B8C1F6AE6}"/>
     <cellStyle name="Normal 35 28" xfId="2308" xr:uid="{41A6881D-6FAF-4874-B715-06F24AC809C7}"/>
+    <cellStyle name="Normal 35 29" xfId="2362" xr:uid="{DE8E2D4B-D2A4-411E-BD33-E75637BE13A2}"/>
     <cellStyle name="Normal 35 3" xfId="1162" xr:uid="{F711045E-FBAB-49E2-B85B-DD7F67FA2A9E}"/>
+    <cellStyle name="Normal 35 30" xfId="2417" xr:uid="{B3F07313-675D-4BCB-973A-BF2F37E61096}"/>
     <cellStyle name="Normal 35 4" xfId="1199" xr:uid="{5C6D934C-C084-456A-8378-EFEE061775E5}"/>
     <cellStyle name="Normal 35 5" xfId="1238" xr:uid="{7CB240F7-BDE4-4E7B-8875-63F971329466}"/>
     <cellStyle name="Normal 35 6" xfId="1278" xr:uid="{EF4981D6-3F62-4CEE-AFBB-7FAF9F704E25}"/>
@@ -5105,6 +5066,8 @@
     <cellStyle name="Normal 36 25" xfId="2201" xr:uid="{DA023B1D-485A-4017-B02B-86EEBBE5B8EA}"/>
     <cellStyle name="Normal 36 26" xfId="2255" xr:uid="{220DD765-7694-46B8-87CB-903BD3317D2B}"/>
     <cellStyle name="Normal 36 27" xfId="2309" xr:uid="{97B3D915-5056-4821-847D-F8F8C8576AA7}"/>
+    <cellStyle name="Normal 36 28" xfId="2363" xr:uid="{6DB1304B-0741-4634-B52A-8E8FA8039D4D}"/>
+    <cellStyle name="Normal 36 29" xfId="2418" xr:uid="{887E7B0C-BF23-4A33-9D41-9A226E958518}"/>
     <cellStyle name="Normal 36 3" xfId="1200" xr:uid="{9B7CD598-05AB-40C9-BCD9-3B8266389254}"/>
     <cellStyle name="Normal 36 4" xfId="1239" xr:uid="{D6071E2A-50A2-4D3C-9968-A1E3E4687B7E}"/>
     <cellStyle name="Normal 36 5" xfId="1279" xr:uid="{F643CB92-74BB-4F63-99A2-B010269425DF}"/>
@@ -5131,6 +5094,8 @@
     <cellStyle name="Normal 37 24" xfId="2202" xr:uid="{3F603DC5-14C0-4799-9768-CD13866D69B2}"/>
     <cellStyle name="Normal 37 25" xfId="2256" xr:uid="{73812A9D-843D-4882-BEFD-D7F11B6646C2}"/>
     <cellStyle name="Normal 37 26" xfId="2310" xr:uid="{59B96874-225F-4A03-9E0C-EFAACEEC5D08}"/>
+    <cellStyle name="Normal 37 27" xfId="2364" xr:uid="{7A30CF3A-89E3-4C39-AAD9-B68114DD075A}"/>
+    <cellStyle name="Normal 37 28" xfId="2419" xr:uid="{07723123-A61A-46E6-BC00-65C8A8ACEB92}"/>
     <cellStyle name="Normal 37 3" xfId="1240" xr:uid="{542FBE86-F5EE-4D1E-9F91-6EA7599E5748}"/>
     <cellStyle name="Normal 37 4" xfId="1280" xr:uid="{BB9F55A5-BDD5-4597-90A0-CF5B0C044934}"/>
     <cellStyle name="Normal 37 5" xfId="1321" xr:uid="{C233C0E3-A15F-40DD-88CA-205C74255FCE}"/>
@@ -5157,6 +5122,8 @@
     <cellStyle name="Normal 38 24" xfId="2203" xr:uid="{2DEC600A-5B77-430B-8DED-9127D5A6785B}"/>
     <cellStyle name="Normal 38 25" xfId="2257" xr:uid="{B1C72B38-31BB-41DB-B857-809C65C4A0A5}"/>
     <cellStyle name="Normal 38 26" xfId="2311" xr:uid="{95E19800-C30A-4E51-BD76-3CA390AB5639}"/>
+    <cellStyle name="Normal 38 27" xfId="2365" xr:uid="{99C63C58-EF56-40CD-9558-2D7CD30F36F6}"/>
+    <cellStyle name="Normal 38 28" xfId="2420" xr:uid="{E3DDAD81-A0CC-41AA-813D-A7190C58D172}"/>
     <cellStyle name="Normal 38 3" xfId="1241" xr:uid="{5AB936AE-86CC-45A3-8DE0-331F0E36DDBD}"/>
     <cellStyle name="Normal 38 4" xfId="1281" xr:uid="{06B9E8CD-8E13-44D7-B4A2-3CCA5CF70BFC}"/>
     <cellStyle name="Normal 38 5" xfId="1322" xr:uid="{64D206D8-A195-42CA-8AFF-84B3F657D678}"/>
@@ -5182,6 +5149,8 @@
     <cellStyle name="Normal 39 23" xfId="2204" xr:uid="{905D2147-0F79-4424-B455-6D277D831506}"/>
     <cellStyle name="Normal 39 24" xfId="2258" xr:uid="{535AFA1D-4B0E-4C5A-800E-8591233C18A1}"/>
     <cellStyle name="Normal 39 25" xfId="2312" xr:uid="{E14F26CF-CD5D-4C43-99F3-8F92071A3966}"/>
+    <cellStyle name="Normal 39 26" xfId="2366" xr:uid="{C94ED76E-DF7F-4450-80CF-D75B2CAAB926}"/>
+    <cellStyle name="Normal 39 27" xfId="2421" xr:uid="{18F96B56-B490-4659-B0CE-42068A35FBEB}"/>
     <cellStyle name="Normal 39 3" xfId="1282" xr:uid="{0296B16D-DA08-43E9-9663-8A88969E79F4}"/>
     <cellStyle name="Normal 39 4" xfId="1323" xr:uid="{15831E53-2DBD-4A2E-B270-23C619CA089E}"/>
     <cellStyle name="Normal 39 5" xfId="1365" xr:uid="{F009ABEF-0BCE-4955-ADC3-3578DB39F7F8}"/>
@@ -5279,6 +5248,8 @@
     <cellStyle name="Normal 4 89" xfId="2223" xr:uid="{D9A261C1-36A9-45A1-90B2-75A64B39BD8C}"/>
     <cellStyle name="Normal 4 9" xfId="53" xr:uid="{08E3772A-E9B7-4C5E-B672-596AFF50976B}"/>
     <cellStyle name="Normal 4 90" xfId="2277" xr:uid="{237462F5-BB1D-4C48-9ADF-BE20CF931E26}"/>
+    <cellStyle name="Normal 4 91" xfId="2331" xr:uid="{A0EB0CBE-1F94-41C7-98FF-4DAECF115BCB}"/>
+    <cellStyle name="Normal 4 92" xfId="2386" xr:uid="{949304E3-ABC1-4BC5-8027-03D8E13BC5CC}"/>
     <cellStyle name="Normal 40" xfId="1204" xr:uid="{9A758E20-7263-44F0-A0A0-3D5D1FE88C83}"/>
     <cellStyle name="Normal 40 10" xfId="1584" xr:uid="{00514BDB-1937-4C34-97E1-6B15E53A4098}"/>
     <cellStyle name="Normal 40 11" xfId="1628" xr:uid="{858AF8D4-5153-4B46-93B1-00B25FF415FB}"/>
@@ -5297,6 +5268,8 @@
     <cellStyle name="Normal 40 23" xfId="2205" xr:uid="{C0AAD3F3-BB90-4E4A-960C-DE8956C31E4B}"/>
     <cellStyle name="Normal 40 24" xfId="2259" xr:uid="{3AA457D2-1E7D-49BD-BC36-4A604733300F}"/>
     <cellStyle name="Normal 40 25" xfId="2313" xr:uid="{3DD46A9E-26FC-4271-A30C-E459C4EE092F}"/>
+    <cellStyle name="Normal 40 26" xfId="2367" xr:uid="{C08016E3-3D86-4965-BA30-A2E3134EB706}"/>
+    <cellStyle name="Normal 40 27" xfId="2422" xr:uid="{D2E03D60-114F-4864-906A-098716246FD2}"/>
     <cellStyle name="Normal 40 3" xfId="1283" xr:uid="{60DC833A-F031-4DBD-BC0B-B48ABCDE6533}"/>
     <cellStyle name="Normal 40 4" xfId="1324" xr:uid="{BC132578-6363-4D48-BB11-F90899981771}"/>
     <cellStyle name="Normal 40 5" xfId="1366" xr:uid="{CCB407F9-2940-4586-A2FB-F175B848303E}"/>
@@ -5321,6 +5294,8 @@
     <cellStyle name="Normal 41 22" xfId="2206" xr:uid="{3B44B64E-D9F1-44D2-9F8B-A2EF092534DB}"/>
     <cellStyle name="Normal 41 23" xfId="2260" xr:uid="{DDFB2237-92D1-4471-8B88-4A43AED0C366}"/>
     <cellStyle name="Normal 41 24" xfId="2314" xr:uid="{97A31EC4-2451-42D8-8741-C4AFA548353B}"/>
+    <cellStyle name="Normal 41 25" xfId="2368" xr:uid="{768D9F1F-9C6B-4DB2-9288-AA0451754DDA}"/>
+    <cellStyle name="Normal 41 26" xfId="2423" xr:uid="{238D28F3-8E81-4BDA-8132-6766EDEBA318}"/>
     <cellStyle name="Normal 41 3" xfId="1325" xr:uid="{DB7266FD-DB20-4504-9181-FDAD4A49F920}"/>
     <cellStyle name="Normal 41 4" xfId="1367" xr:uid="{7EE95D5B-6BEF-49DA-8567-DB37D49C5ABE}"/>
     <cellStyle name="Normal 41 5" xfId="1409" xr:uid="{626DD975-DD53-4D9F-B777-AA700296E57B}"/>
@@ -5344,6 +5319,8 @@
     <cellStyle name="Normal 42 21" xfId="2207" xr:uid="{7FD2750E-290A-4D4C-B57F-BBF4E41B01FD}"/>
     <cellStyle name="Normal 42 22" xfId="2261" xr:uid="{0B62BB22-7FC0-43E8-9633-EE7CA43B1CED}"/>
     <cellStyle name="Normal 42 23" xfId="2315" xr:uid="{6E1BFCE1-6EDE-4667-A457-C497464AB3F7}"/>
+    <cellStyle name="Normal 42 24" xfId="2369" xr:uid="{6D857CC0-A0CC-476A-8A6D-4C179688E51A}"/>
+    <cellStyle name="Normal 42 25" xfId="2424" xr:uid="{EC43C3B1-DD6D-4CAF-A170-627B81DF52D9}"/>
     <cellStyle name="Normal 42 3" xfId="1368" xr:uid="{027F54D2-79FB-429D-8AF6-DC22C57389A3}"/>
     <cellStyle name="Normal 42 4" xfId="1410" xr:uid="{04BC6829-1A0D-4655-BB18-979D575FAF18}"/>
     <cellStyle name="Normal 42 5" xfId="1453" xr:uid="{A41DFB52-1E5B-461C-8EE4-AB2538BAB5D4}"/>
@@ -5366,6 +5343,8 @@
     <cellStyle name="Normal 43 20" xfId="2208" xr:uid="{863323DB-B25B-44E0-8AA0-507DCEFB5E27}"/>
     <cellStyle name="Normal 43 21" xfId="2262" xr:uid="{08000729-FCA7-447A-8293-2AE43813AF6E}"/>
     <cellStyle name="Normal 43 22" xfId="2316" xr:uid="{E6CC6AF2-7ACA-49DA-AA08-6B90ADEDDF35}"/>
+    <cellStyle name="Normal 43 23" xfId="2370" xr:uid="{B0DFF26F-5534-4297-84F4-FCDC90C89B7B}"/>
+    <cellStyle name="Normal 43 24" xfId="2425" xr:uid="{11D196AE-99A0-48B6-AA2A-79A01C2D72B5}"/>
     <cellStyle name="Normal 43 3" xfId="1411" xr:uid="{E9013BFE-34CD-4396-9801-740BE57E4C74}"/>
     <cellStyle name="Normal 43 4" xfId="1454" xr:uid="{8B718497-4D05-4283-B46C-590C40CCD3B5}"/>
     <cellStyle name="Normal 43 5" xfId="1498" xr:uid="{8E7273E6-D96E-4807-9FA4-FD3FAA93ABEC}"/>
@@ -5386,6 +5365,8 @@
     <cellStyle name="Normal 44 19" xfId="2263" xr:uid="{166376C5-5132-4181-8CEE-C4540FB64AA3}"/>
     <cellStyle name="Normal 44 2" xfId="1455" xr:uid="{FB733BCC-778D-482A-8F7C-76DD90096D45}"/>
     <cellStyle name="Normal 44 20" xfId="2317" xr:uid="{37A14A11-41D7-4793-9EB1-375B7C7BC519}"/>
+    <cellStyle name="Normal 44 21" xfId="2371" xr:uid="{39BEE483-4692-476C-9313-D62EA4633326}"/>
+    <cellStyle name="Normal 44 22" xfId="2426" xr:uid="{3BA62BB1-792D-45F3-8659-AF5C7965BF92}"/>
     <cellStyle name="Normal 44 3" xfId="1499" xr:uid="{19841630-1868-4129-AF65-9439A8362635}"/>
     <cellStyle name="Normal 44 4" xfId="1543" xr:uid="{B24CAFA4-F870-42C6-835A-841530B7459E}"/>
     <cellStyle name="Normal 44 5" xfId="1588" xr:uid="{F3149A38-5BF0-4CF4-92A1-CEBFBCA9E57B}"/>
@@ -5405,6 +5386,8 @@
     <cellStyle name="Normal 45 18" xfId="2264" xr:uid="{DFD0FB7C-1F4D-4665-A7DC-5308508319F8}"/>
     <cellStyle name="Normal 45 19" xfId="2318" xr:uid="{35A59C85-A695-422D-9858-4CDF82238F16}"/>
     <cellStyle name="Normal 45 2" xfId="1500" xr:uid="{5027BECF-87E9-4D4B-9BEF-85E1909AE39A}"/>
+    <cellStyle name="Normal 45 20" xfId="2372" xr:uid="{0E3AA70B-706E-422D-BA4C-6FFD45EF939A}"/>
+    <cellStyle name="Normal 45 21" xfId="2427" xr:uid="{6B8EEB3E-EF73-45B8-A5A6-B1DEF269080F}"/>
     <cellStyle name="Normal 45 3" xfId="1544" xr:uid="{1787A129-1435-4B42-BEEC-006984305340}"/>
     <cellStyle name="Normal 45 4" xfId="1589" xr:uid="{D8955FBC-9811-4F2B-8AA5-1BB672F751BC}"/>
     <cellStyle name="Normal 45 5" xfId="1633" xr:uid="{282C9639-360C-473E-852D-2521B8E40B05}"/>
@@ -5417,6 +5400,8 @@
     <cellStyle name="Normal 46 11" xfId="2211" xr:uid="{4CCEBE56-1DE9-49F7-8509-55D7277C1498}"/>
     <cellStyle name="Normal 46 12" xfId="2265" xr:uid="{3AEF7A84-CA9C-484F-A3AE-D3B3F4B217F8}"/>
     <cellStyle name="Normal 46 13" xfId="2319" xr:uid="{38549543-DF9E-40D8-AE60-3A34235A86E0}"/>
+    <cellStyle name="Normal 46 14" xfId="2373" xr:uid="{7A6B0829-52CF-4AAA-B0A9-41465DAF1112}"/>
+    <cellStyle name="Normal 46 15" xfId="2428" xr:uid="{6298130A-51EC-40A6-98EF-E2DD1DB3D487}"/>
     <cellStyle name="Normal 46 2" xfId="1722" xr:uid="{A92ECEED-86A5-4AF8-A45B-3F5122E4A57C}"/>
     <cellStyle name="Normal 46 3" xfId="1812" xr:uid="{9B7FD6F8-A2AE-4D9F-97CA-07164D6BFAED}"/>
     <cellStyle name="Normal 46 4" xfId="1858" xr:uid="{5099E28A-8E05-4821-9D0F-B6E84C8944BB}"/>
@@ -5429,6 +5414,8 @@
     <cellStyle name="Normal 47 10" xfId="2212" xr:uid="{F43E13EB-5486-41DD-9B54-66E3BFB2D7E5}"/>
     <cellStyle name="Normal 47 11" xfId="2266" xr:uid="{80CEFB79-1988-41B1-992F-AFC4DF579F63}"/>
     <cellStyle name="Normal 47 12" xfId="2320" xr:uid="{22719D81-FE51-4E4D-9A75-CA6E683278BA}"/>
+    <cellStyle name="Normal 47 13" xfId="2374" xr:uid="{3F8FE100-EE70-4751-A9C3-33DCE7F70579}"/>
+    <cellStyle name="Normal 47 14" xfId="2429" xr:uid="{F18DB719-115E-4829-B5B1-308C2A730787}"/>
     <cellStyle name="Normal 47 2" xfId="1813" xr:uid="{C2210DC9-C26B-4BF3-AF35-FBEBA6756BF6}"/>
     <cellStyle name="Normal 47 3" xfId="1859" xr:uid="{68779769-7635-477C-A18C-EF4DCCAC4899}"/>
     <cellStyle name="Normal 47 4" xfId="1906" xr:uid="{2F6200A8-6C6E-4A93-87BA-36E965276181}"/>
@@ -5439,6 +5426,8 @@
     <cellStyle name="Normal 47 9" xfId="2159" xr:uid="{DDCC4EBF-294A-4E59-96D0-B5E85CA7A74E}"/>
     <cellStyle name="Normal 48" xfId="1860" xr:uid="{D754A0F8-F63E-4AD0-874E-32729C62B7FF}"/>
     <cellStyle name="Normal 48 10" xfId="2321" xr:uid="{6B69415D-73A4-4BFC-AC96-9262FC2857E0}"/>
+    <cellStyle name="Normal 48 11" xfId="2375" xr:uid="{285896D6-321F-4B7F-9545-76A6FB4A4CB1}"/>
+    <cellStyle name="Normal 48 12" xfId="2430" xr:uid="{1E16A4FB-6A23-42C5-92DD-9358F7CD93D9}"/>
     <cellStyle name="Normal 48 2" xfId="1907" xr:uid="{CB91C6DC-62B0-4992-A8A4-FEC63EC908A5}"/>
     <cellStyle name="Normal 48 3" xfId="1955" xr:uid="{9140C7D6-0A03-4AEF-AB80-301C7410CF0E}"/>
     <cellStyle name="Normal 48 4" xfId="2004" xr:uid="{4958E27D-47B3-4CE5-9C94-AA09930271BA}"/>
@@ -5448,6 +5437,8 @@
     <cellStyle name="Normal 48 8" xfId="2213" xr:uid="{C27ED5A0-3138-4DCF-A3C5-C9E614B5ED94}"/>
     <cellStyle name="Normal 48 9" xfId="2267" xr:uid="{714E9D5B-F650-4245-A09D-394BD672EEDD}"/>
     <cellStyle name="Normal 49" xfId="1908" xr:uid="{181FE46B-5ADF-443B-A5AF-43C8E8CE7316}"/>
+    <cellStyle name="Normal 49 10" xfId="2376" xr:uid="{619ACDF0-205F-48D6-B6CC-1EDBCCC8946B}"/>
+    <cellStyle name="Normal 49 11" xfId="2431" xr:uid="{3A259915-4B6F-47C2-9EBC-4246A0DD5807}"/>
     <cellStyle name="Normal 49 2" xfId="1956" xr:uid="{AB9E1C32-A524-46A2-A8BF-A94BB89130A2}"/>
     <cellStyle name="Normal 49 3" xfId="2005" xr:uid="{049F4BEA-0C06-4129-947B-575F3F21ED78}"/>
     <cellStyle name="Normal 49 4" xfId="2055" xr:uid="{17958B43-E79B-4901-9FE3-F7F09DD6273F}"/>
@@ -5546,7 +5537,10 @@
     <cellStyle name="Normal 5 89" xfId="2224" xr:uid="{0FE96D1E-20E1-459E-AB35-943AD932DE52}"/>
     <cellStyle name="Normal 5 9" xfId="54" xr:uid="{CE8D6C37-D2B6-44C6-B512-1A53C4CC471E}"/>
     <cellStyle name="Normal 5 90" xfId="2278" xr:uid="{923232B3-278A-4CAB-9FB5-60044FAE477E}"/>
+    <cellStyle name="Normal 5 91" xfId="2332" xr:uid="{74847720-2D89-4817-8202-5A3D4B1520D1}"/>
+    <cellStyle name="Normal 5 92" xfId="2387" xr:uid="{1FD4D425-4F5A-4A82-9330-53EC3285CDFB}"/>
     <cellStyle name="Normal 50" xfId="1957" xr:uid="{F694FC52-4B0F-47E1-92DF-CD4D0A8F23AF}"/>
+    <cellStyle name="Normal 50 10" xfId="2432" xr:uid="{2354729D-8ABA-4246-92CA-A3C324BC2D2A}"/>
     <cellStyle name="Normal 50 2" xfId="2006" xr:uid="{5EA267D6-8E66-4747-B152-4678861E6E9C}"/>
     <cellStyle name="Normal 50 3" xfId="2056" xr:uid="{94B7053D-F0C4-43EA-8BBD-E8EEE51A73B1}"/>
     <cellStyle name="Normal 50 4" xfId="2109" xr:uid="{27280868-ECF2-4D7D-8DEB-75C7CAA06413}"/>
@@ -5554,6 +5548,7 @@
     <cellStyle name="Normal 50 6" xfId="2215" xr:uid="{32168E51-5EEA-48F6-B78B-D5D641208253}"/>
     <cellStyle name="Normal 50 7" xfId="2269" xr:uid="{DC181CFA-13CC-4B2F-B891-3E3CF592BB02}"/>
     <cellStyle name="Normal 50 8" xfId="2323" xr:uid="{75A7C4B9-3FE6-4180-AA85-67592ABAF173}"/>
+    <cellStyle name="Normal 50 9" xfId="2377" xr:uid="{17CA0364-118F-4F64-99D0-9C535EAEFD78}"/>
     <cellStyle name="Normal 51" xfId="2007" xr:uid="{1602E624-09BF-4F71-AF6A-9A39C4FDA28D}"/>
     <cellStyle name="Normal 51 2" xfId="2057" xr:uid="{05B9550F-EDC2-4B34-8448-0CE71335699D}"/>
     <cellStyle name="Normal 51 3" xfId="2110" xr:uid="{EEADDD94-46EB-4534-81FD-415BB9146977}"/>
@@ -5561,27 +5556,39 @@
     <cellStyle name="Normal 51 5" xfId="2216" xr:uid="{D17E7BA8-3116-4F5F-8179-74E08399A4EF}"/>
     <cellStyle name="Normal 51 6" xfId="2270" xr:uid="{D651389D-4352-41F9-AB5A-43DC398B80DD}"/>
     <cellStyle name="Normal 51 7" xfId="2324" xr:uid="{FCC29057-9F84-494B-A087-84A367B80F4E}"/>
+    <cellStyle name="Normal 51 8" xfId="2378" xr:uid="{CA89F152-B08F-4A80-A825-FC8BAF49EA75}"/>
+    <cellStyle name="Normal 51 9" xfId="2433" xr:uid="{87E97C19-6A6E-44A6-A765-32E185B6092D}"/>
     <cellStyle name="Normal 52" xfId="2058" xr:uid="{0CE4F744-196E-4D85-989F-D205FE46F16C}"/>
     <cellStyle name="Normal 52 2" xfId="2111" xr:uid="{2C609632-C4ED-40F2-8062-2BB9333D71A1}"/>
     <cellStyle name="Normal 52 3" xfId="2164" xr:uid="{38502271-BE6F-47FA-9158-64F5F05DCB08}"/>
     <cellStyle name="Normal 52 4" xfId="2217" xr:uid="{BB0FA74F-2845-479E-940A-6418FF10EDEA}"/>
     <cellStyle name="Normal 52 5" xfId="2271" xr:uid="{7EDE6A6E-6245-40E0-AAE7-27AB621DE21E}"/>
     <cellStyle name="Normal 52 6" xfId="2325" xr:uid="{8AF073A8-07B1-4AEC-893E-12DA8FB05D8D}"/>
+    <cellStyle name="Normal 52 7" xfId="2379" xr:uid="{8953833D-E593-45FB-BA9A-89DE85F3367D}"/>
+    <cellStyle name="Normal 52 8" xfId="2434" xr:uid="{2C5D1FE8-E7B2-4688-A30D-AA204DEF33CF}"/>
     <cellStyle name="Normal 53" xfId="2059" xr:uid="{3EE05AE3-F5B9-4F71-93D8-B780EEE67BD1}"/>
     <cellStyle name="Normal 53 2" xfId="2112" xr:uid="{16C62648-6EA8-4037-9ED8-095F822FF00A}"/>
     <cellStyle name="Normal 53 3" xfId="2165" xr:uid="{06B1AB3E-FD03-476B-ABB1-E3CA9C13FD86}"/>
     <cellStyle name="Normal 53 4" xfId="2218" xr:uid="{3C01CD0D-BB46-489D-BB4D-0F40A7561659}"/>
     <cellStyle name="Normal 53 5" xfId="2272" xr:uid="{9A948023-87A5-454D-B748-B968765580AB}"/>
     <cellStyle name="Normal 53 6" xfId="2326" xr:uid="{E0E0C773-FA00-483B-9072-C942818E34A4}"/>
+    <cellStyle name="Normal 53 7" xfId="2380" xr:uid="{2072F87A-F786-48EC-A7D2-AE91A3BEB1E5}"/>
+    <cellStyle name="Normal 53 8" xfId="2435" xr:uid="{5C97FA71-FC66-4909-9C05-A3B7FB57E66D}"/>
     <cellStyle name="Normal 54" xfId="2060" xr:uid="{AE4474E6-4D1D-4C68-ACD4-E1952962F9F8}"/>
     <cellStyle name="Normal 54 2" xfId="2113" xr:uid="{52C4B073-4C53-40E7-A256-18B3D9AD7A02}"/>
     <cellStyle name="Normal 54 3" xfId="2166" xr:uid="{5464CF50-21BE-4C16-B689-EB526957E877}"/>
     <cellStyle name="Normal 54 4" xfId="2219" xr:uid="{DFDA0EC6-330A-4F76-B02D-67ECB9E2963B}"/>
     <cellStyle name="Normal 54 5" xfId="2273" xr:uid="{644BA510-66C4-42CC-A3EC-7F9DAFD552F7}"/>
     <cellStyle name="Normal 54 6" xfId="2327" xr:uid="{55EF33D0-6E3D-455B-A82B-6A9C2F6B3BAC}"/>
+    <cellStyle name="Normal 54 7" xfId="2381" xr:uid="{05B083E7-E93A-465F-AD6D-116CF354D2B0}"/>
+    <cellStyle name="Normal 54 8" xfId="2436" xr:uid="{B7883CF5-9F52-4891-BAA2-505887CBE3B9}"/>
     <cellStyle name="Normal 55" xfId="2220" xr:uid="{F2DBE977-3055-4B8C-8DB1-9063802CB3CE}"/>
     <cellStyle name="Normal 55 2" xfId="2274" xr:uid="{2AFC1409-514C-44F8-A16A-009B4AAA5942}"/>
     <cellStyle name="Normal 55 3" xfId="2328" xr:uid="{1779E91A-B6EE-4CCD-A0AA-3104AAC79AD1}"/>
+    <cellStyle name="Normal 55 4" xfId="2382" xr:uid="{82A622E9-AAF1-4266-998C-63CC070A21C0}"/>
+    <cellStyle name="Normal 55 5" xfId="2437" xr:uid="{A3132FCE-3118-4D83-BD66-780B5BB8B4B9}"/>
+    <cellStyle name="Normal 56" xfId="2383" xr:uid="{A9CCEEB6-8E80-47DA-918C-160799DDECFE}"/>
+    <cellStyle name="Normal 56 2" xfId="2438" xr:uid="{EA476B24-9472-4541-8F5A-FCAE56DDBF2E}"/>
     <cellStyle name="Normal 6" xfId="5" xr:uid="{31BE2080-B222-435D-8A48-DEEADDEF6488}"/>
     <cellStyle name="Normal 6 10" xfId="62" xr:uid="{F76AEC00-2B15-423C-8653-788DAF9DBB9C}"/>
     <cellStyle name="Normal 6 11" xfId="69" xr:uid="{69EF0E4C-7EAA-4CE4-BF59-7EC105A17AD6}"/>
@@ -5672,6 +5679,8 @@
     <cellStyle name="Normal 6 89" xfId="2225" xr:uid="{5A3FA82B-2247-4E84-9C7F-1CDF4678F3F9}"/>
     <cellStyle name="Normal 6 9" xfId="55" xr:uid="{F6988132-7CE0-49E6-B6AF-1F12276705C3}"/>
     <cellStyle name="Normal 6 90" xfId="2279" xr:uid="{06EE96EA-EAD6-468F-B2AF-96E6265EF28B}"/>
+    <cellStyle name="Normal 6 91" xfId="2333" xr:uid="{8A1D3E8B-D1A5-47A6-BBB2-C109B4871F0E}"/>
+    <cellStyle name="Normal 6 92" xfId="2388" xr:uid="{C135A5E6-5C3D-4830-89B5-3D0520DA2838}"/>
     <cellStyle name="Normal 7" xfId="6" xr:uid="{8FDF4D0E-5067-42C1-8AB6-21A2DD8B8199}"/>
     <cellStyle name="Normal 7 10" xfId="63" xr:uid="{076EEBFE-E343-48C7-AD51-40C5F37875B2}"/>
     <cellStyle name="Normal 7 11" xfId="70" xr:uid="{C92A195D-1E83-4EB3-9856-15A82899A737}"/>
@@ -5762,6 +5771,8 @@
     <cellStyle name="Normal 7 89" xfId="2226" xr:uid="{6E65A86B-FFA0-4794-A027-D6D5A42D6110}"/>
     <cellStyle name="Normal 7 9" xfId="56" xr:uid="{511FEC04-DA32-4322-AA1A-C9828FAC2A50}"/>
     <cellStyle name="Normal 7 90" xfId="2280" xr:uid="{3DA0ABFA-1CCE-4CA0-A956-CC53B58810BC}"/>
+    <cellStyle name="Normal 7 91" xfId="2334" xr:uid="{D477CCCE-F30D-43A7-9E53-C355DDF51A0B}"/>
+    <cellStyle name="Normal 7 92" xfId="2389" xr:uid="{E03EC799-9821-4D71-B66B-72F90FBE39B6}"/>
     <cellStyle name="Normal 8" xfId="43" xr:uid="{B3C5BFDC-2A95-4E6A-803F-B149318E48CC}"/>
     <cellStyle name="Normal 8 10" xfId="109" xr:uid="{2C5F0F9A-3251-494A-998A-DF2DB5E1065F}"/>
     <cellStyle name="Normal 8 11" xfId="117" xr:uid="{A66804B5-EC5B-4C85-82CD-D00400FFCA77}"/>
@@ -5845,6 +5856,8 @@
     <cellStyle name="Normal 8 82" xfId="2173" xr:uid="{07616DCE-72F7-4CC5-B43B-1BC07089989D}"/>
     <cellStyle name="Normal 8 83" xfId="2227" xr:uid="{C13360E3-3A65-4AC7-BB51-E75B28873577}"/>
     <cellStyle name="Normal 8 84" xfId="2281" xr:uid="{60C0B795-2541-486C-9198-8DC05CA563AD}"/>
+    <cellStyle name="Normal 8 85" xfId="2335" xr:uid="{AAD6890D-63DB-4C8A-8A32-998ED113A0BF}"/>
+    <cellStyle name="Normal 8 86" xfId="2390" xr:uid="{E132F386-A7C7-4587-8EB3-0AF430E209A1}"/>
     <cellStyle name="Normal 8 9" xfId="101" xr:uid="{EF361D85-BD7F-4E58-9FE7-65473E5583EE}"/>
     <cellStyle name="Normal 9" xfId="86" xr:uid="{63C162E7-EB2C-460C-8F1B-D9BC4CBB1C65}"/>
     <cellStyle name="Normal 9 10" xfId="158" xr:uid="{EA44C88E-C9B8-4EDC-99A4-D9EF32DAD79D}"/>
@@ -5922,7 +5935,9 @@
     <cellStyle name="Normal 9 76" xfId="2174" xr:uid="{1D71255C-A503-4216-A336-8750E88242BA}"/>
     <cellStyle name="Normal 9 77" xfId="2228" xr:uid="{46932FCD-ABAD-430F-8F23-CBCEBDE50F82}"/>
     <cellStyle name="Normal 9 78" xfId="2282" xr:uid="{9F45FA21-7E20-434F-9A49-483B944788B7}"/>
+    <cellStyle name="Normal 9 79" xfId="2336" xr:uid="{C559C16F-DB6C-49BE-A51D-8CD882767249}"/>
     <cellStyle name="Normal 9 8" xfId="142" xr:uid="{E908BA3A-342A-42A4-9F3A-16B68FBD5C5D}"/>
+    <cellStyle name="Normal 9 80" xfId="2391" xr:uid="{4C05A15E-331E-4A69-BB5F-547555C33CB4}"/>
     <cellStyle name="Normal 9 9" xfId="150" xr:uid="{5810B583-F0FF-4873-A2AE-BF7471C0EA6E}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6223,10 +6238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD20"/>
+  <dimension ref="A1:CD7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6511,1246 +6526,188 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:82" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="P2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="7">
+        <v>22500</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="AC2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="6">
+        <v>33837</v>
+      </c>
+      <c r="AL2" s="6">
+        <v>32560</v>
+      </c>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BE2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="BF2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5"/>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2">
-        <v>41365</v>
-      </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI2" s="2"/>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="4">
-        <v>30400</v>
-      </c>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="2"/>
-      <c r="AN2" s="2"/>
-      <c r="AO2" s="2"/>
-      <c r="AP2" s="2"/>
-      <c r="AQ2" s="2"/>
-      <c r="AR2" s="2"/>
-      <c r="AS2" s="2"/>
-      <c r="AT2" s="2"/>
-      <c r="AU2" s="2"/>
-      <c r="AV2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW2" s="2"/>
-      <c r="AX2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ2" s="2"/>
-      <c r="BA2" s="2"/>
-      <c r="BB2" s="2"/>
-      <c r="BC2" s="2"/>
-      <c r="BD2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF2" s="2"/>
-      <c r="BG2" s="2"/>
-      <c r="BH2" s="2"/>
-      <c r="BI2" s="2"/>
-      <c r="BJ2" s="2"/>
-      <c r="BK2" s="2"/>
-      <c r="BL2" s="2"/>
-      <c r="BM2" s="2"/>
-      <c r="BN2" s="2"/>
-      <c r="BO2" s="2"/>
-      <c r="BP2" s="2"/>
-      <c r="BQ2" s="2"/>
-      <c r="BR2" s="2"/>
-      <c r="BS2" s="2"/>
-      <c r="BT2" s="2"/>
-      <c r="BU2" s="2"/>
-      <c r="BV2" s="2"/>
-      <c r="BW2" s="2"/>
-      <c r="BX2" s="2"/>
-      <c r="BY2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BZ2" s="2"/>
-      <c r="CA2" s="2"/>
-      <c r="CB2" s="2"/>
-      <c r="CC2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="CD2" s="2"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5"/>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5"/>
+      <c r="CD2" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="3" spans="1:82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2">
-        <v>40700</v>
-      </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
-      <c r="AK3" s="4">
-        <v>30400</v>
-      </c>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="2"/>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="2"/>
-      <c r="AP3" s="2"/>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
-      <c r="AS3" s="2"/>
-      <c r="AT3" s="2"/>
-      <c r="AU3" s="2"/>
-      <c r="AV3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW3" s="2"/>
-      <c r="AX3" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ3" s="2"/>
-      <c r="BA3" s="2"/>
-      <c r="BB3" s="2"/>
-      <c r="BC3" s="2"/>
-      <c r="BD3" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BE3" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF3" s="2"/>
-      <c r="BG3" s="2"/>
-      <c r="BH3" s="2"/>
-      <c r="BI3" s="2"/>
-      <c r="BJ3" s="2"/>
-      <c r="BK3" s="2"/>
-      <c r="BL3" s="2"/>
-      <c r="BM3" s="2"/>
-      <c r="BN3" s="2"/>
-      <c r="BO3" s="2"/>
-      <c r="BP3" s="2"/>
-      <c r="BQ3" s="2"/>
-      <c r="BR3" s="2"/>
-      <c r="BS3" s="2"/>
-      <c r="BT3" s="2"/>
-      <c r="BU3" s="2"/>
-      <c r="BV3" s="2"/>
-      <c r="BW3" s="2"/>
-      <c r="BX3" s="2"/>
-      <c r="BY3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BZ3" s="2"/>
-      <c r="CA3" s="2"/>
-      <c r="CB3" s="2"/>
-      <c r="CC3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="CD3" s="2"/>
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2">
-        <v>2150</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AJ4" s="2"/>
-      <c r="AK4" s="4">
-        <v>32157</v>
-      </c>
-      <c r="AL4" s="4">
-        <v>33435</v>
-      </c>
-      <c r="AM4" s="2"/>
-      <c r="AN4" s="2"/>
-      <c r="AO4" s="2"/>
-      <c r="AP4" s="2"/>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="2"/>
-      <c r="AT4" s="2"/>
-      <c r="AU4" s="2"/>
-      <c r="AV4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW4" s="2"/>
-      <c r="AX4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ4" s="2"/>
-      <c r="BA4" s="2"/>
-      <c r="BB4" s="2"/>
-      <c r="BC4" s="2"/>
-      <c r="BD4" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="BE4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF4" s="2"/>
-      <c r="BG4" s="2"/>
-      <c r="BH4" s="2"/>
-      <c r="BI4" s="2"/>
-      <c r="BJ4" s="2"/>
-      <c r="BK4" s="2"/>
-      <c r="BL4" s="2"/>
-      <c r="BM4" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="BN4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BO4" s="2"/>
-      <c r="BP4" s="2"/>
-      <c r="BQ4" s="2"/>
-      <c r="BR4" s="2"/>
-      <c r="BS4" s="2"/>
-      <c r="BT4" s="2"/>
-      <c r="BU4" s="2"/>
-      <c r="BV4" s="2"/>
-      <c r="BW4" s="2"/>
-      <c r="BX4" s="2"/>
-      <c r="BY4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="BZ4" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="CA4" s="2"/>
-      <c r="CB4" s="2"/>
-      <c r="CC4" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="CD4" s="2"/>
+      <c r="O4" s="4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2">
-        <v>12505</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="4">
-        <v>29782</v>
-      </c>
-      <c r="AL5" s="4">
-        <v>28737</v>
-      </c>
-      <c r="AM5" s="2"/>
-      <c r="AN5" s="2"/>
-      <c r="AO5" s="2"/>
-      <c r="AP5" s="2"/>
-      <c r="AQ5" s="2"/>
-      <c r="AR5" s="2"/>
-      <c r="AS5" s="2"/>
-      <c r="AT5" s="2"/>
-      <c r="AU5" s="2"/>
-      <c r="AV5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW5" s="2"/>
-      <c r="AX5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AY5" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ5" s="2"/>
-      <c r="BA5" s="2"/>
-      <c r="BB5" s="2"/>
-      <c r="BC5" s="2"/>
-      <c r="BD5" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BE5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF5" s="2"/>
-      <c r="BG5" s="2"/>
-      <c r="BH5" s="2"/>
-      <c r="BI5" s="2"/>
-      <c r="BJ5" s="2"/>
-      <c r="BK5" s="2"/>
-      <c r="BL5" s="2"/>
-      <c r="BM5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="BO5" s="2"/>
-      <c r="BP5" s="2"/>
-      <c r="BQ5" s="2"/>
-      <c r="BR5" s="2"/>
-      <c r="BS5" s="2"/>
-      <c r="BT5" s="2"/>
-      <c r="BU5" s="2"/>
-      <c r="BV5" s="2"/>
-      <c r="BW5" s="2"/>
-      <c r="BX5" s="2"/>
-      <c r="BY5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="BZ5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="CA5" s="2"/>
-      <c r="CB5" s="2"/>
-      <c r="CC5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="CD5" s="2"/>
+      <c r="T5" s="3"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
     </row>
     <row r="6" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2">
-        <v>30900</v>
-      </c>
-      <c r="U6" s="2"/>
-      <c r="V6" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="2"/>
-      <c r="AT6" s="2"/>
-      <c r="AU6" s="2"/>
-      <c r="AV6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW6" s="2"/>
-      <c r="AX6" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ6" s="2"/>
-      <c r="BA6" s="2"/>
-      <c r="BB6" s="2"/>
-      <c r="BC6" s="2"/>
-      <c r="BD6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="BE6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF6" s="2"/>
-      <c r="BG6" s="2"/>
-      <c r="BH6" s="2"/>
-      <c r="BI6" s="2"/>
-      <c r="BJ6" s="2"/>
-      <c r="BK6" s="2"/>
-      <c r="BL6" s="2"/>
-      <c r="BM6" s="2"/>
-      <c r="BN6" s="2"/>
-      <c r="BO6" s="2"/>
-      <c r="BP6" s="2"/>
-      <c r="BQ6" s="2"/>
-      <c r="BR6" s="2"/>
-      <c r="BS6" s="2"/>
-      <c r="BT6" s="2"/>
-      <c r="BU6" s="2"/>
-      <c r="BV6" s="2"/>
-      <c r="BW6" s="2">
-        <v>13475411</v>
-      </c>
-      <c r="BX6" s="2"/>
-      <c r="BY6" s="2"/>
-      <c r="BZ6" s="2"/>
-      <c r="CA6" s="2"/>
-      <c r="CB6" s="2"/>
-      <c r="CC6" s="2"/>
-      <c r="CD6" s="2"/>
+      <c r="T6" s="3"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2">
-        <v>42059</v>
-      </c>
-      <c r="U7" s="2"/>
-      <c r="V7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="4">
-        <v>28491</v>
-      </c>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
-      <c r="AQ7" s="2"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="2"/>
-      <c r="AT7" s="2"/>
-      <c r="AU7" s="2"/>
-      <c r="AV7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW7" s="2"/>
-      <c r="AX7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AY7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ7" s="2"/>
-      <c r="BA7" s="2"/>
-      <c r="BB7" s="2"/>
-      <c r="BC7" s="2"/>
-      <c r="BD7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="BE7" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF7" s="2"/>
-      <c r="BG7" s="2"/>
-      <c r="BH7" s="2"/>
-      <c r="BI7" s="2"/>
-      <c r="BJ7" s="2"/>
-      <c r="BK7" s="2"/>
-      <c r="BL7" s="2"/>
-      <c r="BM7" s="2"/>
-      <c r="BN7" s="2"/>
-      <c r="BO7" s="2"/>
-      <c r="BP7" s="2"/>
-      <c r="BQ7" s="2"/>
-      <c r="BR7" s="2"/>
-      <c r="BS7" s="2"/>
-      <c r="BT7" s="2"/>
-      <c r="BU7" s="2"/>
-      <c r="BV7" s="2"/>
-      <c r="BW7" s="2"/>
-      <c r="BX7" s="2"/>
-      <c r="BY7" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="BZ7" s="2"/>
-      <c r="CA7" s="2"/>
-      <c r="CB7" s="2"/>
-      <c r="CC7" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="CD7" s="2"/>
-    </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2">
-        <v>15500</v>
-      </c>
-      <c r="U8" s="2"/>
-      <c r="V8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-      <c r="AE8" s="2"/>
-      <c r="AF8" s="2"/>
-      <c r="AG8" s="2"/>
-      <c r="AH8" s="2"/>
-      <c r="AI8" s="2"/>
-      <c r="AJ8" s="2"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
-      <c r="AM8" s="2"/>
-      <c r="AN8" s="2"/>
-      <c r="AO8" s="2"/>
-      <c r="AP8" s="2"/>
-      <c r="AQ8" s="2"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="2"/>
-      <c r="AT8" s="2"/>
-      <c r="AU8" s="2"/>
-      <c r="AV8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW8" s="2"/>
-      <c r="AX8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ8" s="2"/>
-      <c r="BA8" s="2"/>
-      <c r="BB8" s="2"/>
-      <c r="BC8" s="2"/>
-      <c r="BD8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="BE8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF8" s="2"/>
-      <c r="BG8" s="2"/>
-      <c r="BH8" s="2"/>
-      <c r="BI8" s="2"/>
-      <c r="BJ8" s="2"/>
-      <c r="BK8" s="2"/>
-      <c r="BL8" s="2"/>
-      <c r="BM8" s="2"/>
-      <c r="BN8" s="2"/>
-      <c r="BO8" s="2"/>
-      <c r="BP8" s="2"/>
-      <c r="BQ8" s="2"/>
-      <c r="BR8" s="2"/>
-      <c r="BS8" s="2"/>
-      <c r="BT8" s="2"/>
-      <c r="BU8" s="2"/>
-      <c r="BV8" s="2"/>
-      <c r="BW8" s="2">
-        <v>13732527</v>
-      </c>
-      <c r="BX8" s="2"/>
-      <c r="BY8" s="2"/>
-      <c r="BZ8" s="2"/>
-      <c r="CA8" s="2"/>
-      <c r="CB8" s="2"/>
-      <c r="CC8" s="2">
-        <v>13732527</v>
-      </c>
-      <c r="CD8" s="2"/>
-    </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2"/>
-      <c r="V9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD9" s="2"/>
-      <c r="AE9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="AF9" s="2"/>
-      <c r="AG9" s="2"/>
-      <c r="AH9" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AJ9" s="2"/>
-      <c r="AK9" s="4">
-        <v>34881</v>
-      </c>
-      <c r="AL9" s="4">
-        <v>32744</v>
-      </c>
-      <c r="AM9" s="2"/>
-      <c r="AN9" s="2"/>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2"/>
-      <c r="AQ9" s="2"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2"/>
-      <c r="AT9" s="2"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW9" s="2"/>
-      <c r="AX9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
-      <c r="BB9" s="2"/>
-      <c r="BC9" s="2"/>
-      <c r="BD9" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="BE9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF9" s="2"/>
-      <c r="BG9" s="2"/>
-      <c r="BH9" s="2"/>
-      <c r="BI9" s="2"/>
-      <c r="BJ9" s="2"/>
-      <c r="BK9" s="2"/>
-      <c r="BL9" s="2"/>
-      <c r="BM9" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="BN9" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="BO9" s="2"/>
-      <c r="BP9" s="2"/>
-      <c r="BQ9" s="2"/>
-      <c r="BR9" s="2"/>
-      <c r="BS9" s="2"/>
-      <c r="BT9" s="2"/>
-      <c r="BU9" s="2"/>
-      <c r="BV9" s="2"/>
-      <c r="BW9" s="2"/>
-      <c r="BX9" s="2"/>
-      <c r="BY9" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="BZ9" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="CA9" s="2"/>
-      <c r="CB9" s="2"/>
-      <c r="CC9" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="CD9" s="2"/>
-    </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2">
-        <v>13420</v>
-      </c>
-      <c r="U10" s="2"/>
-      <c r="V10" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="AI10" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="4">
-        <v>18703</v>
-      </c>
-      <c r="AL10" s="4">
-        <v>28194</v>
-      </c>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
-      <c r="AQ10" s="2"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-      <c r="AU10" s="2"/>
-      <c r="AV10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AW10" s="2"/>
-      <c r="AX10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY10" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
-      <c r="BB10" s="2"/>
-      <c r="BC10" s="2"/>
-      <c r="BD10" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BE10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BF10" s="2"/>
-      <c r="BG10" s="2"/>
-      <c r="BH10" s="2"/>
-      <c r="BI10" s="2"/>
-      <c r="BJ10" s="2"/>
-      <c r="BK10" s="2"/>
-      <c r="BL10" s="2"/>
-      <c r="BM10" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="BN10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="BO10" s="2"/>
-      <c r="BP10" s="2"/>
-      <c r="BQ10" s="2"/>
-      <c r="BR10" s="2"/>
-      <c r="BS10" s="2"/>
-      <c r="BT10" s="2"/>
-      <c r="BU10" s="2"/>
-      <c r="BV10" s="2"/>
-      <c r="BW10" s="2"/>
-      <c r="BX10" s="2"/>
-      <c r="BY10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BZ10" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="CA10" s="2"/>
-      <c r="CB10" s="2"/>
-      <c r="CC10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="CD10" s="2"/>
-    </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AZ7"/>
+      <c r="BA7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Code updated to lastest run
</commit_message>
<xml_diff>
--- a/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
+++ b/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Taylors\DocumentUnderstandingFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCA9BB-BA6A-4EFE-83DC-5C38EC011466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7365F03-BD69-4EC2-BF27-714833042D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
   <si>
     <t>Insight Ref</t>
   </si>
@@ -274,71 +274,122 @@
     <t>No</t>
   </si>
   <si>
-    <t>Freehold</t>
-  </si>
-  <si>
-    <t>MRT1723</t>
-  </si>
-  <si>
-    <t>Katarzyna Maria Szczerba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17B Church Rise, London, </t>
-  </si>
-  <si>
-    <t>Lewisham</t>
-  </si>
-  <si>
-    <t>Michael Brian Wood</t>
-  </si>
-  <si>
-    <t>17b Church Rise, Forest Hill, London, SE23 2UD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Katarzyna Maria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pierre Mathieu </t>
-  </si>
-  <si>
-    <t>Szczerba</t>
-  </si>
-  <si>
-    <t>Blacque- Florentin</t>
-  </si>
-  <si>
-    <t>SGL507353</t>
-  </si>
-  <si>
-    <t>Michael Brian Wood and Claire Jessica Harding</t>
-  </si>
-  <si>
-    <t>17B Church Rise, London</t>
-  </si>
-  <si>
-    <t>SE23 2UD</t>
-  </si>
-  <si>
-    <t>Claire Jessica Harding</t>
-  </si>
-  <si>
-    <t>17B Church Rise, Forest Hill, London, SE23 2UD</t>
-  </si>
-  <si>
-    <t>Pierre Mathieu Blacque- Florentin</t>
-  </si>
-  <si>
-    <t>SN352872A</t>
-  </si>
-  <si>
-    <t>SN382090C</t>
+    <t>Leasehold</t>
+  </si>
+  <si>
+    <t>NNT1028</t>
+  </si>
+  <si>
+    <t>Beenish Ali</t>
+  </si>
+  <si>
+    <t>39 Parkes Avenue, Birmingham</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>GALLIARD WAVENSMERE (MIDDLEWAY) LIMITED</t>
+  </si>
+  <si>
+    <t>3rd Floor Sterling House Langston Road Loughton Essex IG10 3TS</t>
+  </si>
+  <si>
+    <t>12/31/3021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beenish </t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>B12 9AW</t>
+  </si>
+  <si>
+    <t>SC809688A</t>
+  </si>
+  <si>
+    <t>NBT1872</t>
+  </si>
+  <si>
+    <t>Marius Catalin Voica</t>
+  </si>
+  <si>
+    <t>17 Elder Crescent, St Neots</t>
+  </si>
+  <si>
+    <t>Huntingdon</t>
+  </si>
+  <si>
+    <t>DURKAN (ST NEOTS) LIMITED</t>
+  </si>
+  <si>
+    <t>4 Elstree Gate, Elstree Way, Borehamwood, WD6 1JD</t>
+  </si>
+  <si>
+    <t>05/30/3021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marius Catalin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria-Magdalena </t>
+  </si>
+  <si>
+    <t>Voica</t>
+  </si>
+  <si>
+    <t>PE19 0BF</t>
+  </si>
+  <si>
+    <t>SS438175D</t>
+  </si>
+  <si>
+    <t>ST210146C</t>
+  </si>
+  <si>
+    <t>NNT1227</t>
+  </si>
+  <si>
+    <t>Silje Merete Saethren Gronning</t>
+  </si>
+  <si>
+    <t>37 Pembrey Court, Bollo Lane</t>
+  </si>
+  <si>
+    <t>Ealing</t>
+  </si>
+  <si>
+    <t>ACTON GARDENS LLP</t>
+  </si>
+  <si>
+    <t>Countryside House The Drive Brentwood Essex CM13 3AT</t>
+  </si>
+  <si>
+    <t>01/29/2021</t>
+  </si>
+  <si>
+    <t>01/25/2271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silje Merete Saethren </t>
+  </si>
+  <si>
+    <t>Gronning</t>
+  </si>
+  <si>
+    <t>W3 8QR</t>
+  </si>
+  <si>
+    <t>SY217118C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="99" x14ac:knownFonts="1">
+  <fonts count="104" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1023,6 +1074,40 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1048,13 +1133,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2439">
+  <cellStyleXfs count="2659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
@@ -1068,6 +1177,8 @@
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
@@ -1080,6 +1191,8 @@
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
@@ -1107,6 +1220,8 @@
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="84" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="83" fillId="0" borderId="0"/>
@@ -1121,6 +1236,8 @@
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="81" fillId="0" borderId="0"/>
@@ -1176,6 +1293,9 @@
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
@@ -1192,6 +1312,9 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
@@ -1200,6 +1323,14 @@
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
@@ -1219,6 +1350,14 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
@@ -1242,6 +1381,14 @@
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
@@ -1269,6 +1416,14 @@
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
@@ -1300,6 +1455,13 @@
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
@@ -1335,6 +1497,9 @@
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
@@ -1394,6 +1559,8 @@
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
@@ -1434,6 +1601,8 @@
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
@@ -1454,6 +1623,9 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
@@ -1496,6 +1668,9 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
@@ -1540,6 +1715,11 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
@@ -1585,6 +1765,14 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0"/>
@@ -1632,6 +1820,11 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
@@ -1792,6 +1985,8 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
@@ -1846,6 +2041,8 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
@@ -1873,6 +2070,9 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
@@ -1929,6 +2129,10 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
@@ -1987,6 +2191,14 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
@@ -2046,6 +2258,17 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
@@ -2109,6 +2332,19 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
@@ -2178,6 +2414,17 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
@@ -2254,6 +2501,12 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
@@ -2335,6 +2588,11 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
@@ -2419,6 +2677,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
@@ -2595,6 +2857,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
@@ -2683,6 +2946,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
@@ -2773,6 +3041,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
@@ -2863,6 +3138,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
@@ -2958,6 +3243,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
@@ -3057,6 +3351,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
@@ -3163,6 +3462,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
@@ -3216,6 +3516,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -3324,6 +3627,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -3489,17 +3794,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2439">
+  <cellStyles count="2659">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="159" xr:uid="{22378139-A9D0-4012-B7E1-FB95B8397E06}"/>
     <cellStyle name="Normal 10 10" xfId="276" xr:uid="{2FF1057A-C0FD-428A-B8F5-F70C6C4ED22C}"/>
@@ -3570,6 +3878,10 @@
     <cellStyle name="Normal 10 7" xfId="228" xr:uid="{267F1CFF-9F4B-436A-AEEC-36F3EF937E54}"/>
     <cellStyle name="Normal 10 70" xfId="2337" xr:uid="{6AF9F2A8-BD6D-4090-98D2-C3FA834F8D6A}"/>
     <cellStyle name="Normal 10 71" xfId="2392" xr:uid="{B54803D1-1FBD-49E8-A559-9E1C0366BC41}"/>
+    <cellStyle name="Normal 10 72" xfId="2447" xr:uid="{570629E8-79D5-4395-828F-5FE5D78887AE}"/>
+    <cellStyle name="Normal 10 73" xfId="2502" xr:uid="{8AF875CF-F651-4302-A3AA-3E7056484FC8}"/>
+    <cellStyle name="Normal 10 74" xfId="2557" xr:uid="{49E28582-A60D-4E32-B0D2-7FE8CAE252C0}"/>
+    <cellStyle name="Normal 10 75" xfId="2612" xr:uid="{EC917C18-EB20-4349-B638-A60B5299BAB4}"/>
     <cellStyle name="Normal 10 8" xfId="243" xr:uid="{731BFDFC-42EF-40DB-B469-49423BAFDD34}"/>
     <cellStyle name="Normal 10 9" xfId="259" xr:uid="{C9BCE7F2-A0DC-424E-BD2A-3833A66918FA}"/>
     <cellStyle name="Normal 11" xfId="169" xr:uid="{24883276-07D4-417F-A269-AF8F8014D6B0}"/>
@@ -3640,6 +3952,10 @@
     <cellStyle name="Normal 11 69" xfId="2338" xr:uid="{EC2E0160-8B90-4700-8AE5-F6F4DD62D0EF}"/>
     <cellStyle name="Normal 11 7" xfId="244" xr:uid="{3EAFC835-4A7D-45CE-AE77-990DDEAAFDC0}"/>
     <cellStyle name="Normal 11 70" xfId="2393" xr:uid="{6D271227-DFD7-4B1C-AF1B-4F79A7D80EDB}"/>
+    <cellStyle name="Normal 11 71" xfId="2448" xr:uid="{B8FBF655-531F-4197-9021-4C5426255FAC}"/>
+    <cellStyle name="Normal 11 72" xfId="2503" xr:uid="{2DFE5952-5804-4494-974F-A1A32EFB97D8}"/>
+    <cellStyle name="Normal 11 73" xfId="2558" xr:uid="{AC4A5DD0-35B8-4401-BAED-320FE3BEA9E9}"/>
+    <cellStyle name="Normal 11 74" xfId="2613" xr:uid="{FCF100BA-F732-4A2A-8BD9-F8B34A42C056}"/>
     <cellStyle name="Normal 11 8" xfId="260" xr:uid="{F04D5FA1-BA3E-4D95-B369-72C9BC4A33B2}"/>
     <cellStyle name="Normal 11 9" xfId="277" xr:uid="{2BA3F0B3-DDFB-4ED8-8F9B-FB1DE74EA628}"/>
     <cellStyle name="Normal 12" xfId="180" xr:uid="{64C12A1D-7934-48F2-9578-4F1C04C3D62D}"/>
@@ -3709,6 +4025,10 @@
     <cellStyle name="Normal 12 68" xfId="2339" xr:uid="{B423458D-728F-44E9-9CAB-11D9C3A57F13}"/>
     <cellStyle name="Normal 12 69" xfId="2394" xr:uid="{2B8431ED-EBFA-4D86-96A7-1791264F5ADE}"/>
     <cellStyle name="Normal 12 7" xfId="261" xr:uid="{83DDF630-CAFE-4366-8DB0-A3134118B594}"/>
+    <cellStyle name="Normal 12 70" xfId="2449" xr:uid="{542AD60F-347C-4CAB-86BC-629DA3C8CCA0}"/>
+    <cellStyle name="Normal 12 71" xfId="2504" xr:uid="{3615E3BD-D9C4-4BAB-885E-EFA81AACADDB}"/>
+    <cellStyle name="Normal 12 72" xfId="2559" xr:uid="{FF88AEF1-874E-4270-97A7-9EC34BE1C4CD}"/>
+    <cellStyle name="Normal 12 73" xfId="2614" xr:uid="{F6CCAAA2-324E-4AEA-BF07-043F0A246A18}"/>
     <cellStyle name="Normal 12 8" xfId="278" xr:uid="{F6B4CBEB-461D-400D-9C34-7FB47B2F92C3}"/>
     <cellStyle name="Normal 12 9" xfId="296" xr:uid="{030E8C75-BAB4-4848-8367-E74DEC184755}"/>
     <cellStyle name="Normal 13" xfId="192" xr:uid="{6C53067C-9D55-4747-9EF8-9B2403AC3FD0}"/>
@@ -3776,7 +4096,11 @@
     <cellStyle name="Normal 13 66" xfId="2286" xr:uid="{383FAE42-0127-4E2D-B79E-9CCC5E40F900}"/>
     <cellStyle name="Normal 13 67" xfId="2340" xr:uid="{20C31C95-B57F-4B02-B667-FB76C66C9674}"/>
     <cellStyle name="Normal 13 68" xfId="2395" xr:uid="{47E0422F-177D-4FB0-B60C-0CBAE2D3DB26}"/>
+    <cellStyle name="Normal 13 69" xfId="2450" xr:uid="{C693F131-1443-435C-B8F3-7C97AC75AD24}"/>
     <cellStyle name="Normal 13 7" xfId="279" xr:uid="{2D9D628C-A27B-4B86-8C7E-7C9804E457BC}"/>
+    <cellStyle name="Normal 13 70" xfId="2505" xr:uid="{C64E3BA5-FF66-43EF-BFD7-75D5FEA3EDDA}"/>
+    <cellStyle name="Normal 13 71" xfId="2560" xr:uid="{C99F9691-E2FA-4D52-BDFA-E514FB7B812B}"/>
+    <cellStyle name="Normal 13 72" xfId="2615" xr:uid="{7A83B077-482A-4B51-9768-C62DA4F9B90F}"/>
     <cellStyle name="Normal 13 8" xfId="297" xr:uid="{4A5D7C9D-C5C5-40A5-8715-701C74A7B825}"/>
     <cellStyle name="Normal 13 9" xfId="316" xr:uid="{62B80AA8-8706-4987-866E-1A4286CD93CB}"/>
     <cellStyle name="Normal 14" xfId="205" xr:uid="{BCD27467-3820-4B0C-8969-F2BEB1D1C65E}"/>
@@ -3843,7 +4167,11 @@
     <cellStyle name="Normal 14 65" xfId="2287" xr:uid="{19D61C33-98A2-4173-AB9B-E40113E087DC}"/>
     <cellStyle name="Normal 14 66" xfId="2341" xr:uid="{CC58DE51-6FC2-4826-BEEA-B6F7806042D4}"/>
     <cellStyle name="Normal 14 67" xfId="2396" xr:uid="{9CBB6B57-ACBB-4988-A69F-89E2CF9EA0AB}"/>
+    <cellStyle name="Normal 14 68" xfId="2451" xr:uid="{D8822773-C721-49B9-8686-CF539D1DB053}"/>
+    <cellStyle name="Normal 14 69" xfId="2506" xr:uid="{8AE28513-27A0-441D-975C-DCEB0194AFCE}"/>
     <cellStyle name="Normal 14 7" xfId="298" xr:uid="{CD68E702-2F82-4764-9927-11DABC2F5829}"/>
+    <cellStyle name="Normal 14 70" xfId="2561" xr:uid="{7817E3AD-CD9D-4811-A502-04BB718C11BF}"/>
+    <cellStyle name="Normal 14 71" xfId="2616" xr:uid="{1EEA5952-33B0-4DE5-91F2-2A9BBA452B97}"/>
     <cellStyle name="Normal 14 8" xfId="317" xr:uid="{6DB7F330-9C64-4B26-AF4F-17A09E12CEC6}"/>
     <cellStyle name="Normal 14 9" xfId="337" xr:uid="{104D5C09-BA78-4885-AA2B-E347E11C3013}"/>
     <cellStyle name="Normal 15" xfId="219" xr:uid="{AFBD9F23-4328-44E1-ABF9-3CA063A03969}"/>
@@ -3909,7 +4237,11 @@
     <cellStyle name="Normal 15 64" xfId="2288" xr:uid="{37E8890E-A66E-4B4F-8104-4017DE5D9878}"/>
     <cellStyle name="Normal 15 65" xfId="2342" xr:uid="{B5581F79-5361-439D-8669-4102E08F839E}"/>
     <cellStyle name="Normal 15 66" xfId="2397" xr:uid="{C97F2FF7-D326-4A21-9CE0-A21A9C68AE6F}"/>
+    <cellStyle name="Normal 15 67" xfId="2452" xr:uid="{39C84769-4A8F-49A0-841C-0D88ACDC05C4}"/>
+    <cellStyle name="Normal 15 68" xfId="2507" xr:uid="{673A436A-C802-428D-A7BD-4176A8DF6A42}"/>
+    <cellStyle name="Normal 15 69" xfId="2562" xr:uid="{972B9C56-438D-45D8-9D24-C5C9558B9A4A}"/>
     <cellStyle name="Normal 15 7" xfId="318" xr:uid="{BC74AE1A-9CA6-4EA4-BFD8-B522F63CB6FF}"/>
+    <cellStyle name="Normal 15 70" xfId="2617" xr:uid="{1D79FB92-1D04-47CD-B5E8-80E88211DD5B}"/>
     <cellStyle name="Normal 15 8" xfId="338" xr:uid="{52CEAA3B-3AF8-4A6A-ADD3-4403D3D982ED}"/>
     <cellStyle name="Normal 15 9" xfId="358" xr:uid="{52621DB2-9BFC-4EF1-B2FF-A1D2EBD982F8}"/>
     <cellStyle name="Normal 16" xfId="234" xr:uid="{E124F5C7-1AAD-4493-AE1C-3BD849B8317F}"/>
@@ -3974,6 +4306,10 @@
     <cellStyle name="Normal 16 63" xfId="2289" xr:uid="{E5EDA437-73CB-4309-8F89-6D6C3CC00A52}"/>
     <cellStyle name="Normal 16 64" xfId="2343" xr:uid="{554CC56B-E56F-4FC5-803A-F93332F5EFCF}"/>
     <cellStyle name="Normal 16 65" xfId="2398" xr:uid="{2CCE9BA0-146A-44DC-9107-50616C3BCBDC}"/>
+    <cellStyle name="Normal 16 66" xfId="2453" xr:uid="{EA26E797-9DF0-438C-895B-91D1D1B201B1}"/>
+    <cellStyle name="Normal 16 67" xfId="2508" xr:uid="{89D1DFD3-C573-420D-9211-A580908A005E}"/>
+    <cellStyle name="Normal 16 68" xfId="2563" xr:uid="{76850B5F-C664-4D3E-A016-922E180CB12B}"/>
+    <cellStyle name="Normal 16 69" xfId="2618" xr:uid="{5A2B1924-4398-4DE5-AC88-3FB28BCB6039}"/>
     <cellStyle name="Normal 16 7" xfId="339" xr:uid="{FAA81CF7-9E8B-4D43-8B87-FEA4DEA195A2}"/>
     <cellStyle name="Normal 16 8" xfId="359" xr:uid="{71945961-3DA4-41F9-B589-733CD154B56B}"/>
     <cellStyle name="Normal 16 9" xfId="379" xr:uid="{2D615019-0C6B-4533-BF0F-B9FB56006E3E}"/>
@@ -4038,6 +4374,10 @@
     <cellStyle name="Normal 17 62" xfId="2290" xr:uid="{AA8020A6-90EC-45DD-AF0E-DCC2A23AF4C2}"/>
     <cellStyle name="Normal 17 63" xfId="2344" xr:uid="{0C62EA86-D42E-48CE-ADC8-3297522089DB}"/>
     <cellStyle name="Normal 17 64" xfId="2399" xr:uid="{99F82004-39D7-4B04-B53C-8B36B0136401}"/>
+    <cellStyle name="Normal 17 65" xfId="2454" xr:uid="{2E86E913-02BD-4EE1-820B-55BB660795B4}"/>
+    <cellStyle name="Normal 17 66" xfId="2509" xr:uid="{B7EC4B85-098B-4390-9F9C-776C10F548B2}"/>
+    <cellStyle name="Normal 17 67" xfId="2564" xr:uid="{6936AE38-FA2C-4289-B99B-6C91220C7710}"/>
+    <cellStyle name="Normal 17 68" xfId="2619" xr:uid="{9C851FCC-8BF9-4A5B-B2FE-1763AD5FDB0F}"/>
     <cellStyle name="Normal 17 7" xfId="360" xr:uid="{EF50DC9C-CCDF-49C3-BD04-EC1F385C2EB2}"/>
     <cellStyle name="Normal 17 8" xfId="380" xr:uid="{F7FF7910-81D8-41FE-87E6-74E265C4FE49}"/>
     <cellStyle name="Normal 17 9" xfId="400" xr:uid="{0131EC3E-0935-425F-A406-A9A4A62BE59C}"/>
@@ -4101,6 +4441,10 @@
     <cellStyle name="Normal 18 61" xfId="2291" xr:uid="{92331A33-9B7A-4686-95A9-FC3B065D72F4}"/>
     <cellStyle name="Normal 18 62" xfId="2345" xr:uid="{1B5483A4-1DA1-4A8A-8066-EAD76FE37848}"/>
     <cellStyle name="Normal 18 63" xfId="2400" xr:uid="{67645393-6B54-41BA-9ECD-63C645356B52}"/>
+    <cellStyle name="Normal 18 64" xfId="2455" xr:uid="{AE246BD2-A085-4EF2-8122-FD1CE760D2A7}"/>
+    <cellStyle name="Normal 18 65" xfId="2510" xr:uid="{45DA049D-DA2E-4ABA-9720-CEFEACB7FBF1}"/>
+    <cellStyle name="Normal 18 66" xfId="2565" xr:uid="{4B7414EA-3337-48F6-A515-DAB45D1E7FB1}"/>
+    <cellStyle name="Normal 18 67" xfId="2620" xr:uid="{CDCE5D23-5134-4657-AB84-108242296EBF}"/>
     <cellStyle name="Normal 18 7" xfId="381" xr:uid="{AA0AB4C2-AC98-4892-8993-9C51D645351A}"/>
     <cellStyle name="Normal 18 8" xfId="401" xr:uid="{97EBEF4A-C9B9-484A-A9B8-2BD6E9C715B6}"/>
     <cellStyle name="Normal 18 9" xfId="421" xr:uid="{E88C8D00-A684-4B81-9E3E-D25CD466C39D}"/>
@@ -4163,6 +4507,10 @@
     <cellStyle name="Normal 19 60" xfId="2292" xr:uid="{18D3992C-C8CC-45C4-B22A-DB4F56CC3651}"/>
     <cellStyle name="Normal 19 61" xfId="2346" xr:uid="{4A485BF6-DB43-4F04-8375-658BA274D870}"/>
     <cellStyle name="Normal 19 62" xfId="2401" xr:uid="{7978AFB6-E21D-4EF3-AAD4-EAA63A4D14AE}"/>
+    <cellStyle name="Normal 19 63" xfId="2456" xr:uid="{1F2796A6-7C11-416B-B99D-C223A6862267}"/>
+    <cellStyle name="Normal 19 64" xfId="2511" xr:uid="{51901CFF-9289-4D93-A0F9-181AA2258AD0}"/>
+    <cellStyle name="Normal 19 65" xfId="2566" xr:uid="{5A011BA0-47FF-430C-A91E-9A5AF35EB2F0}"/>
+    <cellStyle name="Normal 19 66" xfId="2621" xr:uid="{53DC0A07-674B-4744-A10C-FB1CD3088EAB}"/>
     <cellStyle name="Normal 19 7" xfId="402" xr:uid="{7C70AE42-3659-4E21-B1E7-5A2B14B05D2D}"/>
     <cellStyle name="Normal 19 8" xfId="422" xr:uid="{258ACE1C-8C37-43E9-8F9E-504F66369A2C}"/>
     <cellStyle name="Normal 19 9" xfId="443" xr:uid="{AED5C701-AD5D-4D29-BEA5-DC3E31B13CEA}"/>
@@ -4258,6 +4606,10 @@
     <cellStyle name="Normal 2 90" xfId="2275" xr:uid="{26A141F5-DF12-4532-9EC1-5C4AA47F9FB1}"/>
     <cellStyle name="Normal 2 91" xfId="2329" xr:uid="{2FB8B8B4-D88E-4A7E-B88B-02CDD96C20BA}"/>
     <cellStyle name="Normal 2 92" xfId="2384" xr:uid="{5F89FF23-273B-4DAC-A8B3-C925288C6339}"/>
+    <cellStyle name="Normal 2 93" xfId="2439" xr:uid="{10EA13D2-92E1-456D-B66E-092A4905FF53}"/>
+    <cellStyle name="Normal 2 94" xfId="2494" xr:uid="{77880587-4369-48CD-94BD-0D5381A5EBB1}"/>
+    <cellStyle name="Normal 2 95" xfId="2549" xr:uid="{2F6F4E85-5134-450A-A2AE-91D593659995}"/>
+    <cellStyle name="Normal 2 96" xfId="2604" xr:uid="{E68285F5-DDC2-443D-B366-0D48402A7849}"/>
     <cellStyle name="Normal 20" xfId="304" xr:uid="{46E9EC2A-F4CD-4474-8F1F-128DC22F7FEE}"/>
     <cellStyle name="Normal 20 10" xfId="487" xr:uid="{7BB6CDCC-D9F1-4CB0-A7DC-4C2435A3C632}"/>
     <cellStyle name="Normal 20 11" xfId="509" xr:uid="{BC3D68B8-B4B0-466B-88F8-0FB74407A0D0}"/>
@@ -4316,6 +4668,10 @@
     <cellStyle name="Normal 20 6" xfId="403" xr:uid="{EDE2DB7C-D6C6-4FFB-9944-879D931D902B}"/>
     <cellStyle name="Normal 20 60" xfId="2347" xr:uid="{EC1B911F-0406-4638-8B43-775F966355F1}"/>
     <cellStyle name="Normal 20 61" xfId="2402" xr:uid="{CE530E64-C64A-4892-89C0-F9E0D96226C8}"/>
+    <cellStyle name="Normal 20 62" xfId="2457" xr:uid="{977230EB-51E8-4C88-A519-3C076CA4CD30}"/>
+    <cellStyle name="Normal 20 63" xfId="2512" xr:uid="{45A6C02A-AC02-4447-A552-6858B635C221}"/>
+    <cellStyle name="Normal 20 64" xfId="2567" xr:uid="{4960C961-6572-4D98-9C70-EC5764237F0F}"/>
+    <cellStyle name="Normal 20 65" xfId="2622" xr:uid="{5E2CFFB7-5EAD-4F04-8726-7E5FDEBB8548}"/>
     <cellStyle name="Normal 20 7" xfId="423" xr:uid="{086835B6-4345-4031-B11A-51B0C72CE8BF}"/>
     <cellStyle name="Normal 20 8" xfId="444" xr:uid="{AB563AA1-827B-4C23-99CE-81D8ACA1B263}"/>
     <cellStyle name="Normal 20 9" xfId="465" xr:uid="{8753642A-194D-4639-8E76-06C881170BFA}"/>
@@ -4376,6 +4732,10 @@
     <cellStyle name="Normal 21 59" xfId="2348" xr:uid="{FB4B6430-E2E6-4FD6-9C08-27ED49C36461}"/>
     <cellStyle name="Normal 21 6" xfId="424" xr:uid="{697EF57E-FC1D-456D-A2E3-7187FCE63ED8}"/>
     <cellStyle name="Normal 21 60" xfId="2403" xr:uid="{22F3B7FD-8FE5-46C7-9284-4283A3DE614A}"/>
+    <cellStyle name="Normal 21 61" xfId="2458" xr:uid="{C84B03B1-7E5E-43EC-A51E-32B58E6AFF2F}"/>
+    <cellStyle name="Normal 21 62" xfId="2513" xr:uid="{73DE3A93-0B21-4690-9E41-0B93A8F62024}"/>
+    <cellStyle name="Normal 21 63" xfId="2568" xr:uid="{4F7E2053-8815-4594-868A-2A89B2ABC360}"/>
+    <cellStyle name="Normal 21 64" xfId="2623" xr:uid="{450C0F4B-1CFC-4ED9-944C-8E7EA9C3369D}"/>
     <cellStyle name="Normal 21 7" xfId="445" xr:uid="{1C2BB24F-B439-48A3-AEEA-D7AB69CCFDC1}"/>
     <cellStyle name="Normal 21 8" xfId="466" xr:uid="{5E3619D4-D275-4EB0-A165-F875F480DB0E}"/>
     <cellStyle name="Normal 21 9" xfId="488" xr:uid="{B9BF371B-ACB6-4682-B3CB-DE98962B0D2B}"/>
@@ -4430,6 +4790,10 @@
     <cellStyle name="Normal 22 53" xfId="2295" xr:uid="{17D870F7-133C-4111-AEC0-1C397AC42314}"/>
     <cellStyle name="Normal 22 54" xfId="2349" xr:uid="{393FD145-9595-4778-81E4-0E7053058E53}"/>
     <cellStyle name="Normal 22 55" xfId="2404" xr:uid="{6D9BDD54-182A-43EF-BF31-6BDF2EB6430B}"/>
+    <cellStyle name="Normal 22 56" xfId="2459" xr:uid="{8C2DB1BD-8544-4FFE-A46C-87544AD6920F}"/>
+    <cellStyle name="Normal 22 57" xfId="2514" xr:uid="{F2343005-C7C8-4736-9421-3626B11E6299}"/>
+    <cellStyle name="Normal 22 58" xfId="2569" xr:uid="{2BA44A11-0904-4BC4-BAE1-C39622B27FBB}"/>
+    <cellStyle name="Normal 22 59" xfId="2624" xr:uid="{E3DC98DA-C070-41FE-9005-F32402B04C50}"/>
     <cellStyle name="Normal 22 6" xfId="533" xr:uid="{6D06BD98-20DD-45B0-8C60-88A9912CEF28}"/>
     <cellStyle name="Normal 22 7" xfId="556" xr:uid="{C4538170-DB37-479E-96ED-6FC8842F1A26}"/>
     <cellStyle name="Normal 22 8" xfId="579" xr:uid="{E69F69A2-D4D9-4555-B390-12901B969277}"/>
@@ -4483,6 +4847,10 @@
     <cellStyle name="Normal 23 51" xfId="2296" xr:uid="{D525B771-3269-4E6E-973E-351C3A8CD281}"/>
     <cellStyle name="Normal 23 52" xfId="2350" xr:uid="{67833818-5129-42D8-818C-CE70B4C6E1F9}"/>
     <cellStyle name="Normal 23 53" xfId="2405" xr:uid="{19CB0872-A789-4EEA-A697-B19375F4B6DF}"/>
+    <cellStyle name="Normal 23 54" xfId="2460" xr:uid="{3D34159B-ED8D-4A1F-BB64-F5D971C7DF21}"/>
+    <cellStyle name="Normal 23 55" xfId="2515" xr:uid="{7ABA03C1-736E-4214-B8AD-51A3A1E8A334}"/>
+    <cellStyle name="Normal 23 56" xfId="2570" xr:uid="{3B7F3BE9-E1D7-4448-AEC2-CCB93619DD8D}"/>
+    <cellStyle name="Normal 23 57" xfId="2625" xr:uid="{3C0C10A5-14DE-49C2-BD4E-FFA26EF15C55}"/>
     <cellStyle name="Normal 23 6" xfId="580" xr:uid="{AAB043AD-CE0D-40DF-9A63-8A4C5A6D4F58}"/>
     <cellStyle name="Normal 23 7" xfId="604" xr:uid="{34A3DB58-17AE-4BF6-9728-A09FFBA397E1}"/>
     <cellStyle name="Normal 23 8" xfId="629" xr:uid="{F434F633-2719-4E36-A0A3-945AC33697C3}"/>
@@ -4533,6 +4901,10 @@
     <cellStyle name="Normal 24 49" xfId="2351" xr:uid="{8BBBA13F-D5A6-4D17-A26B-5AC251374C5F}"/>
     <cellStyle name="Normal 24 5" xfId="630" xr:uid="{EF3257C5-660E-46BC-92EF-B371A268B966}"/>
     <cellStyle name="Normal 24 50" xfId="2406" xr:uid="{FF89A4E2-CBB3-4CF1-820B-6D3AEC466467}"/>
+    <cellStyle name="Normal 24 51" xfId="2461" xr:uid="{89C41953-2D34-466E-B106-1BA9942D91D0}"/>
+    <cellStyle name="Normal 24 52" xfId="2516" xr:uid="{A82D1AB8-0B44-471A-A540-AABB5882FA4E}"/>
+    <cellStyle name="Normal 24 53" xfId="2571" xr:uid="{E8BE0504-92AD-475D-8C93-438A762CC47D}"/>
+    <cellStyle name="Normal 24 54" xfId="2626" xr:uid="{B6D35BBD-1EE9-46B4-958C-52F77CD36B82}"/>
     <cellStyle name="Normal 24 6" xfId="657" xr:uid="{32CD1B47-986E-462F-9668-4C8456D8C1B2}"/>
     <cellStyle name="Normal 24 7" xfId="684" xr:uid="{4CA8DE0A-B4AD-4241-8614-A270B05E4B04}"/>
     <cellStyle name="Normal 24 8" xfId="711" xr:uid="{C4B81C6D-EA33-4229-A72E-E576757A69AA}"/>
@@ -4580,7 +4952,11 @@
     <cellStyle name="Normal 25 46" xfId="2298" xr:uid="{91170925-8CF6-4E16-8978-AF71AD52EB30}"/>
     <cellStyle name="Normal 25 47" xfId="2352" xr:uid="{66108485-3E38-4511-BE80-6B3463342FD1}"/>
     <cellStyle name="Normal 25 48" xfId="2407" xr:uid="{E0C0AFC1-4590-4240-9197-3F84798DD155}"/>
+    <cellStyle name="Normal 25 49" xfId="2462" xr:uid="{225CF4CE-9A02-49AC-9D35-DE87119C35E9}"/>
     <cellStyle name="Normal 25 5" xfId="685" xr:uid="{DD6998FF-E097-4F7D-A460-95B18DABE8A9}"/>
+    <cellStyle name="Normal 25 50" xfId="2517" xr:uid="{8F0BD65E-6C64-4635-922D-F44DF59A8FC7}"/>
+    <cellStyle name="Normal 25 51" xfId="2572" xr:uid="{ED64F920-17F3-4E8C-8DF1-604C81AE3D9E}"/>
+    <cellStyle name="Normal 25 52" xfId="2627" xr:uid="{420ADA81-9315-4993-9997-BF3BD07ADBE4}"/>
     <cellStyle name="Normal 25 6" xfId="712" xr:uid="{829BB221-C705-476D-A467-70C6FED9B8ED}"/>
     <cellStyle name="Normal 25 7" xfId="739" xr:uid="{B64EF1EB-9F92-4BEC-BEAD-2E23DE7EC71A}"/>
     <cellStyle name="Normal 25 8" xfId="766" xr:uid="{88AEE39D-1A12-41B0-AF55-E0D06D5E7B20}"/>
@@ -4627,7 +5003,11 @@
     <cellStyle name="Normal 26 45" xfId="2299" xr:uid="{36644ADC-8F18-4CD8-82F2-5F6EDFE8309E}"/>
     <cellStyle name="Normal 26 46" xfId="2353" xr:uid="{8A495161-9B41-48C2-B731-E58D2D7FDF89}"/>
     <cellStyle name="Normal 26 47" xfId="2408" xr:uid="{8E8831B9-C32D-4746-A6BD-1B89DC3538E7}"/>
+    <cellStyle name="Normal 26 48" xfId="2463" xr:uid="{92BC106E-7EC7-46F0-8213-C86AC89535AA}"/>
+    <cellStyle name="Normal 26 49" xfId="2518" xr:uid="{FB05DC9E-5511-4750-B751-3C227EFC53E9}"/>
     <cellStyle name="Normal 26 5" xfId="713" xr:uid="{D344AFEE-A03D-4DA9-BD02-29F7ABE09946}"/>
+    <cellStyle name="Normal 26 50" xfId="2573" xr:uid="{B80F0946-702C-49C9-9827-5D854C2F8B97}"/>
+    <cellStyle name="Normal 26 51" xfId="2628" xr:uid="{7480B03D-F904-42F4-9091-2815BE7B1725}"/>
     <cellStyle name="Normal 26 6" xfId="740" xr:uid="{55099FE6-EF4A-4F80-A025-FC0681D4C856}"/>
     <cellStyle name="Normal 26 7" xfId="767" xr:uid="{E0D5D6CA-66CD-46E6-81F6-E5EF5A9B9699}"/>
     <cellStyle name="Normal 26 8" xfId="794" xr:uid="{8CA05745-9C12-4B23-8366-0110D6A2E67D}"/>
@@ -4673,7 +5053,11 @@
     <cellStyle name="Normal 27 44" xfId="2300" xr:uid="{7F64AC8D-D54B-4551-B7D6-FAC321FCFDE9}"/>
     <cellStyle name="Normal 27 45" xfId="2354" xr:uid="{35ED50A4-119A-42DB-8B12-F81EECFB6985}"/>
     <cellStyle name="Normal 27 46" xfId="2409" xr:uid="{921F6FEA-C33A-4779-920B-7DBA20603530}"/>
+    <cellStyle name="Normal 27 47" xfId="2464" xr:uid="{BAA97DA1-E79B-4330-A403-03BE03CA237F}"/>
+    <cellStyle name="Normal 27 48" xfId="2519" xr:uid="{EAD1FBA1-A307-48E7-B4E2-95E4AA85C4A5}"/>
+    <cellStyle name="Normal 27 49" xfId="2574" xr:uid="{E9404426-EF7E-45ED-B50A-733C111446F7}"/>
     <cellStyle name="Normal 27 5" xfId="741" xr:uid="{73F13B32-388D-4D89-9F01-E89AA863010F}"/>
+    <cellStyle name="Normal 27 50" xfId="2629" xr:uid="{B2D9E922-308D-4610-B916-15EA96B9CF94}"/>
     <cellStyle name="Normal 27 6" xfId="768" xr:uid="{C1FF1113-E4F1-409B-9342-01929F68ADCD}"/>
     <cellStyle name="Normal 27 7" xfId="795" xr:uid="{637C3645-B9B7-4559-9CFF-F3A6B8FF3C81}"/>
     <cellStyle name="Normal 27 8" xfId="822" xr:uid="{10EAD9CA-D6B3-4A76-91D8-4478130AB4E2}"/>
@@ -4719,7 +5103,11 @@
     <cellStyle name="Normal 28 44" xfId="2301" xr:uid="{5AB414CF-DD12-4AFC-A3F7-E4B94DEE0D7F}"/>
     <cellStyle name="Normal 28 45" xfId="2355" xr:uid="{54B74C83-6C34-4A7D-9AD3-9A1EA78BECC5}"/>
     <cellStyle name="Normal 28 46" xfId="2410" xr:uid="{F60F07C7-4DE0-49FD-9622-192482283209}"/>
+    <cellStyle name="Normal 28 47" xfId="2465" xr:uid="{8B01CB7F-83F7-4B73-92A4-8C5C573EE1B4}"/>
+    <cellStyle name="Normal 28 48" xfId="2520" xr:uid="{BC30CF03-7BD3-409B-BBAD-919DD741A619}"/>
+    <cellStyle name="Normal 28 49" xfId="2575" xr:uid="{ABCA9612-907D-403E-AA90-787CD7FB4435}"/>
     <cellStyle name="Normal 28 5" xfId="742" xr:uid="{0E873815-9144-409F-9560-E3292F714AD5}"/>
+    <cellStyle name="Normal 28 50" xfId="2630" xr:uid="{2FF253B9-A898-405E-83D6-E0778B761150}"/>
     <cellStyle name="Normal 28 6" xfId="769" xr:uid="{E1B9D957-F371-47A0-AEBA-EB4390991517}"/>
     <cellStyle name="Normal 28 7" xfId="796" xr:uid="{CE95D840-1DED-4550-9B45-79BB1A30B661}"/>
     <cellStyle name="Normal 28 8" xfId="823" xr:uid="{75DAFBA6-27A3-47FE-B0FD-AC8663496528}"/>
@@ -4756,7 +5144,11 @@
     <cellStyle name="Normal 29 36" xfId="2302" xr:uid="{1AD7A340-A7DB-4D71-9501-31DCAF062C83}"/>
     <cellStyle name="Normal 29 37" xfId="2356" xr:uid="{929283DC-4112-4FB7-BC9D-DF7DBF16E899}"/>
     <cellStyle name="Normal 29 38" xfId="2411" xr:uid="{32B4EF5D-097A-4490-AB57-B12BF3203489}"/>
+    <cellStyle name="Normal 29 39" xfId="2466" xr:uid="{1D21D564-CC51-419A-B080-A50C7B3326B4}"/>
     <cellStyle name="Normal 29 4" xfId="936" xr:uid="{B0ED404B-A0BC-4005-9C07-3ADBBFE5F173}"/>
+    <cellStyle name="Normal 29 40" xfId="2521" xr:uid="{7023392D-2709-4943-9C7A-0EA736D62434}"/>
+    <cellStyle name="Normal 29 41" xfId="2576" xr:uid="{07E3A54A-6A39-4486-A4EC-C2F0E5CF5933}"/>
+    <cellStyle name="Normal 29 42" xfId="2631" xr:uid="{663ACD19-5261-423E-A199-12144B535E20}"/>
     <cellStyle name="Normal 29 5" xfId="965" xr:uid="{E4F2ED17-F04A-4AF1-A706-C14A73357E91}"/>
     <cellStyle name="Normal 29 6" xfId="994" xr:uid="{CAF38D46-8974-47D6-914C-330FB88EC9BB}"/>
     <cellStyle name="Normal 29 7" xfId="1024" xr:uid="{89E0CC64-087C-41A9-B0ED-A634EDD2A24E}"/>
@@ -4854,6 +5246,10 @@
     <cellStyle name="Normal 3 90" xfId="2276" xr:uid="{05D0FD9A-2C4D-4E67-B715-F48881962247}"/>
     <cellStyle name="Normal 3 91" xfId="2330" xr:uid="{7C9CB010-F1E7-4EFD-804C-07FFFC147F7B}"/>
     <cellStyle name="Normal 3 92" xfId="2385" xr:uid="{C802E603-F79D-484A-8796-D10DCC293D44}"/>
+    <cellStyle name="Normal 3 93" xfId="2440" xr:uid="{B0FFF112-1AF3-4B0D-B56D-FD26D3F8C6D8}"/>
+    <cellStyle name="Normal 3 94" xfId="2495" xr:uid="{861C0826-6EB8-4CDD-9449-B83DC31A913A}"/>
+    <cellStyle name="Normal 3 95" xfId="2550" xr:uid="{58AA66E0-C1C7-4D30-B1E6-BF3992BDC85F}"/>
+    <cellStyle name="Normal 3 96" xfId="2605" xr:uid="{528AA4E6-A7FF-48A6-9B0F-75BD4AA62468}"/>
     <cellStyle name="Normal 30" xfId="908" xr:uid="{29060677-DDC7-44E4-9DB7-833832E2C2EF}"/>
     <cellStyle name="Normal 30 10" xfId="1194" xr:uid="{87CB8D63-90E2-489B-B2F1-CACD93DC026A}"/>
     <cellStyle name="Normal 30 11" xfId="1233" xr:uid="{BE9D1AC2-FA84-447C-980B-7C0F52813116}"/>
@@ -4884,7 +5280,11 @@
     <cellStyle name="Normal 30 34" xfId="2303" xr:uid="{600E12BF-5A9C-4BD3-A3CA-2ABA40241DF6}"/>
     <cellStyle name="Normal 30 35" xfId="2357" xr:uid="{ABD7D2C6-C14A-4E7C-98E4-7A6F126BC750}"/>
     <cellStyle name="Normal 30 36" xfId="2412" xr:uid="{C360F1EF-5219-46D6-9B03-DCDF440403A4}"/>
+    <cellStyle name="Normal 30 37" xfId="2467" xr:uid="{89CFF7FF-250D-4470-BF7E-A7920F61B839}"/>
+    <cellStyle name="Normal 30 38" xfId="2522" xr:uid="{9F615AC8-21F0-4281-B048-6B7A426F6F4B}"/>
+    <cellStyle name="Normal 30 39" xfId="2577" xr:uid="{840D2EFC-978A-4345-92A2-B6E33B690D9A}"/>
     <cellStyle name="Normal 30 4" xfId="995" xr:uid="{8A471471-CC73-4677-8055-BF9B78704B15}"/>
+    <cellStyle name="Normal 30 40" xfId="2632" xr:uid="{C6040655-0458-4CAF-B497-74DC85D9610D}"/>
     <cellStyle name="Normal 30 5" xfId="1025" xr:uid="{8A88A566-55ED-4197-B3EC-34A2D6F4693C}"/>
     <cellStyle name="Normal 30 6" xfId="1056" xr:uid="{C7E13848-0B37-42F9-92EF-9D5A7F8289AC}"/>
     <cellStyle name="Normal 30 7" xfId="1088" xr:uid="{A17CA1F5-FE5F-4F1B-89F7-FE42660C5DC5}"/>
@@ -4917,6 +5317,10 @@
     <cellStyle name="Normal 31 31" xfId="2304" xr:uid="{6902C0B4-6563-4408-9608-C6349C3F6E17}"/>
     <cellStyle name="Normal 31 32" xfId="2358" xr:uid="{EF15EB66-4386-4230-A612-ED933C7471FB}"/>
     <cellStyle name="Normal 31 33" xfId="2413" xr:uid="{89E2EA3F-47F5-47C0-A540-133C298E781A}"/>
+    <cellStyle name="Normal 31 34" xfId="2468" xr:uid="{81DE2275-2884-4358-A818-FCDDB90599A7}"/>
+    <cellStyle name="Normal 31 35" xfId="2523" xr:uid="{41E38385-1124-44A7-8B1C-4EA87E2C2B69}"/>
+    <cellStyle name="Normal 31 36" xfId="2578" xr:uid="{1BE42E08-24D8-41AD-A0A9-C39492ADD2DB}"/>
+    <cellStyle name="Normal 31 37" xfId="2633" xr:uid="{B637D5AB-C4A9-4219-96D5-3677ECA6B10C}"/>
     <cellStyle name="Normal 31 4" xfId="1089" xr:uid="{115B4DBC-0A4B-43C2-8D38-B8E1346CA496}"/>
     <cellStyle name="Normal 31 5" xfId="1123" xr:uid="{17785C55-2ED2-45EA-9422-1590CD144DCC}"/>
     <cellStyle name="Normal 31 6" xfId="1158" xr:uid="{5257BC80-708E-436F-B0A2-DE856F2C5DBA}"/>
@@ -4949,6 +5353,10 @@
     <cellStyle name="Normal 32 30" xfId="2305" xr:uid="{F9553DB4-A148-47E3-9FF7-0F065C20ED3F}"/>
     <cellStyle name="Normal 32 31" xfId="2359" xr:uid="{3E9B7C91-4175-4E1E-A314-4613B40E6C7A}"/>
     <cellStyle name="Normal 32 32" xfId="2414" xr:uid="{EEB684C7-4033-4182-BB34-C200845CF3B8}"/>
+    <cellStyle name="Normal 32 33" xfId="2469" xr:uid="{2767A65C-83DD-4F8D-A987-C61869B50B84}"/>
+    <cellStyle name="Normal 32 34" xfId="2524" xr:uid="{47A48D37-3155-4508-BC2A-2C06457875E7}"/>
+    <cellStyle name="Normal 32 35" xfId="2579" xr:uid="{2AA15E46-370C-43A3-8935-26F782454E98}"/>
+    <cellStyle name="Normal 32 36" xfId="2634" xr:uid="{80852F55-B1DC-4B2A-9E96-56F6F94B8D47}"/>
     <cellStyle name="Normal 32 4" xfId="1124" xr:uid="{02CC8B8D-088C-499C-99A0-F631BCDD8473}"/>
     <cellStyle name="Normal 32 5" xfId="1159" xr:uid="{D2F78B05-994A-4DB4-A496-D9328EBBE67B}"/>
     <cellStyle name="Normal 32 6" xfId="1196" xr:uid="{2DCB929C-297C-4C53-82E4-0403B87AF2B1}"/>
@@ -4980,6 +5388,10 @@
     <cellStyle name="Normal 33 3" xfId="1125" xr:uid="{DA4B6EED-C769-4BE0-BA7E-E741A1CD3FB3}"/>
     <cellStyle name="Normal 33 30" xfId="2360" xr:uid="{6ECE6C43-8104-47B9-B117-B38271699D3A}"/>
     <cellStyle name="Normal 33 31" xfId="2415" xr:uid="{52E82BF7-BDDE-4D85-BE3E-EF35E155C12A}"/>
+    <cellStyle name="Normal 33 32" xfId="2470" xr:uid="{D586BBFB-A480-45FD-A1C9-A2745532A6AA}"/>
+    <cellStyle name="Normal 33 33" xfId="2525" xr:uid="{2FDCE2FA-E5C2-443C-ACB6-88B99FCD9A18}"/>
+    <cellStyle name="Normal 33 34" xfId="2580" xr:uid="{5B5E38BD-E6E2-42A6-8E04-7225903D5289}"/>
+    <cellStyle name="Normal 33 35" xfId="2635" xr:uid="{47DF46BC-9148-4BE0-AAB3-BA6F6681CBAD}"/>
     <cellStyle name="Normal 33 4" xfId="1160" xr:uid="{740C5F2E-4830-4E49-BDD6-9A5138A262C0}"/>
     <cellStyle name="Normal 33 5" xfId="1197" xr:uid="{63D7510F-076E-4560-907D-87441A3EC81D}"/>
     <cellStyle name="Normal 33 6" xfId="1236" xr:uid="{32588593-4A0B-46F3-8C61-023846E9132B}"/>
@@ -5010,6 +5422,10 @@
     <cellStyle name="Normal 34 29" xfId="2361" xr:uid="{63FDA86C-8D93-4610-8F20-F59CA8ED1F80}"/>
     <cellStyle name="Normal 34 3" xfId="1161" xr:uid="{984471BB-698B-4FEC-BE51-290CAAFB126E}"/>
     <cellStyle name="Normal 34 30" xfId="2416" xr:uid="{83F2861E-D22C-423E-BDA5-D7F16A77409B}"/>
+    <cellStyle name="Normal 34 31" xfId="2471" xr:uid="{E4A81BBC-4B18-49A7-864E-5B25E19326FF}"/>
+    <cellStyle name="Normal 34 32" xfId="2526" xr:uid="{10A2FDA6-BFA6-4CFA-98B4-0A840EBB2E5A}"/>
+    <cellStyle name="Normal 34 33" xfId="2581" xr:uid="{DD105E7E-441F-41E9-9408-B1E3C8521CD6}"/>
+    <cellStyle name="Normal 34 34" xfId="2636" xr:uid="{DE36D422-D4D8-4B3B-B886-4669F4CC72DB}"/>
     <cellStyle name="Normal 34 4" xfId="1198" xr:uid="{8F856BAA-2847-43FC-BEA2-D1DAFE5D5C08}"/>
     <cellStyle name="Normal 34 5" xfId="1237" xr:uid="{E8D324D6-0564-42C7-A347-F071F77AD38C}"/>
     <cellStyle name="Normal 34 6" xfId="1277" xr:uid="{78E23A18-BA39-450B-AF6F-829AB866D556}"/>
@@ -5040,6 +5456,10 @@
     <cellStyle name="Normal 35 29" xfId="2362" xr:uid="{DE8E2D4B-D2A4-411E-BD33-E75637BE13A2}"/>
     <cellStyle name="Normal 35 3" xfId="1162" xr:uid="{F711045E-FBAB-49E2-B85B-DD7F67FA2A9E}"/>
     <cellStyle name="Normal 35 30" xfId="2417" xr:uid="{B3F07313-675D-4BCB-973A-BF2F37E61096}"/>
+    <cellStyle name="Normal 35 31" xfId="2472" xr:uid="{5A83D64C-346F-4232-B563-1725D572D426}"/>
+    <cellStyle name="Normal 35 32" xfId="2527" xr:uid="{E343B2F7-1F4F-41C7-BEA5-0687D0F8567E}"/>
+    <cellStyle name="Normal 35 33" xfId="2582" xr:uid="{E3472DD8-BF44-4FAA-8F23-B0B259F2C546}"/>
+    <cellStyle name="Normal 35 34" xfId="2637" xr:uid="{7375C592-CDC4-4E6E-9BDC-07152104C8FF}"/>
     <cellStyle name="Normal 35 4" xfId="1199" xr:uid="{5C6D934C-C084-456A-8378-EFEE061775E5}"/>
     <cellStyle name="Normal 35 5" xfId="1238" xr:uid="{7CB240F7-BDE4-4E7B-8875-63F971329466}"/>
     <cellStyle name="Normal 35 6" xfId="1278" xr:uid="{EF4981D6-3F62-4CEE-AFBB-7FAF9F704E25}"/>
@@ -5069,6 +5489,10 @@
     <cellStyle name="Normal 36 28" xfId="2363" xr:uid="{6DB1304B-0741-4634-B52A-8E8FA8039D4D}"/>
     <cellStyle name="Normal 36 29" xfId="2418" xr:uid="{887E7B0C-BF23-4A33-9D41-9A226E958518}"/>
     <cellStyle name="Normal 36 3" xfId="1200" xr:uid="{9B7CD598-05AB-40C9-BCD9-3B8266389254}"/>
+    <cellStyle name="Normal 36 30" xfId="2473" xr:uid="{5581A8CE-0FA9-48A6-9D7B-0D2FBCB5A52D}"/>
+    <cellStyle name="Normal 36 31" xfId="2528" xr:uid="{A51D5C9B-C51F-45C7-8CB3-D186C51F1862}"/>
+    <cellStyle name="Normal 36 32" xfId="2583" xr:uid="{903B5BA5-7C47-4979-983F-76E943151007}"/>
+    <cellStyle name="Normal 36 33" xfId="2638" xr:uid="{DBE0A2AF-3F5E-4F68-AFC0-38D10F8A4990}"/>
     <cellStyle name="Normal 36 4" xfId="1239" xr:uid="{D6071E2A-50A2-4D3C-9968-A1E3E4687B7E}"/>
     <cellStyle name="Normal 36 5" xfId="1279" xr:uid="{F643CB92-74BB-4F63-99A2-B010269425DF}"/>
     <cellStyle name="Normal 36 6" xfId="1320" xr:uid="{A54925E5-DBB1-4E4A-A7E8-D13C59949278}"/>
@@ -5096,7 +5520,11 @@
     <cellStyle name="Normal 37 26" xfId="2310" xr:uid="{59B96874-225F-4A03-9E0C-EFAACEEC5D08}"/>
     <cellStyle name="Normal 37 27" xfId="2364" xr:uid="{7A30CF3A-89E3-4C39-AAD9-B68114DD075A}"/>
     <cellStyle name="Normal 37 28" xfId="2419" xr:uid="{07723123-A61A-46E6-BC00-65C8A8ACEB92}"/>
+    <cellStyle name="Normal 37 29" xfId="2474" xr:uid="{82EFCB37-1074-4245-8247-7B1B31BE4723}"/>
     <cellStyle name="Normal 37 3" xfId="1240" xr:uid="{542FBE86-F5EE-4D1E-9F91-6EA7599E5748}"/>
+    <cellStyle name="Normal 37 30" xfId="2529" xr:uid="{3A652BB0-A70B-4BBD-B6BF-4DF249A443EA}"/>
+    <cellStyle name="Normal 37 31" xfId="2584" xr:uid="{AA99344E-F1BB-406C-9284-8EC5BD558673}"/>
+    <cellStyle name="Normal 37 32" xfId="2639" xr:uid="{DE962FA6-FAD7-498A-B3C7-F593975FD3F4}"/>
     <cellStyle name="Normal 37 4" xfId="1280" xr:uid="{BB9F55A5-BDD5-4597-90A0-CF5B0C044934}"/>
     <cellStyle name="Normal 37 5" xfId="1321" xr:uid="{C233C0E3-A15F-40DD-88CA-205C74255FCE}"/>
     <cellStyle name="Normal 37 6" xfId="1363" xr:uid="{BF242644-0A31-474B-BA33-9B0FA600A6E1}"/>
@@ -5124,7 +5552,11 @@
     <cellStyle name="Normal 38 26" xfId="2311" xr:uid="{95E19800-C30A-4E51-BD76-3CA390AB5639}"/>
     <cellStyle name="Normal 38 27" xfId="2365" xr:uid="{99C63C58-EF56-40CD-9558-2D7CD30F36F6}"/>
     <cellStyle name="Normal 38 28" xfId="2420" xr:uid="{E3DDAD81-A0CC-41AA-813D-A7190C58D172}"/>
+    <cellStyle name="Normal 38 29" xfId="2475" xr:uid="{1B55301E-5256-4E2A-A611-1179C880BD1A}"/>
     <cellStyle name="Normal 38 3" xfId="1241" xr:uid="{5AB936AE-86CC-45A3-8DE0-331F0E36DDBD}"/>
+    <cellStyle name="Normal 38 30" xfId="2530" xr:uid="{07BFE165-0C73-4794-ABD6-61BFC651DF7E}"/>
+    <cellStyle name="Normal 38 31" xfId="2585" xr:uid="{3B7B97CB-CF69-4248-BA93-3793AF85C633}"/>
+    <cellStyle name="Normal 38 32" xfId="2640" xr:uid="{32043AFA-59BD-4271-AA46-0306589BA734}"/>
     <cellStyle name="Normal 38 4" xfId="1281" xr:uid="{06B9E8CD-8E13-44D7-B4A2-3CCA5CF70BFC}"/>
     <cellStyle name="Normal 38 5" xfId="1322" xr:uid="{64D206D8-A195-42CA-8AFF-84B3F657D678}"/>
     <cellStyle name="Normal 38 6" xfId="1364" xr:uid="{A37FD0CC-7CC6-439F-9126-06B26282AAA9}"/>
@@ -5151,7 +5583,11 @@
     <cellStyle name="Normal 39 25" xfId="2312" xr:uid="{E14F26CF-CD5D-4C43-99F3-8F92071A3966}"/>
     <cellStyle name="Normal 39 26" xfId="2366" xr:uid="{C94ED76E-DF7F-4450-80CF-D75B2CAAB926}"/>
     <cellStyle name="Normal 39 27" xfId="2421" xr:uid="{18F96B56-B490-4659-B0CE-42068A35FBEB}"/>
+    <cellStyle name="Normal 39 28" xfId="2476" xr:uid="{8C6700AC-DC82-47EF-A258-CA4FC53961C5}"/>
+    <cellStyle name="Normal 39 29" xfId="2531" xr:uid="{B17CF32D-DD02-4487-ABD2-5D8B3010A288}"/>
     <cellStyle name="Normal 39 3" xfId="1282" xr:uid="{0296B16D-DA08-43E9-9663-8A88969E79F4}"/>
+    <cellStyle name="Normal 39 30" xfId="2586" xr:uid="{6DFF16CF-67E4-4DD5-8603-E0CA064031AE}"/>
+    <cellStyle name="Normal 39 31" xfId="2641" xr:uid="{A9F2DB4C-9778-49B9-B98D-A3F7D714FA5F}"/>
     <cellStyle name="Normal 39 4" xfId="1323" xr:uid="{15831E53-2DBD-4A2E-B270-23C619CA089E}"/>
     <cellStyle name="Normal 39 5" xfId="1365" xr:uid="{F009ABEF-0BCE-4955-ADC3-3578DB39F7F8}"/>
     <cellStyle name="Normal 39 6" xfId="1407" xr:uid="{726EFD29-EDCE-49BC-825A-A138625D51CD}"/>
@@ -5250,6 +5686,10 @@
     <cellStyle name="Normal 4 90" xfId="2277" xr:uid="{237462F5-BB1D-4C48-9ADF-BE20CF931E26}"/>
     <cellStyle name="Normal 4 91" xfId="2331" xr:uid="{A0EB0CBE-1F94-41C7-98FF-4DAECF115BCB}"/>
     <cellStyle name="Normal 4 92" xfId="2386" xr:uid="{949304E3-ABC1-4BC5-8027-03D8E13BC5CC}"/>
+    <cellStyle name="Normal 4 93" xfId="2441" xr:uid="{12EE009D-6CA8-4F80-9149-5A4F26AB3C24}"/>
+    <cellStyle name="Normal 4 94" xfId="2496" xr:uid="{7AEC0261-4350-465C-8F83-41FF9454D6DE}"/>
+    <cellStyle name="Normal 4 95" xfId="2551" xr:uid="{0521DAAF-579E-4EB5-A892-1824F512F272}"/>
+    <cellStyle name="Normal 4 96" xfId="2606" xr:uid="{81B8554B-195D-41A4-B1CE-733020EA6D7B}"/>
     <cellStyle name="Normal 40" xfId="1204" xr:uid="{9A758E20-7263-44F0-A0A0-3D5D1FE88C83}"/>
     <cellStyle name="Normal 40 10" xfId="1584" xr:uid="{00514BDB-1937-4C34-97E1-6B15E53A4098}"/>
     <cellStyle name="Normal 40 11" xfId="1628" xr:uid="{858AF8D4-5153-4B46-93B1-00B25FF415FB}"/>
@@ -5270,7 +5710,11 @@
     <cellStyle name="Normal 40 25" xfId="2313" xr:uid="{3DD46A9E-26FC-4271-A30C-E459C4EE092F}"/>
     <cellStyle name="Normal 40 26" xfId="2367" xr:uid="{C08016E3-3D86-4965-BA30-A2E3134EB706}"/>
     <cellStyle name="Normal 40 27" xfId="2422" xr:uid="{D2E03D60-114F-4864-906A-098716246FD2}"/>
+    <cellStyle name="Normal 40 28" xfId="2477" xr:uid="{13993A5A-43A2-46E7-B17B-63108268C96E}"/>
+    <cellStyle name="Normal 40 29" xfId="2532" xr:uid="{6D3E85BC-39B3-4144-89E0-062D8331A1AA}"/>
     <cellStyle name="Normal 40 3" xfId="1283" xr:uid="{60DC833A-F031-4DBD-BC0B-B48ABCDE6533}"/>
+    <cellStyle name="Normal 40 30" xfId="2587" xr:uid="{0E60E04E-AB8C-41D1-975C-2E5D4DAA9195}"/>
+    <cellStyle name="Normal 40 31" xfId="2642" xr:uid="{E5EBFCBF-3FAB-4093-872F-65B412F95D30}"/>
     <cellStyle name="Normal 40 4" xfId="1324" xr:uid="{BC132578-6363-4D48-BB11-F90899981771}"/>
     <cellStyle name="Normal 40 5" xfId="1366" xr:uid="{CCB407F9-2940-4586-A2FB-F175B848303E}"/>
     <cellStyle name="Normal 40 6" xfId="1408" xr:uid="{7548B4F1-5CC1-4EA1-9223-B76BCC53A8BD}"/>
@@ -5296,7 +5740,11 @@
     <cellStyle name="Normal 41 24" xfId="2314" xr:uid="{97A31EC4-2451-42D8-8741-C4AFA548353B}"/>
     <cellStyle name="Normal 41 25" xfId="2368" xr:uid="{768D9F1F-9C6B-4DB2-9288-AA0451754DDA}"/>
     <cellStyle name="Normal 41 26" xfId="2423" xr:uid="{238D28F3-8E81-4BDA-8132-6766EDEBA318}"/>
+    <cellStyle name="Normal 41 27" xfId="2478" xr:uid="{42382D01-82FF-4CA8-9AC0-561A26852C32}"/>
+    <cellStyle name="Normal 41 28" xfId="2533" xr:uid="{BB4D77D5-C30C-4245-88E6-E30A10B7B997}"/>
+    <cellStyle name="Normal 41 29" xfId="2588" xr:uid="{9EC65DA9-F820-4E50-AA99-FF308522A26D}"/>
     <cellStyle name="Normal 41 3" xfId="1325" xr:uid="{DB7266FD-DB20-4504-9181-FDAD4A49F920}"/>
+    <cellStyle name="Normal 41 30" xfId="2643" xr:uid="{5A70FD02-EF28-4CB5-B20D-AF73372F3BCE}"/>
     <cellStyle name="Normal 41 4" xfId="1367" xr:uid="{7EE95D5B-6BEF-49DA-8567-DB37D49C5ABE}"/>
     <cellStyle name="Normal 41 5" xfId="1409" xr:uid="{626DD975-DD53-4D9F-B777-AA700296E57B}"/>
     <cellStyle name="Normal 41 6" xfId="1452" xr:uid="{6CE0B273-A5D0-46F8-A408-8A59B910B884}"/>
@@ -5321,6 +5769,10 @@
     <cellStyle name="Normal 42 23" xfId="2315" xr:uid="{6E1BFCE1-6EDE-4667-A457-C497464AB3F7}"/>
     <cellStyle name="Normal 42 24" xfId="2369" xr:uid="{6D857CC0-A0CC-476A-8A6D-4C179688E51A}"/>
     <cellStyle name="Normal 42 25" xfId="2424" xr:uid="{EC43C3B1-DD6D-4CAF-A170-627B81DF52D9}"/>
+    <cellStyle name="Normal 42 26" xfId="2479" xr:uid="{01B97FB4-4207-49CE-B533-E396A67985E6}"/>
+    <cellStyle name="Normal 42 27" xfId="2534" xr:uid="{45078A23-7538-415A-8CDA-E1FE86CFBCFF}"/>
+    <cellStyle name="Normal 42 28" xfId="2589" xr:uid="{807D0CC8-9AB4-4E1F-829A-BA8CE8E1A61B}"/>
+    <cellStyle name="Normal 42 29" xfId="2644" xr:uid="{82416638-6DDE-4130-B174-F4443FA4C084}"/>
     <cellStyle name="Normal 42 3" xfId="1368" xr:uid="{027F54D2-79FB-429D-8AF6-DC22C57389A3}"/>
     <cellStyle name="Normal 42 4" xfId="1410" xr:uid="{04BC6829-1A0D-4655-BB18-979D575FAF18}"/>
     <cellStyle name="Normal 42 5" xfId="1453" xr:uid="{A41DFB52-1E5B-461C-8EE4-AB2538BAB5D4}"/>
@@ -5345,6 +5797,10 @@
     <cellStyle name="Normal 43 22" xfId="2316" xr:uid="{E6CC6AF2-7ACA-49DA-AA08-6B90ADEDDF35}"/>
     <cellStyle name="Normal 43 23" xfId="2370" xr:uid="{B0DFF26F-5534-4297-84F4-FCDC90C89B7B}"/>
     <cellStyle name="Normal 43 24" xfId="2425" xr:uid="{11D196AE-99A0-48B6-AA2A-79A01C2D72B5}"/>
+    <cellStyle name="Normal 43 25" xfId="2480" xr:uid="{5BE1AF82-6C8A-4031-9433-32649BA35018}"/>
+    <cellStyle name="Normal 43 26" xfId="2535" xr:uid="{13849D65-AA3D-421C-9F10-23D08DCD8FE9}"/>
+    <cellStyle name="Normal 43 27" xfId="2590" xr:uid="{BFB8FA52-F487-40E1-8D18-17137293FCBC}"/>
+    <cellStyle name="Normal 43 28" xfId="2645" xr:uid="{86B6D99C-6592-46CC-BA91-E3DC06CFC223}"/>
     <cellStyle name="Normal 43 3" xfId="1411" xr:uid="{E9013BFE-34CD-4396-9801-740BE57E4C74}"/>
     <cellStyle name="Normal 43 4" xfId="1454" xr:uid="{8B718497-4D05-4283-B46C-590C40CCD3B5}"/>
     <cellStyle name="Normal 43 5" xfId="1498" xr:uid="{8E7273E6-D96E-4807-9FA4-FD3FAA93ABEC}"/>
@@ -5367,6 +5823,10 @@
     <cellStyle name="Normal 44 20" xfId="2317" xr:uid="{37A14A11-41D7-4793-9EB1-375B7C7BC519}"/>
     <cellStyle name="Normal 44 21" xfId="2371" xr:uid="{39BEE483-4692-476C-9313-D62EA4633326}"/>
     <cellStyle name="Normal 44 22" xfId="2426" xr:uid="{3BA62BB1-792D-45F3-8659-AF5C7965BF92}"/>
+    <cellStyle name="Normal 44 23" xfId="2481" xr:uid="{5979DBC0-65FE-4382-AA2B-9CA548DC88C9}"/>
+    <cellStyle name="Normal 44 24" xfId="2536" xr:uid="{BA975EB6-7634-44DC-B476-BFAAA0821F6E}"/>
+    <cellStyle name="Normal 44 25" xfId="2591" xr:uid="{1F7DE00D-A6C1-4A9E-8BFB-7AA0C5B7FCF8}"/>
+    <cellStyle name="Normal 44 26" xfId="2646" xr:uid="{9726AF58-BCBA-4D0A-A55F-A2E5B65F6CC9}"/>
     <cellStyle name="Normal 44 3" xfId="1499" xr:uid="{19841630-1868-4129-AF65-9439A8362635}"/>
     <cellStyle name="Normal 44 4" xfId="1543" xr:uid="{B24CAFA4-F870-42C6-835A-841530B7459E}"/>
     <cellStyle name="Normal 44 5" xfId="1588" xr:uid="{F3149A38-5BF0-4CF4-92A1-CEBFBCA9E57B}"/>
@@ -5388,6 +5848,10 @@
     <cellStyle name="Normal 45 2" xfId="1500" xr:uid="{5027BECF-87E9-4D4B-9BEF-85E1909AE39A}"/>
     <cellStyle name="Normal 45 20" xfId="2372" xr:uid="{0E3AA70B-706E-422D-BA4C-6FFD45EF939A}"/>
     <cellStyle name="Normal 45 21" xfId="2427" xr:uid="{6B8EEB3E-EF73-45B8-A5A6-B1DEF269080F}"/>
+    <cellStyle name="Normal 45 22" xfId="2482" xr:uid="{860D4BE7-897A-468C-87DC-248651837E59}"/>
+    <cellStyle name="Normal 45 23" xfId="2537" xr:uid="{BFE2DAAA-B94B-40B0-94ED-BA82B45EF879}"/>
+    <cellStyle name="Normal 45 24" xfId="2592" xr:uid="{B776F09F-482E-4A29-9779-68E1BC542E91}"/>
+    <cellStyle name="Normal 45 25" xfId="2647" xr:uid="{76C85D64-BEC3-40E2-AF82-B27533CF7EAC}"/>
     <cellStyle name="Normal 45 3" xfId="1544" xr:uid="{1787A129-1435-4B42-BEEC-006984305340}"/>
     <cellStyle name="Normal 45 4" xfId="1589" xr:uid="{D8955FBC-9811-4F2B-8AA5-1BB672F751BC}"/>
     <cellStyle name="Normal 45 5" xfId="1633" xr:uid="{282C9639-360C-473E-852D-2521B8E40B05}"/>
@@ -5402,6 +5866,10 @@
     <cellStyle name="Normal 46 13" xfId="2319" xr:uid="{38549543-DF9E-40D8-AE60-3A34235A86E0}"/>
     <cellStyle name="Normal 46 14" xfId="2373" xr:uid="{7A6B0829-52CF-4AAA-B0A9-41465DAF1112}"/>
     <cellStyle name="Normal 46 15" xfId="2428" xr:uid="{6298130A-51EC-40A6-98EF-E2DD1DB3D487}"/>
+    <cellStyle name="Normal 46 16" xfId="2483" xr:uid="{C9F6E7BD-ED39-488F-9C54-0B2DB6914C21}"/>
+    <cellStyle name="Normal 46 17" xfId="2538" xr:uid="{7CF823EA-B6B4-4A3E-9A3B-722927714719}"/>
+    <cellStyle name="Normal 46 18" xfId="2593" xr:uid="{66F26B5C-8E69-47D1-8428-45F31C6B4FC8}"/>
+    <cellStyle name="Normal 46 19" xfId="2648" xr:uid="{0CCF7C06-7E7F-4698-904D-6FB64062790F}"/>
     <cellStyle name="Normal 46 2" xfId="1722" xr:uid="{A92ECEED-86A5-4AF8-A45B-3F5122E4A57C}"/>
     <cellStyle name="Normal 46 3" xfId="1812" xr:uid="{9B7FD6F8-A2AE-4D9F-97CA-07164D6BFAED}"/>
     <cellStyle name="Normal 46 4" xfId="1858" xr:uid="{5099E28A-8E05-4821-9D0F-B6E84C8944BB}"/>
@@ -5416,6 +5884,10 @@
     <cellStyle name="Normal 47 12" xfId="2320" xr:uid="{22719D81-FE51-4E4D-9A75-CA6E683278BA}"/>
     <cellStyle name="Normal 47 13" xfId="2374" xr:uid="{3F8FE100-EE70-4751-A9C3-33DCE7F70579}"/>
     <cellStyle name="Normal 47 14" xfId="2429" xr:uid="{F18DB719-115E-4829-B5B1-308C2A730787}"/>
+    <cellStyle name="Normal 47 15" xfId="2484" xr:uid="{DEAB1C60-789D-4F03-B260-5407188BFBA4}"/>
+    <cellStyle name="Normal 47 16" xfId="2539" xr:uid="{2FC79E6F-B9D4-48AD-B16C-3C3B6B31B74D}"/>
+    <cellStyle name="Normal 47 17" xfId="2594" xr:uid="{0AEE451B-3F60-47D7-8640-887E17B22603}"/>
+    <cellStyle name="Normal 47 18" xfId="2649" xr:uid="{EA7667C7-C1DD-40B6-A318-2C0C47212009}"/>
     <cellStyle name="Normal 47 2" xfId="1813" xr:uid="{C2210DC9-C26B-4BF3-AF35-FBEBA6756BF6}"/>
     <cellStyle name="Normal 47 3" xfId="1859" xr:uid="{68779769-7635-477C-A18C-EF4DCCAC4899}"/>
     <cellStyle name="Normal 47 4" xfId="1906" xr:uid="{2F6200A8-6C6E-4A93-87BA-36E965276181}"/>
@@ -5428,6 +5900,10 @@
     <cellStyle name="Normal 48 10" xfId="2321" xr:uid="{6B69415D-73A4-4BFC-AC96-9262FC2857E0}"/>
     <cellStyle name="Normal 48 11" xfId="2375" xr:uid="{285896D6-321F-4B7F-9545-76A6FB4A4CB1}"/>
     <cellStyle name="Normal 48 12" xfId="2430" xr:uid="{1E16A4FB-6A23-42C5-92DD-9358F7CD93D9}"/>
+    <cellStyle name="Normal 48 13" xfId="2485" xr:uid="{849983C2-3C20-4EB3-8E97-09F0E0B29156}"/>
+    <cellStyle name="Normal 48 14" xfId="2540" xr:uid="{502A937D-F975-404A-AFA2-D58C2AB2303E}"/>
+    <cellStyle name="Normal 48 15" xfId="2595" xr:uid="{4623B74F-9F0C-4AAA-B3F1-BAE059E5B8A9}"/>
+    <cellStyle name="Normal 48 16" xfId="2650" xr:uid="{D0006705-DECE-4952-A764-E6ADDE980A8D}"/>
     <cellStyle name="Normal 48 2" xfId="1907" xr:uid="{CB91C6DC-62B0-4992-A8A4-FEC63EC908A5}"/>
     <cellStyle name="Normal 48 3" xfId="1955" xr:uid="{9140C7D6-0A03-4AEF-AB80-301C7410CF0E}"/>
     <cellStyle name="Normal 48 4" xfId="2004" xr:uid="{4958E27D-47B3-4CE5-9C94-AA09930271BA}"/>
@@ -5439,6 +5915,10 @@
     <cellStyle name="Normal 49" xfId="1908" xr:uid="{181FE46B-5ADF-443B-A5AF-43C8E8CE7316}"/>
     <cellStyle name="Normal 49 10" xfId="2376" xr:uid="{619ACDF0-205F-48D6-B6CC-1EDBCCC8946B}"/>
     <cellStyle name="Normal 49 11" xfId="2431" xr:uid="{3A259915-4B6F-47C2-9EBC-4246A0DD5807}"/>
+    <cellStyle name="Normal 49 12" xfId="2486" xr:uid="{0728544E-ED0E-4C9A-B015-BB833103C74B}"/>
+    <cellStyle name="Normal 49 13" xfId="2541" xr:uid="{02F45A4E-86FD-4BB1-BEC6-FEE9F7C27D78}"/>
+    <cellStyle name="Normal 49 14" xfId="2596" xr:uid="{AD88EABD-127C-45C5-AB5B-FCFF698F0AAF}"/>
+    <cellStyle name="Normal 49 15" xfId="2651" xr:uid="{9D6D2683-4B16-4C7E-AA58-5678DAC277C2}"/>
     <cellStyle name="Normal 49 2" xfId="1956" xr:uid="{AB9E1C32-A524-46A2-A8BF-A94BB89130A2}"/>
     <cellStyle name="Normal 49 3" xfId="2005" xr:uid="{049F4BEA-0C06-4129-947B-575F3F21ED78}"/>
     <cellStyle name="Normal 49 4" xfId="2055" xr:uid="{17958B43-E79B-4901-9FE3-F7F09DD6273F}"/>
@@ -5539,8 +6019,16 @@
     <cellStyle name="Normal 5 90" xfId="2278" xr:uid="{923232B3-278A-4CAB-9FB5-60044FAE477E}"/>
     <cellStyle name="Normal 5 91" xfId="2332" xr:uid="{74847720-2D89-4817-8202-5A3D4B1520D1}"/>
     <cellStyle name="Normal 5 92" xfId="2387" xr:uid="{1FD4D425-4F5A-4A82-9330-53EC3285CDFB}"/>
+    <cellStyle name="Normal 5 93" xfId="2442" xr:uid="{48FB4E41-B435-4BFF-B994-6A0EB00130EE}"/>
+    <cellStyle name="Normal 5 94" xfId="2497" xr:uid="{BAA3D145-A84A-4E03-94FC-05B9F720FD9A}"/>
+    <cellStyle name="Normal 5 95" xfId="2552" xr:uid="{4FE77182-375F-4D42-A41A-846285BFB9D6}"/>
+    <cellStyle name="Normal 5 96" xfId="2607" xr:uid="{6F37AC54-F363-49A4-B837-9005DB98231B}"/>
     <cellStyle name="Normal 50" xfId="1957" xr:uid="{F694FC52-4B0F-47E1-92DF-CD4D0A8F23AF}"/>
     <cellStyle name="Normal 50 10" xfId="2432" xr:uid="{2354729D-8ABA-4246-92CA-A3C324BC2D2A}"/>
+    <cellStyle name="Normal 50 11" xfId="2487" xr:uid="{138B7319-971A-4BFF-B9A2-4FB00311A37F}"/>
+    <cellStyle name="Normal 50 12" xfId="2542" xr:uid="{673A2782-1DD1-4B34-AA50-A418268828F0}"/>
+    <cellStyle name="Normal 50 13" xfId="2597" xr:uid="{52EB8DB8-D289-4C7F-A347-25BFF8F032C9}"/>
+    <cellStyle name="Normal 50 14" xfId="2652" xr:uid="{5B1EBE0D-4CBF-453E-B54A-8B3C3A213A70}"/>
     <cellStyle name="Normal 50 2" xfId="2006" xr:uid="{5EA267D6-8E66-4747-B152-4678861E6E9C}"/>
     <cellStyle name="Normal 50 3" xfId="2056" xr:uid="{94B7053D-F0C4-43EA-8BBD-E8EEE51A73B1}"/>
     <cellStyle name="Normal 50 4" xfId="2109" xr:uid="{27280868-ECF2-4D7D-8DEB-75C7CAA06413}"/>
@@ -5550,6 +6038,10 @@
     <cellStyle name="Normal 50 8" xfId="2323" xr:uid="{75A7C4B9-3FE6-4180-AA85-67592ABAF173}"/>
     <cellStyle name="Normal 50 9" xfId="2377" xr:uid="{17CA0364-118F-4F64-99D0-9C535EAEFD78}"/>
     <cellStyle name="Normal 51" xfId="2007" xr:uid="{1602E624-09BF-4F71-AF6A-9A39C4FDA28D}"/>
+    <cellStyle name="Normal 51 10" xfId="2488" xr:uid="{98FD1495-FA05-48C4-A7E6-FEACB2B2AFB9}"/>
+    <cellStyle name="Normal 51 11" xfId="2543" xr:uid="{602C832C-1E0E-4C8B-A86E-DFCC7C206A00}"/>
+    <cellStyle name="Normal 51 12" xfId="2598" xr:uid="{3411D145-5D70-4277-9C19-98C1E7FBD1D2}"/>
+    <cellStyle name="Normal 51 13" xfId="2653" xr:uid="{01F34818-BD22-4F8A-9D1A-DFADC559C11D}"/>
     <cellStyle name="Normal 51 2" xfId="2057" xr:uid="{05B9550F-EDC2-4B34-8448-0CE71335699D}"/>
     <cellStyle name="Normal 51 3" xfId="2110" xr:uid="{EEADDD94-46EB-4534-81FD-415BB9146977}"/>
     <cellStyle name="Normal 51 4" xfId="2163" xr:uid="{D49AB824-E1AD-412A-B267-FD7C3B6A5F1D}"/>
@@ -5559,6 +6051,9 @@
     <cellStyle name="Normal 51 8" xfId="2378" xr:uid="{CA89F152-B08F-4A80-A825-FC8BAF49EA75}"/>
     <cellStyle name="Normal 51 9" xfId="2433" xr:uid="{87E97C19-6A6E-44A6-A765-32E185B6092D}"/>
     <cellStyle name="Normal 52" xfId="2058" xr:uid="{0CE4F744-196E-4D85-989F-D205FE46F16C}"/>
+    <cellStyle name="Normal 52 10" xfId="2544" xr:uid="{BA2FE816-9D57-4C39-8C1D-8FFD9462F1A2}"/>
+    <cellStyle name="Normal 52 11" xfId="2599" xr:uid="{48869502-3B3C-4D2E-A9D4-F18D8144C2A4}"/>
+    <cellStyle name="Normal 52 12" xfId="2654" xr:uid="{C87CF75B-EF7C-45CB-9521-97307C655F76}"/>
     <cellStyle name="Normal 52 2" xfId="2111" xr:uid="{2C609632-C4ED-40F2-8062-2BB9333D71A1}"/>
     <cellStyle name="Normal 52 3" xfId="2164" xr:uid="{38502271-BE6F-47FA-9158-64F5F05DCB08}"/>
     <cellStyle name="Normal 52 4" xfId="2217" xr:uid="{BB0FA74F-2845-479E-940A-6418FF10EDEA}"/>
@@ -5566,7 +6061,11 @@
     <cellStyle name="Normal 52 6" xfId="2325" xr:uid="{8AF073A8-07B1-4AEC-893E-12DA8FB05D8D}"/>
     <cellStyle name="Normal 52 7" xfId="2379" xr:uid="{8953833D-E593-45FB-BA9A-89DE85F3367D}"/>
     <cellStyle name="Normal 52 8" xfId="2434" xr:uid="{2C5D1FE8-E7B2-4688-A30D-AA204DEF33CF}"/>
+    <cellStyle name="Normal 52 9" xfId="2489" xr:uid="{C179ADBE-137E-4CE1-9C73-18AF2FE296AA}"/>
     <cellStyle name="Normal 53" xfId="2059" xr:uid="{3EE05AE3-F5B9-4F71-93D8-B780EEE67BD1}"/>
+    <cellStyle name="Normal 53 10" xfId="2545" xr:uid="{8C6530DA-41F7-4571-80BF-CE550551732B}"/>
+    <cellStyle name="Normal 53 11" xfId="2600" xr:uid="{63BC088F-798F-4007-A069-AB104C765385}"/>
+    <cellStyle name="Normal 53 12" xfId="2655" xr:uid="{2CAF221B-D2F4-4F52-AAA8-12F076279079}"/>
     <cellStyle name="Normal 53 2" xfId="2112" xr:uid="{16C62648-6EA8-4037-9ED8-095F822FF00A}"/>
     <cellStyle name="Normal 53 3" xfId="2165" xr:uid="{06B1AB3E-FD03-476B-ABB1-E3CA9C13FD86}"/>
     <cellStyle name="Normal 53 4" xfId="2218" xr:uid="{3C01CD0D-BB46-489D-BB4D-0F40A7561659}"/>
@@ -5574,7 +6073,11 @@
     <cellStyle name="Normal 53 6" xfId="2326" xr:uid="{E0E0C773-FA00-483B-9072-C942818E34A4}"/>
     <cellStyle name="Normal 53 7" xfId="2380" xr:uid="{2072F87A-F786-48EC-A7D2-AE91A3BEB1E5}"/>
     <cellStyle name="Normal 53 8" xfId="2435" xr:uid="{5C97FA71-FC66-4909-9C05-A3B7FB57E66D}"/>
+    <cellStyle name="Normal 53 9" xfId="2490" xr:uid="{7E4E2ACB-CF1A-43BB-8491-9E1EA3E80ADC}"/>
     <cellStyle name="Normal 54" xfId="2060" xr:uid="{AE4474E6-4D1D-4C68-ACD4-E1952962F9F8}"/>
+    <cellStyle name="Normal 54 10" xfId="2546" xr:uid="{506FFD66-3A0A-4238-96D3-4AFFA4C56879}"/>
+    <cellStyle name="Normal 54 11" xfId="2601" xr:uid="{1EBEAD19-BB8E-4118-A3D6-E322867DDD06}"/>
+    <cellStyle name="Normal 54 12" xfId="2656" xr:uid="{6237C52D-F099-4572-9D05-82FB1661022A}"/>
     <cellStyle name="Normal 54 2" xfId="2113" xr:uid="{52C4B073-4C53-40E7-A256-18B3D9AD7A02}"/>
     <cellStyle name="Normal 54 3" xfId="2166" xr:uid="{5464CF50-21BE-4C16-B689-EB526957E877}"/>
     <cellStyle name="Normal 54 4" xfId="2219" xr:uid="{DFDA0EC6-330A-4F76-B02D-67ECB9E2963B}"/>
@@ -5582,13 +6085,22 @@
     <cellStyle name="Normal 54 6" xfId="2327" xr:uid="{55EF33D0-6E3D-455B-A82B-6A9C2F6B3BAC}"/>
     <cellStyle name="Normal 54 7" xfId="2381" xr:uid="{05B083E7-E93A-465F-AD6D-116CF354D2B0}"/>
     <cellStyle name="Normal 54 8" xfId="2436" xr:uid="{B7883CF5-9F52-4891-BAA2-505887CBE3B9}"/>
+    <cellStyle name="Normal 54 9" xfId="2491" xr:uid="{CE13531C-89CA-4088-A71C-09946268A9C5}"/>
     <cellStyle name="Normal 55" xfId="2220" xr:uid="{F2DBE977-3055-4B8C-8DB1-9063802CB3CE}"/>
     <cellStyle name="Normal 55 2" xfId="2274" xr:uid="{2AFC1409-514C-44F8-A16A-009B4AAA5942}"/>
     <cellStyle name="Normal 55 3" xfId="2328" xr:uid="{1779E91A-B6EE-4CCD-A0AA-3104AAC79AD1}"/>
     <cellStyle name="Normal 55 4" xfId="2382" xr:uid="{82A622E9-AAF1-4266-998C-63CC070A21C0}"/>
     <cellStyle name="Normal 55 5" xfId="2437" xr:uid="{A3132FCE-3118-4D83-BD66-780B5BB8B4B9}"/>
+    <cellStyle name="Normal 55 6" xfId="2492" xr:uid="{B1F7CAF8-3E4D-479C-BBEF-8721924C6A0D}"/>
+    <cellStyle name="Normal 55 7" xfId="2547" xr:uid="{04499E0B-EE07-424F-8A0E-F106056CFD4E}"/>
+    <cellStyle name="Normal 55 8" xfId="2602" xr:uid="{3F7D91E9-8E15-4C2B-AD8B-54544E42ED39}"/>
+    <cellStyle name="Normal 55 9" xfId="2657" xr:uid="{2332CC96-CAB7-4C4F-AB22-1982EB42FB84}"/>
     <cellStyle name="Normal 56" xfId="2383" xr:uid="{A9CCEEB6-8E80-47DA-918C-160799DDECFE}"/>
     <cellStyle name="Normal 56 2" xfId="2438" xr:uid="{EA476B24-9472-4541-8F5A-FCAE56DDBF2E}"/>
+    <cellStyle name="Normal 56 3" xfId="2493" xr:uid="{6EB1B442-4D38-4DA0-BE5C-8BDA89B86CB0}"/>
+    <cellStyle name="Normal 56 4" xfId="2548" xr:uid="{C4EF64E2-6B10-47A6-AC84-1B2E1223A04A}"/>
+    <cellStyle name="Normal 56 5" xfId="2603" xr:uid="{3A0B3AB3-F81A-4C14-8937-2F0F8CBDCCCB}"/>
+    <cellStyle name="Normal 56 6" xfId="2658" xr:uid="{E700C0E4-3C35-479B-B321-E16FD5A757F6}"/>
     <cellStyle name="Normal 6" xfId="5" xr:uid="{31BE2080-B222-435D-8A48-DEEADDEF6488}"/>
     <cellStyle name="Normal 6 10" xfId="62" xr:uid="{F76AEC00-2B15-423C-8653-788DAF9DBB9C}"/>
     <cellStyle name="Normal 6 11" xfId="69" xr:uid="{69EF0E4C-7EAA-4CE4-BF59-7EC105A17AD6}"/>
@@ -5681,6 +6193,10 @@
     <cellStyle name="Normal 6 90" xfId="2279" xr:uid="{06EE96EA-EAD6-468F-B2AF-96E6265EF28B}"/>
     <cellStyle name="Normal 6 91" xfId="2333" xr:uid="{8A1D3E8B-D1A5-47A6-BBB2-C109B4871F0E}"/>
     <cellStyle name="Normal 6 92" xfId="2388" xr:uid="{C135A5E6-5C3D-4830-89B5-3D0520DA2838}"/>
+    <cellStyle name="Normal 6 93" xfId="2443" xr:uid="{D6C30ACF-7EE8-453C-A6DB-38EFD2638D0B}"/>
+    <cellStyle name="Normal 6 94" xfId="2498" xr:uid="{47FD3778-BDE7-4B81-85DC-C40989C808B6}"/>
+    <cellStyle name="Normal 6 95" xfId="2553" xr:uid="{2D64A2C1-ACA0-46A6-8978-38AE9C3F0541}"/>
+    <cellStyle name="Normal 6 96" xfId="2608" xr:uid="{DD4C3072-729B-4CDD-B99B-CC3C38B280EA}"/>
     <cellStyle name="Normal 7" xfId="6" xr:uid="{8FDF4D0E-5067-42C1-8AB6-21A2DD8B8199}"/>
     <cellStyle name="Normal 7 10" xfId="63" xr:uid="{076EEBFE-E343-48C7-AD51-40C5F37875B2}"/>
     <cellStyle name="Normal 7 11" xfId="70" xr:uid="{C92A195D-1E83-4EB3-9856-15A82899A737}"/>
@@ -5773,6 +6289,10 @@
     <cellStyle name="Normal 7 90" xfId="2280" xr:uid="{3DA0ABFA-1CCE-4CA0-A956-CC53B58810BC}"/>
     <cellStyle name="Normal 7 91" xfId="2334" xr:uid="{D477CCCE-F30D-43A7-9E53-C355DDF51A0B}"/>
     <cellStyle name="Normal 7 92" xfId="2389" xr:uid="{E03EC799-9821-4D71-B66B-72F90FBE39B6}"/>
+    <cellStyle name="Normal 7 93" xfId="2444" xr:uid="{5AD4DF28-5F05-46C8-9ABC-E14722F55C2B}"/>
+    <cellStyle name="Normal 7 94" xfId="2499" xr:uid="{C123C8E0-A08F-4E26-9A73-77BA00C8621B}"/>
+    <cellStyle name="Normal 7 95" xfId="2554" xr:uid="{DE55F490-1530-4336-9520-0F427D50F2C5}"/>
+    <cellStyle name="Normal 7 96" xfId="2609" xr:uid="{016B4DC6-8175-41FB-88EE-1C6A602C4928}"/>
     <cellStyle name="Normal 8" xfId="43" xr:uid="{B3C5BFDC-2A95-4E6A-803F-B149318E48CC}"/>
     <cellStyle name="Normal 8 10" xfId="109" xr:uid="{2C5F0F9A-3251-494A-998A-DF2DB5E1065F}"/>
     <cellStyle name="Normal 8 11" xfId="117" xr:uid="{A66804B5-EC5B-4C85-82CD-D00400FFCA77}"/>
@@ -5858,7 +6378,11 @@
     <cellStyle name="Normal 8 84" xfId="2281" xr:uid="{60C0B795-2541-486C-9198-8DC05CA563AD}"/>
     <cellStyle name="Normal 8 85" xfId="2335" xr:uid="{AAD6890D-63DB-4C8A-8A32-998ED113A0BF}"/>
     <cellStyle name="Normal 8 86" xfId="2390" xr:uid="{E132F386-A7C7-4587-8EB3-0AF430E209A1}"/>
+    <cellStyle name="Normal 8 87" xfId="2445" xr:uid="{615C99C2-1E28-4FD9-93AF-046827DE317D}"/>
+    <cellStyle name="Normal 8 88" xfId="2500" xr:uid="{781EFB90-80F0-44F8-8439-C3271C7D1EFF}"/>
+    <cellStyle name="Normal 8 89" xfId="2555" xr:uid="{F6C155A5-4017-4361-8DB6-AF51C97C6BB4}"/>
     <cellStyle name="Normal 8 9" xfId="101" xr:uid="{EF361D85-BD7F-4E58-9FE7-65473E5583EE}"/>
+    <cellStyle name="Normal 8 90" xfId="2610" xr:uid="{B10BCBE7-C417-4176-B770-6D4AF5496FDE}"/>
     <cellStyle name="Normal 9" xfId="86" xr:uid="{63C162E7-EB2C-460C-8F1B-D9BC4CBB1C65}"/>
     <cellStyle name="Normal 9 10" xfId="158" xr:uid="{EA44C88E-C9B8-4EDC-99A4-D9EF32DAD79D}"/>
     <cellStyle name="Normal 9 11" xfId="167" xr:uid="{361119E1-3FCE-4102-8A43-24B6D72873F7}"/>
@@ -5938,6 +6462,10 @@
     <cellStyle name="Normal 9 79" xfId="2336" xr:uid="{C559C16F-DB6C-49BE-A51D-8CD882767249}"/>
     <cellStyle name="Normal 9 8" xfId="142" xr:uid="{E908BA3A-342A-42A4-9F3A-16B68FBD5C5D}"/>
     <cellStyle name="Normal 9 80" xfId="2391" xr:uid="{4C05A15E-331E-4A69-BB5F-547555C33CB4}"/>
+    <cellStyle name="Normal 9 81" xfId="2446" xr:uid="{F7C6DAAD-C7E4-404C-AF6A-3D5841C72195}"/>
+    <cellStyle name="Normal 9 82" xfId="2501" xr:uid="{9C379A32-672A-4123-9C85-292B6C63FB20}"/>
+    <cellStyle name="Normal 9 83" xfId="2556" xr:uid="{4058EEFE-43E1-4197-B4FE-D2D046E6A8B2}"/>
+    <cellStyle name="Normal 9 84" xfId="2611" xr:uid="{516B1A08-7F68-4A1B-BB56-F4DAAE27CD74}"/>
     <cellStyle name="Normal 9 9" xfId="150" xr:uid="{5810B583-F0FF-4873-A2AE-BF7471C0EA6E}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6238,10 +6766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CD7"/>
+  <dimension ref="A1:CD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6527,165 +7055,241 @@
       </c>
     </row>
     <row r="2" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" s="3">
+        <v>5610</v>
+      </c>
+      <c r="V2" s="2">
+        <v>44562</v>
+      </c>
+      <c r="W2" t="s">
+        <v>91</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>33136</v>
+      </c>
+      <c r="AL2" s="2"/>
+      <c r="AT2" s="7"/>
+      <c r="AV2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="AX2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BD2" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="7">
-        <v>22500</v>
-      </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI2" s="5" t="s">
+      <c r="BE2" t="s">
         <v>94</v>
       </c>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="6">
-        <v>33837</v>
-      </c>
-      <c r="AL2" s="6">
-        <v>32560</v>
-      </c>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5" t="s">
+      <c r="BQ2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY2" t="s">
         <v>95</v>
       </c>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="BE2" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="BF2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="BN2" s="5"/>
-      <c r="BO2" s="5"/>
-      <c r="BP2" s="5"/>
-      <c r="BQ2" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5"/>
-      <c r="BY2" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="BZ2" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="CA2" s="5"/>
-      <c r="CB2" s="5"/>
-      <c r="CC2" s="5"/>
-      <c r="CD2" s="5" t="s">
-        <v>102</v>
+      <c r="CD2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="AK3" s="2"/>
-      <c r="AL3" s="2"/>
+      <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" t="s">
+        <v>99</v>
+      </c>
+      <c r="O3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3" s="3">
+        <v>497</v>
+      </c>
+      <c r="V3" s="2">
+        <v>44713</v>
+      </c>
+      <c r="W3" t="s">
+        <v>102</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>28183</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>29090</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>100</v>
+      </c>
       <c r="AZ3"/>
       <c r="BA3"/>
+      <c r="BD3" t="s">
+        <v>98</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>108</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="O4" s="4"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="AK4" s="2"/>
+      <c r="A4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>111</v>
+      </c>
+      <c r="N4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O4" t="s">
+        <v>113</v>
+      </c>
+      <c r="P4" t="s">
+        <v>114</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1750</v>
+      </c>
+      <c r="V4" t="s">
+        <v>115</v>
+      </c>
+      <c r="W4" t="s">
+        <v>116</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>32902</v>
+      </c>
       <c r="AL4" s="2"/>
+      <c r="AV4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>113</v>
+      </c>
       <c r="AZ4"/>
       <c r="BA4"/>
+      <c r="BD4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>119</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>83</v>
+      </c>
+      <c r="BY4" t="s">
+        <v>120</v>
+      </c>
+      <c r="CD4" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="T5" s="3"/>
       <c r="V5"/>
       <c r="W5"/>
@@ -6696,19 +7300,105 @@
       <c r="BA5"/>
     </row>
     <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="T6" s="3"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
       <c r="AZ6"/>
       <c r="BA6"/>
     </row>
     <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="T7" s="3"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AZ7"/>
       <c r="BA7"/>
     </row>
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="T8" s="3"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+    </row>
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="T9" s="3"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AZ9"/>
+      <c r="BA9"/>
+    </row>
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="T10" s="3"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AZ10"/>
+      <c r="BA10"/>
+    </row>
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="T11" s="5"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AZ11"/>
+      <c r="BA11"/>
+    </row>
+    <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="T12" s="3"/>
+      <c r="AZ12"/>
+      <c r="BA12"/>
+    </row>
+    <row r="13" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="T13" s="3"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AZ13"/>
+      <c r="BA13"/>
+    </row>
+    <row r="14" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="T14" s="3"/>
+      <c r="AK14" s="2"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+    </row>
+    <row r="15" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="H15" s="4"/>
+      <c r="T15" s="5"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AZ15"/>
+      <c r="BA15"/>
+    </row>
+    <row r="16" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="AK16" s="2"/>
+      <c r="AZ16"/>
+      <c r="BA16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated running SDLT CODE with bacs submit date
</commit_message>
<xml_diff>
--- a/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
+++ b/SDLT Running Code/DocumentUnderstandingFinal/extracted_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Taylors\DocumentUnderstandingFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7365F03-BD69-4EC2-BF27-714833042D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77887BEF-EA79-41E4-8C02-6276BAF54FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t>Insight Ref</t>
   </si>
@@ -274,122 +274,101 @@
     <t>No</t>
   </si>
   <si>
-    <t>Leasehold</t>
-  </si>
-  <si>
-    <t>NNT1028</t>
-  </si>
-  <si>
-    <t>Beenish Ali</t>
-  </si>
-  <si>
-    <t>39 Parkes Avenue, Birmingham</t>
-  </si>
-  <si>
-    <t>Birmingham</t>
-  </si>
-  <si>
-    <t>GALLIARD WAVENSMERE (MIDDLEWAY) LIMITED</t>
-  </si>
-  <si>
-    <t>3rd Floor Sterling House Langston Road Loughton Essex IG10 3TS</t>
-  </si>
-  <si>
-    <t>12/31/3021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beenish </t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>B12 9AW</t>
-  </si>
-  <si>
-    <t>SC809688A</t>
-  </si>
-  <si>
-    <t>NBT1872</t>
-  </si>
-  <si>
-    <t>Marius Catalin Voica</t>
-  </si>
-  <si>
-    <t>17 Elder Crescent, St Neots</t>
-  </si>
-  <si>
-    <t>Huntingdon</t>
-  </si>
-  <si>
-    <t>DURKAN (ST NEOTS) LIMITED</t>
-  </si>
-  <si>
-    <t>4 Elstree Gate, Elstree Way, Borehamwood, WD6 1JD</t>
-  </si>
-  <si>
-    <t>05/30/3021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marius Catalin </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria-Magdalena </t>
-  </si>
-  <si>
-    <t>Voica</t>
-  </si>
-  <si>
-    <t>PE19 0BF</t>
-  </si>
-  <si>
-    <t>SS438175D</t>
-  </si>
-  <si>
-    <t>ST210146C</t>
-  </si>
-  <si>
-    <t>NNT1227</t>
-  </si>
-  <si>
-    <t>Silje Merete Saethren Gronning</t>
-  </si>
-  <si>
-    <t>37 Pembrey Court, Bollo Lane</t>
-  </si>
-  <si>
-    <t>Ealing</t>
-  </si>
-  <si>
-    <t>ACTON GARDENS LLP</t>
-  </si>
-  <si>
-    <t>Countryside House The Drive Brentwood Essex CM13 3AT</t>
-  </si>
-  <si>
-    <t>01/29/2021</t>
-  </si>
-  <si>
-    <t>01/25/2271</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silje Merete Saethren </t>
-  </si>
-  <si>
-    <t>Gronning</t>
-  </si>
-  <si>
-    <t>W3 8QR</t>
-  </si>
-  <si>
-    <t>SY217118C</t>
+    <t>Freehold</t>
+  </si>
+  <si>
+    <t>MRT1835</t>
+  </si>
+  <si>
+    <t>Antonia Jane Allen</t>
+  </si>
+  <si>
+    <t>9 Ennismore Gardens,Southend-On-Sea</t>
+  </si>
+  <si>
+    <t>Southend-on-Sea</t>
+  </si>
+  <si>
+    <t>SIMON AARON PIZZULO</t>
+  </si>
+  <si>
+    <t>9 Ennismore Gardens,Southend-on-sea, SS2 5RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonia Jane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eamonn Michael </t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Flynn</t>
+  </si>
+  <si>
+    <t>EX204100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS2 5RA </t>
+  </si>
+  <si>
+    <t>Eamonn Michael Flynn</t>
+  </si>
+  <si>
+    <t>JP406296A</t>
+  </si>
+  <si>
+    <t>JE282389B</t>
+  </si>
+  <si>
+    <t>NBT1893</t>
+  </si>
+  <si>
+    <t>Fulvio Zaccagna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Grey Way Cambridge </t>
+  </si>
+  <si>
+    <t>South Cambridgeshire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HILL MARSHALL (PHASE 2) LLP </t>
+  </si>
+  <si>
+    <t>The Power House Gunpowder Mill Powdermill Lane Waltham Abbey Essex EN9 1BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fulvio </t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Zaccagna</t>
+  </si>
+  <si>
+    <t>Lyasheva</t>
+  </si>
+  <si>
+    <t>CB5 8XT</t>
+  </si>
+  <si>
+    <t>Maria Lyasheva</t>
+  </si>
+  <si>
+    <t>ST077161B</t>
+  </si>
+  <si>
+    <t>SS779628A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="104" x14ac:knownFonts="1">
+  <fonts count="108" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1104,13 +1083,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1133,14 +1141,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2659">
+  <cellStyleXfs count="3118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="101" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="99" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="97" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="95" fillId="0" borderId="0"/>
@@ -1153,6 +1192,8 @@
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="93" fillId="0" borderId="0"/>
@@ -1165,6 +1206,8 @@
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="91" fillId="0" borderId="0"/>
@@ -1185,6 +1228,8 @@
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="88" fillId="0" borderId="0"/>
@@ -1199,6 +1244,7 @@
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
@@ -1206,6 +1252,8 @@
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="85" fillId="0" borderId="0"/>
@@ -1253,6 +1301,9 @@
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="79" fillId="0" borderId="0"/>
@@ -1269,6 +1320,9 @@
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
@@ -1277,6 +1331,15 @@
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="0"/>
@@ -1294,6 +1357,16 @@
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
@@ -1315,6 +1388,16 @@
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0"/>
@@ -1340,6 +1423,16 @@
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0"/>
@@ -1369,6 +1462,15 @@
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
@@ -1402,6 +1504,11 @@
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0"/>
@@ -1439,6 +1546,8 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0"/>
@@ -1479,6 +1588,9 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0"/>
@@ -1519,6 +1631,8 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
@@ -1539,6 +1653,10 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0"/>
@@ -1581,6 +1699,10 @@
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
@@ -1625,6 +1747,14 @@
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
@@ -1670,6 +1800,14 @@
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0"/>
@@ -1717,6 +1855,11 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0"/>
@@ -1850,6 +1993,8 @@
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
@@ -1904,6 +2049,10 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
@@ -1958,6 +2107,10 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0"/>
@@ -2014,6 +2167,12 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0"/>
@@ -2072,6 +2231,17 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
@@ -2131,6 +2301,21 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
@@ -2194,6 +2379,21 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
@@ -2263,6 +2463,18 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
@@ -2339,6 +2551,14 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
@@ -2420,6 +2640,12 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
@@ -2504,6 +2730,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
@@ -2635,7 +2864,8 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
@@ -2724,6 +2954,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
@@ -2768,6 +3000,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
@@ -2858,6 +3097,15 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
@@ -2948,6 +3196,19 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
@@ -3043,6 +3304,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
@@ -3142,6 +3413,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
@@ -3248,6 +3524,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
@@ -3301,6 +3579,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -3409,6 +3690,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
@@ -3519,225 +3802,409 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -3799,15 +4266,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2771"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3117"/>
   </cellXfs>
-  <cellStyles count="2659">
+  <cellStyles count="3118">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="159" xr:uid="{22378139-A9D0-4012-B7E1-FB95B8397E06}"/>
     <cellStyle name="Normal 10 10" xfId="276" xr:uid="{2FF1057A-C0FD-428A-B8F5-F70C6C4ED22C}"/>
@@ -3821,6 +4286,10 @@
     <cellStyle name="Normal 10 18" xfId="434" xr:uid="{566DA8E5-73DD-4ADC-9C00-AC8B82F02C95}"/>
     <cellStyle name="Normal 10 19" xfId="455" xr:uid="{88FA9C08-71ED-463D-8940-F00C4CF4173B}"/>
     <cellStyle name="Normal 10 2" xfId="168" xr:uid="{3716FB09-55A4-492C-96B2-FB32E1B803DB}"/>
+    <cellStyle name="Normal 10 2 2" xfId="2723" xr:uid="{F3B0FCFC-C24A-4A8A-9422-E631A4DA80F5}"/>
+    <cellStyle name="Normal 10 2 3" xfId="2836" xr:uid="{178A18CB-3247-4DC7-BEE8-EDACF3629CC4}"/>
+    <cellStyle name="Normal 10 2 4" xfId="2951" xr:uid="{C75D4F03-5503-413B-BBAB-6A65229E86AE}"/>
+    <cellStyle name="Normal 10 2 5" xfId="3066" xr:uid="{DA75600E-CAB0-4F0D-B716-8394143246AF}"/>
     <cellStyle name="Normal 10 20" xfId="477" xr:uid="{2DB7D6E5-87D7-4738-B504-0339A1B197D2}"/>
     <cellStyle name="Normal 10 21" xfId="499" xr:uid="{8930B16E-2F15-4BF1-B604-76F36DF80C6E}"/>
     <cellStyle name="Normal 10 22" xfId="521" xr:uid="{FE174B41-9072-432C-AE45-D0EE8E84BF49}"/>
@@ -3882,6 +4351,10 @@
     <cellStyle name="Normal 10 73" xfId="2502" xr:uid="{8AF875CF-F651-4302-A3AA-3E7056484FC8}"/>
     <cellStyle name="Normal 10 74" xfId="2557" xr:uid="{49E28582-A60D-4E32-B0D2-7FE8CAE252C0}"/>
     <cellStyle name="Normal 10 75" xfId="2612" xr:uid="{EC917C18-EB20-4349-B638-A60B5299BAB4}"/>
+    <cellStyle name="Normal 10 76" xfId="2668" xr:uid="{2E85F436-C34D-43DF-863E-AC33260D1CF5}"/>
+    <cellStyle name="Normal 10 77" xfId="2781" xr:uid="{A459FC36-3139-4FB8-9C32-E13D046CA508}"/>
+    <cellStyle name="Normal 10 78" xfId="2896" xr:uid="{DED570F2-354D-4426-AA1A-B9B512F8953F}"/>
+    <cellStyle name="Normal 10 79" xfId="3011" xr:uid="{B9C7766F-ACA4-4CE7-8930-4DE374C3C3A6}"/>
     <cellStyle name="Normal 10 8" xfId="243" xr:uid="{731BFDFC-42EF-40DB-B469-49423BAFDD34}"/>
     <cellStyle name="Normal 10 9" xfId="259" xr:uid="{C9BCE7F2-A0DC-424E-BD2A-3833A66918FA}"/>
     <cellStyle name="Normal 11" xfId="169" xr:uid="{24883276-07D4-417F-A269-AF8F8014D6B0}"/>
@@ -3896,6 +4369,10 @@
     <cellStyle name="Normal 11 18" xfId="456" xr:uid="{8CB173FF-5B39-478F-9CC5-3F325A68988E}"/>
     <cellStyle name="Normal 11 19" xfId="478" xr:uid="{5BEFD56E-ADCD-4BB9-AE67-28C8723F18DE}"/>
     <cellStyle name="Normal 11 2" xfId="179" xr:uid="{130016AE-D5FA-4662-9B50-CE6ACC5499A1}"/>
+    <cellStyle name="Normal 11 2 2" xfId="2724" xr:uid="{8F69685B-A219-46F9-B9D4-7A7F8B1DDC5A}"/>
+    <cellStyle name="Normal 11 2 3" xfId="2837" xr:uid="{6020186E-14FB-4B53-BEBC-C08FBE8600E3}"/>
+    <cellStyle name="Normal 11 2 4" xfId="2952" xr:uid="{713C45EC-B86E-4CB9-8AE1-F67208F2129D}"/>
+    <cellStyle name="Normal 11 2 5" xfId="3067" xr:uid="{B3E64FA8-FDD5-4DA0-AD7D-3CE3D92E5F17}"/>
     <cellStyle name="Normal 11 20" xfId="500" xr:uid="{88F4E02F-46CD-4EC6-888D-723B7D083F54}"/>
     <cellStyle name="Normal 11 21" xfId="522" xr:uid="{258FCF74-010E-4A2C-897C-1B21762EABCC}"/>
     <cellStyle name="Normal 11 22" xfId="545" xr:uid="{152CD45D-038B-4567-9C68-09E5D8E6A939}"/>
@@ -3956,6 +4433,10 @@
     <cellStyle name="Normal 11 72" xfId="2503" xr:uid="{2DFE5952-5804-4494-974F-A1A32EFB97D8}"/>
     <cellStyle name="Normal 11 73" xfId="2558" xr:uid="{AC4A5DD0-35B8-4401-BAED-320FE3BEA9E9}"/>
     <cellStyle name="Normal 11 74" xfId="2613" xr:uid="{FCF100BA-F732-4A2A-8BD9-F8B34A42C056}"/>
+    <cellStyle name="Normal 11 75" xfId="2669" xr:uid="{BA58132F-0ADD-468C-B671-BBA2229F4776}"/>
+    <cellStyle name="Normal 11 76" xfId="2782" xr:uid="{E3AAE904-F1FC-4F54-AA21-CEC030E253C9}"/>
+    <cellStyle name="Normal 11 77" xfId="2897" xr:uid="{F557F5EB-96BF-482C-8DE0-8617CEBAEF19}"/>
+    <cellStyle name="Normal 11 78" xfId="3012" xr:uid="{BCF82DC2-F99B-424D-9079-E90AE364E318}"/>
     <cellStyle name="Normal 11 8" xfId="260" xr:uid="{F04D5FA1-BA3E-4D95-B369-72C9BC4A33B2}"/>
     <cellStyle name="Normal 11 9" xfId="277" xr:uid="{2BA3F0B3-DDFB-4ED8-8F9B-FB1DE74EA628}"/>
     <cellStyle name="Normal 12" xfId="180" xr:uid="{64C12A1D-7934-48F2-9578-4F1C04C3D62D}"/>
@@ -3970,6 +4451,10 @@
     <cellStyle name="Normal 12 18" xfId="479" xr:uid="{7A08F92F-C826-49A8-BC45-399BC95EB284}"/>
     <cellStyle name="Normal 12 19" xfId="501" xr:uid="{66A78CF5-EAF9-4D70-A12B-CD2DCF9BF326}"/>
     <cellStyle name="Normal 12 2" xfId="191" xr:uid="{4D1A1AB3-964B-4B10-A0B6-2C98055D3011}"/>
+    <cellStyle name="Normal 12 2 2" xfId="2725" xr:uid="{0FECAFEC-A875-45C4-B280-A18629EBCD4A}"/>
+    <cellStyle name="Normal 12 2 3" xfId="2838" xr:uid="{07054F0B-FC4F-41DD-91C0-4D3F9FC27BFC}"/>
+    <cellStyle name="Normal 12 2 4" xfId="2953" xr:uid="{EDC4DDBA-C50B-497A-ADE5-056A33B5A541}"/>
+    <cellStyle name="Normal 12 2 5" xfId="3068" xr:uid="{1A7497C5-A6BC-4151-A224-AB059D18545B}"/>
     <cellStyle name="Normal 12 20" xfId="523" xr:uid="{7AF5DEAB-3646-4404-BDBA-32B1411EB06E}"/>
     <cellStyle name="Normal 12 21" xfId="546" xr:uid="{FD674B26-97D9-42C3-BB29-9C0A94DE3118}"/>
     <cellStyle name="Normal 12 22" xfId="569" xr:uid="{D951D010-525D-42F0-BC59-6660A7207E10}"/>
@@ -4029,6 +4514,10 @@
     <cellStyle name="Normal 12 71" xfId="2504" xr:uid="{3615E3BD-D9C4-4BAB-885E-EFA81AACADDB}"/>
     <cellStyle name="Normal 12 72" xfId="2559" xr:uid="{FF88AEF1-874E-4270-97A7-9EC34BE1C4CD}"/>
     <cellStyle name="Normal 12 73" xfId="2614" xr:uid="{F6CCAAA2-324E-4AEA-BF07-043F0A246A18}"/>
+    <cellStyle name="Normal 12 74" xfId="2670" xr:uid="{4E6C1416-7E86-458A-A88E-EF260D0A4234}"/>
+    <cellStyle name="Normal 12 75" xfId="2783" xr:uid="{BAF4121C-7EE6-4556-A77E-93AC5B380E6F}"/>
+    <cellStyle name="Normal 12 76" xfId="2898" xr:uid="{322BF0E7-3984-43C6-B910-3E5B7E03D789}"/>
+    <cellStyle name="Normal 12 77" xfId="3013" xr:uid="{A0E9934A-FF73-459F-938E-BA2F51895701}"/>
     <cellStyle name="Normal 12 8" xfId="278" xr:uid="{F6B4CBEB-461D-400D-9C34-7FB47B2F92C3}"/>
     <cellStyle name="Normal 12 9" xfId="296" xr:uid="{030E8C75-BAB4-4848-8367-E74DEC184755}"/>
     <cellStyle name="Normal 13" xfId="192" xr:uid="{6C53067C-9D55-4747-9EF8-9B2403AC3FD0}"/>
@@ -4043,6 +4532,10 @@
     <cellStyle name="Normal 13 18" xfId="502" xr:uid="{925AC024-E2FB-4E98-AB1A-2BB269BE451F}"/>
     <cellStyle name="Normal 13 19" xfId="524" xr:uid="{B57BAA49-146E-45DA-BD81-DB5ACBDF7D7E}"/>
     <cellStyle name="Normal 13 2" xfId="204" xr:uid="{8AE151E9-853F-417B-B941-4AE6B2133EFA}"/>
+    <cellStyle name="Normal 13 2 2" xfId="2726" xr:uid="{1CC0B17B-887A-4BE5-A861-1AFB3583F7DB}"/>
+    <cellStyle name="Normal 13 2 3" xfId="2839" xr:uid="{9DF29648-9783-4F8C-AD92-2BA66AC3F460}"/>
+    <cellStyle name="Normal 13 2 4" xfId="2954" xr:uid="{A33CB213-D311-4D2B-AAC0-78C8F0A7E153}"/>
+    <cellStyle name="Normal 13 2 5" xfId="3069" xr:uid="{32B89852-D60F-40DC-B523-83D9C5DCF865}"/>
     <cellStyle name="Normal 13 20" xfId="547" xr:uid="{5FA670B0-B60D-43E1-9282-22DC76A69A25}"/>
     <cellStyle name="Normal 13 21" xfId="570" xr:uid="{88660E7F-CB5F-46E8-9408-1AB6C5732FD3}"/>
     <cellStyle name="Normal 13 22" xfId="594" xr:uid="{4C9C0519-F79A-4F44-BAC8-FEC742243AE5}"/>
@@ -4101,6 +4594,10 @@
     <cellStyle name="Normal 13 70" xfId="2505" xr:uid="{C64E3BA5-FF66-43EF-BFD7-75D5FEA3EDDA}"/>
     <cellStyle name="Normal 13 71" xfId="2560" xr:uid="{C99F9691-E2FA-4D52-BDFA-E514FB7B812B}"/>
     <cellStyle name="Normal 13 72" xfId="2615" xr:uid="{7A83B077-482A-4B51-9768-C62DA4F9B90F}"/>
+    <cellStyle name="Normal 13 73" xfId="2671" xr:uid="{F1EEA7EA-929E-4309-8052-027D94C7D370}"/>
+    <cellStyle name="Normal 13 74" xfId="2784" xr:uid="{7BEA88AE-FE22-4191-8556-9E0BA84EFA86}"/>
+    <cellStyle name="Normal 13 75" xfId="2899" xr:uid="{FAB58A93-AF1D-4F78-B897-615D9A189226}"/>
+    <cellStyle name="Normal 13 76" xfId="3014" xr:uid="{6730B51D-9839-4120-A9F3-28E83176B6B7}"/>
     <cellStyle name="Normal 13 8" xfId="297" xr:uid="{4A5D7C9D-C5C5-40A5-8715-701C74A7B825}"/>
     <cellStyle name="Normal 13 9" xfId="316" xr:uid="{62B80AA8-8706-4987-866E-1A4286CD93CB}"/>
     <cellStyle name="Normal 14" xfId="205" xr:uid="{BCD27467-3820-4B0C-8969-F2BEB1D1C65E}"/>
@@ -4115,6 +4612,10 @@
     <cellStyle name="Normal 14 18" xfId="525" xr:uid="{96CDE341-5060-4361-8746-CE74C60AC966}"/>
     <cellStyle name="Normal 14 19" xfId="548" xr:uid="{077D2CA1-E330-4235-B865-98B4D69D54A7}"/>
     <cellStyle name="Normal 14 2" xfId="218" xr:uid="{F042C9FE-856D-41E2-A9AA-C2A6D329B35D}"/>
+    <cellStyle name="Normal 14 2 2" xfId="2727" xr:uid="{BE0CDDB7-1EF2-41A0-BC15-F97A8826CF53}"/>
+    <cellStyle name="Normal 14 2 3" xfId="2840" xr:uid="{AAEF7592-A455-419D-8A62-7E1EEC381956}"/>
+    <cellStyle name="Normal 14 2 4" xfId="2955" xr:uid="{2EE8B869-6531-445B-ABB4-3273ED437CD3}"/>
+    <cellStyle name="Normal 14 2 5" xfId="3070" xr:uid="{1C268757-AD40-4B84-BC36-28D504A1132A}"/>
     <cellStyle name="Normal 14 20" xfId="571" xr:uid="{F0B2A752-BEA3-4C7A-A775-93D03899DA88}"/>
     <cellStyle name="Normal 14 21" xfId="595" xr:uid="{6539DD4F-E664-4EE8-A030-2C71ECE485BD}"/>
     <cellStyle name="Normal 14 22" xfId="620" xr:uid="{26DA60DE-185E-41A9-8861-3CF2A57D68F6}"/>
@@ -4172,6 +4673,10 @@
     <cellStyle name="Normal 14 7" xfId="298" xr:uid="{CD68E702-2F82-4764-9927-11DABC2F5829}"/>
     <cellStyle name="Normal 14 70" xfId="2561" xr:uid="{7817E3AD-CD9D-4811-A502-04BB718C11BF}"/>
     <cellStyle name="Normal 14 71" xfId="2616" xr:uid="{1EEA5952-33B0-4DE5-91F2-2A9BBA452B97}"/>
+    <cellStyle name="Normal 14 72" xfId="2672" xr:uid="{A3091588-1418-48F0-A324-8195B7DF598E}"/>
+    <cellStyle name="Normal 14 73" xfId="2785" xr:uid="{82B361B4-B5B2-487D-9DC1-F2B0B6662731}"/>
+    <cellStyle name="Normal 14 74" xfId="2900" xr:uid="{12627874-4675-4F6A-8164-AEA4EE0499E0}"/>
+    <cellStyle name="Normal 14 75" xfId="3015" xr:uid="{54A0508D-5A3C-48DE-A099-1AA71FED807E}"/>
     <cellStyle name="Normal 14 8" xfId="317" xr:uid="{6DB7F330-9C64-4B26-AF4F-17A09E12CEC6}"/>
     <cellStyle name="Normal 14 9" xfId="337" xr:uid="{104D5C09-BA78-4885-AA2B-E347E11C3013}"/>
     <cellStyle name="Normal 15" xfId="219" xr:uid="{AFBD9F23-4328-44E1-ABF9-3CA063A03969}"/>
@@ -4186,6 +4691,10 @@
     <cellStyle name="Normal 15 18" xfId="549" xr:uid="{E546D0E9-90E1-41D9-91CF-A8BD5FBED054}"/>
     <cellStyle name="Normal 15 19" xfId="572" xr:uid="{2BF8E8AB-8D08-43D1-9E07-5F9D8F4B7714}"/>
     <cellStyle name="Normal 15 2" xfId="233" xr:uid="{748092AB-8223-4A46-A040-A424589129F5}"/>
+    <cellStyle name="Normal 15 2 2" xfId="2728" xr:uid="{085F0C71-3094-4FA3-8C7B-C998BBADB232}"/>
+    <cellStyle name="Normal 15 2 3" xfId="2841" xr:uid="{9C23E336-31F8-4EA8-9F8A-7198BF4C018B}"/>
+    <cellStyle name="Normal 15 2 4" xfId="2956" xr:uid="{7D4F3722-E89A-4B1E-B6B4-FF1FA2FE142D}"/>
+    <cellStyle name="Normal 15 2 5" xfId="3071" xr:uid="{985E6283-CA4E-4A1B-AAE7-73AF31D2981C}"/>
     <cellStyle name="Normal 15 20" xfId="596" xr:uid="{47C18674-AC6E-4A5E-BD29-36D300058610}"/>
     <cellStyle name="Normal 15 21" xfId="621" xr:uid="{14D99BBC-1CF1-4B13-A3A0-D76343B99C37}"/>
     <cellStyle name="Normal 15 22" xfId="648" xr:uid="{BF51743B-D4A5-4498-A5A1-B0775A805CD7}"/>
@@ -4242,6 +4751,10 @@
     <cellStyle name="Normal 15 69" xfId="2562" xr:uid="{972B9C56-438D-45D8-9D24-C5C9558B9A4A}"/>
     <cellStyle name="Normal 15 7" xfId="318" xr:uid="{BC74AE1A-9CA6-4EA4-BFD8-B522F63CB6FF}"/>
     <cellStyle name="Normal 15 70" xfId="2617" xr:uid="{1D79FB92-1D04-47CD-B5E8-80E88211DD5B}"/>
+    <cellStyle name="Normal 15 71" xfId="2673" xr:uid="{6A8CED07-B02B-40A8-A38F-C548DDE13684}"/>
+    <cellStyle name="Normal 15 72" xfId="2786" xr:uid="{907BE2F1-9A29-480D-BE36-14EC466F7B5F}"/>
+    <cellStyle name="Normal 15 73" xfId="2901" xr:uid="{2B6BBBC5-42B3-4D7F-BF36-8359B7FD87FC}"/>
+    <cellStyle name="Normal 15 74" xfId="3016" xr:uid="{AF9DC8B6-214C-4756-B0F9-17FF1277E09C}"/>
     <cellStyle name="Normal 15 8" xfId="338" xr:uid="{52CEAA3B-3AF8-4A6A-ADD3-4403D3D982ED}"/>
     <cellStyle name="Normal 15 9" xfId="358" xr:uid="{52621DB2-9BFC-4EF1-B2FF-A1D2EBD982F8}"/>
     <cellStyle name="Normal 16" xfId="234" xr:uid="{E124F5C7-1AAD-4493-AE1C-3BD849B8317F}"/>
@@ -4256,6 +4769,10 @@
     <cellStyle name="Normal 16 18" xfId="573" xr:uid="{57A049D5-BEFF-41DF-BB7F-0BBB54CD44B5}"/>
     <cellStyle name="Normal 16 19" xfId="597" xr:uid="{880B822C-1FC8-4F95-A559-FF8E85FA1B75}"/>
     <cellStyle name="Normal 16 2" xfId="249" xr:uid="{0A5D8F90-9851-49AB-B59B-4362A3840DFA}"/>
+    <cellStyle name="Normal 16 2 2" xfId="2729" xr:uid="{0DFED9F0-686C-4423-8A21-1653C589F822}"/>
+    <cellStyle name="Normal 16 2 3" xfId="2842" xr:uid="{19DB0F42-9A10-4E56-ACE1-623C1C32B52A}"/>
+    <cellStyle name="Normal 16 2 4" xfId="2957" xr:uid="{2E239A37-87F8-4E2D-954C-6D299FFF5ACD}"/>
+    <cellStyle name="Normal 16 2 5" xfId="3072" xr:uid="{77145E72-5AA4-44FE-857A-34F894EABD3F}"/>
     <cellStyle name="Normal 16 20" xfId="622" xr:uid="{7E33DFC5-00EE-4F11-80B5-514DD377DBA3}"/>
     <cellStyle name="Normal 16 21" xfId="649" xr:uid="{C961C8A7-4FAC-4606-9140-332E5F6B1DC0}"/>
     <cellStyle name="Normal 16 22" xfId="676" xr:uid="{D67F08F5-9990-438A-8854-F191C94092D6}"/>
@@ -4311,6 +4828,10 @@
     <cellStyle name="Normal 16 68" xfId="2563" xr:uid="{76850B5F-C664-4D3E-A016-922E180CB12B}"/>
     <cellStyle name="Normal 16 69" xfId="2618" xr:uid="{5A2B1924-4398-4DE5-AC88-3FB28BCB6039}"/>
     <cellStyle name="Normal 16 7" xfId="339" xr:uid="{FAA81CF7-9E8B-4D43-8B87-FEA4DEA195A2}"/>
+    <cellStyle name="Normal 16 70" xfId="2674" xr:uid="{86B46893-1E65-44FF-9BA4-1D36AFFD8EC2}"/>
+    <cellStyle name="Normal 16 71" xfId="2787" xr:uid="{552B0BB5-E915-4AA9-B06B-4F614CF17F6B}"/>
+    <cellStyle name="Normal 16 72" xfId="2902" xr:uid="{C5D868B0-1D63-450F-A191-D684FA37175F}"/>
+    <cellStyle name="Normal 16 73" xfId="3017" xr:uid="{F5B982D0-ADF0-4675-B2AB-0F118A931ADA}"/>
     <cellStyle name="Normal 16 8" xfId="359" xr:uid="{71945961-3DA4-41F9-B589-733CD154B56B}"/>
     <cellStyle name="Normal 16 9" xfId="379" xr:uid="{2D615019-0C6B-4533-BF0F-B9FB56006E3E}"/>
     <cellStyle name="Normal 17" xfId="250" xr:uid="{69954DE4-1D74-4139-BA78-EA933C610DF2}"/>
@@ -4325,6 +4846,10 @@
     <cellStyle name="Normal 17 18" xfId="598" xr:uid="{BD004F43-C58A-4DC4-A877-E3D6FF3FA456}"/>
     <cellStyle name="Normal 17 19" xfId="623" xr:uid="{0E6924D2-C2D1-4B47-8C20-F4425B6AEBFE}"/>
     <cellStyle name="Normal 17 2" xfId="266" xr:uid="{F1D36A7A-8DB5-4D88-8CB4-7A9E178707E7}"/>
+    <cellStyle name="Normal 17 2 2" xfId="2730" xr:uid="{B7D157E8-7E2F-4B96-8696-F9849C969FDA}"/>
+    <cellStyle name="Normal 17 2 3" xfId="2843" xr:uid="{744A1C99-A73A-4815-BF04-03C5691148F5}"/>
+    <cellStyle name="Normal 17 2 4" xfId="2958" xr:uid="{0EF0773C-A357-4A31-946C-9281FE8B6476}"/>
+    <cellStyle name="Normal 17 2 5" xfId="3073" xr:uid="{D35D0836-2201-48AD-AB7F-FDEF30B9085B}"/>
     <cellStyle name="Normal 17 20" xfId="650" xr:uid="{DBD82CD3-50BE-434F-8DC9-8E88545745BB}"/>
     <cellStyle name="Normal 17 21" xfId="677" xr:uid="{AC892011-F1B7-434D-8125-1DFF03A24A87}"/>
     <cellStyle name="Normal 17 22" xfId="704" xr:uid="{103CDE11-D9C3-4621-BBF4-5AA40660B613}"/>
@@ -4378,7 +4903,11 @@
     <cellStyle name="Normal 17 66" xfId="2509" xr:uid="{B7EC4B85-098B-4390-9F9C-776C10F548B2}"/>
     <cellStyle name="Normal 17 67" xfId="2564" xr:uid="{6936AE38-FA2C-4289-B99B-6C91220C7710}"/>
     <cellStyle name="Normal 17 68" xfId="2619" xr:uid="{9C851FCC-8BF9-4A5B-B2FE-1763AD5FDB0F}"/>
+    <cellStyle name="Normal 17 69" xfId="2675" xr:uid="{F65D5AAA-47CE-46D9-AA7D-84CC435E81C3}"/>
     <cellStyle name="Normal 17 7" xfId="360" xr:uid="{EF50DC9C-CCDF-49C3-BD04-EC1F385C2EB2}"/>
+    <cellStyle name="Normal 17 70" xfId="2788" xr:uid="{A7EEB7C3-7997-4699-A623-A305C771DD93}"/>
+    <cellStyle name="Normal 17 71" xfId="2903" xr:uid="{A5DC367F-5CE3-4E4F-8F32-3BBE22418895}"/>
+    <cellStyle name="Normal 17 72" xfId="3018" xr:uid="{B0C441C4-13BB-476D-B105-02064533FD0F}"/>
     <cellStyle name="Normal 17 8" xfId="380" xr:uid="{F7FF7910-81D8-41FE-87E6-74E265C4FE49}"/>
     <cellStyle name="Normal 17 9" xfId="400" xr:uid="{0131EC3E-0935-425F-A406-A9A4A62BE59C}"/>
     <cellStyle name="Normal 18" xfId="267" xr:uid="{FDAF5E90-B172-4DBD-A1E6-B7FF5860A653}"/>
@@ -4393,6 +4922,10 @@
     <cellStyle name="Normal 18 18" xfId="624" xr:uid="{267C44AE-9D10-4202-9AC0-4349BB70CDE2}"/>
     <cellStyle name="Normal 18 19" xfId="651" xr:uid="{98BCDEC0-B674-4806-949C-1FDB4DA04753}"/>
     <cellStyle name="Normal 18 2" xfId="284" xr:uid="{B765F507-3D95-43E7-BED7-151FB829D077}"/>
+    <cellStyle name="Normal 18 2 2" xfId="2731" xr:uid="{8ACDE65C-077D-424E-A8BB-AE8DEADB94EC}"/>
+    <cellStyle name="Normal 18 2 3" xfId="2844" xr:uid="{77119264-11C6-4CC3-BB78-3510EFD35720}"/>
+    <cellStyle name="Normal 18 2 4" xfId="2959" xr:uid="{F36637FB-A1BB-4B01-A2C1-3BB0BB7A279D}"/>
+    <cellStyle name="Normal 18 2 5" xfId="3074" xr:uid="{9E782847-B273-492C-A6C4-97BF0ABF1C66}"/>
     <cellStyle name="Normal 18 20" xfId="678" xr:uid="{D0053275-ACB2-4577-A806-A91398544E41}"/>
     <cellStyle name="Normal 18 21" xfId="705" xr:uid="{6B4728C5-62B5-4D66-B3FA-9D44766A2901}"/>
     <cellStyle name="Normal 18 22" xfId="732" xr:uid="{1CF657F2-D12B-44D8-AA6D-91FBC49F271A}"/>
@@ -4445,7 +4978,11 @@
     <cellStyle name="Normal 18 65" xfId="2510" xr:uid="{45DA049D-DA2E-4ABA-9720-CEFEACB7FBF1}"/>
     <cellStyle name="Normal 18 66" xfId="2565" xr:uid="{4B7414EA-3337-48F6-A515-DAB45D1E7FB1}"/>
     <cellStyle name="Normal 18 67" xfId="2620" xr:uid="{CDCE5D23-5134-4657-AB84-108242296EBF}"/>
+    <cellStyle name="Normal 18 68" xfId="2676" xr:uid="{90B42988-A297-47C9-9E59-482A6D2BCD2D}"/>
+    <cellStyle name="Normal 18 69" xfId="2789" xr:uid="{C3FA29DA-5E1D-43B6-B613-8C90BFF5597A}"/>
     <cellStyle name="Normal 18 7" xfId="381" xr:uid="{AA0AB4C2-AC98-4892-8993-9C51D645351A}"/>
+    <cellStyle name="Normal 18 70" xfId="2904" xr:uid="{5113557A-DD49-412A-A136-CFFB279A1B15}"/>
+    <cellStyle name="Normal 18 71" xfId="3019" xr:uid="{5405B1A6-4606-40A3-85B0-4742D0B0042D}"/>
     <cellStyle name="Normal 18 8" xfId="401" xr:uid="{97EBEF4A-C9B9-484A-A9B8-2BD6E9C715B6}"/>
     <cellStyle name="Normal 18 9" xfId="421" xr:uid="{E88C8D00-A684-4B81-9E3E-D25CD466C39D}"/>
     <cellStyle name="Normal 19" xfId="285" xr:uid="{F0C31ECC-C139-4351-BA1F-5C2CAEB650E8}"/>
@@ -4460,6 +4997,10 @@
     <cellStyle name="Normal 19 18" xfId="652" xr:uid="{CB28CE08-0BD9-4A14-815F-2A1A1949AFB6}"/>
     <cellStyle name="Normal 19 19" xfId="679" xr:uid="{0FDB0091-57EF-46D2-A546-22A560D1DC4D}"/>
     <cellStyle name="Normal 19 2" xfId="303" xr:uid="{313C1CD9-EF59-45B4-AB9B-BCBD812E852F}"/>
+    <cellStyle name="Normal 19 2 2" xfId="2732" xr:uid="{7A4717AE-374B-4D7E-8452-675A18D2C2BB}"/>
+    <cellStyle name="Normal 19 2 3" xfId="2845" xr:uid="{131CD0EF-B3CF-4BCF-B4C0-424A3B44940D}"/>
+    <cellStyle name="Normal 19 2 4" xfId="2960" xr:uid="{7BBD7375-DF81-4139-8852-70C58A1C97B2}"/>
+    <cellStyle name="Normal 19 2 5" xfId="3075" xr:uid="{E2FA4F33-1F7E-429A-BD05-3F45924132AA}"/>
     <cellStyle name="Normal 19 20" xfId="706" xr:uid="{E55A7E61-E7A7-459B-9CE4-9D85CFA0D402}"/>
     <cellStyle name="Normal 19 21" xfId="733" xr:uid="{7A446A96-9468-4BB1-8917-124B0421AF2F}"/>
     <cellStyle name="Normal 19 22" xfId="760" xr:uid="{DBF21CB2-C484-49D1-B4AE-0D504ABF26EE}"/>
@@ -4511,11 +5052,16 @@
     <cellStyle name="Normal 19 64" xfId="2511" xr:uid="{51901CFF-9289-4D93-A0F9-181AA2258AD0}"/>
     <cellStyle name="Normal 19 65" xfId="2566" xr:uid="{5A011BA0-47FF-430C-A91E-9A5AF35EB2F0}"/>
     <cellStyle name="Normal 19 66" xfId="2621" xr:uid="{53DC0A07-674B-4744-A10C-FB1CD3088EAB}"/>
+    <cellStyle name="Normal 19 67" xfId="2677" xr:uid="{C1821A5C-24B2-49FC-8512-4C44869B09BE}"/>
+    <cellStyle name="Normal 19 68" xfId="2790" xr:uid="{70B359CD-2F3D-470F-94EA-009E80A9A671}"/>
+    <cellStyle name="Normal 19 69" xfId="2905" xr:uid="{6AD099A2-6A3E-4674-8678-57D19D43A0C5}"/>
     <cellStyle name="Normal 19 7" xfId="402" xr:uid="{7C70AE42-3659-4E21-B1E7-5A2B14B05D2D}"/>
+    <cellStyle name="Normal 19 70" xfId="3020" xr:uid="{0A2C9D49-1B5A-4B3B-8177-73C4034CF287}"/>
     <cellStyle name="Normal 19 8" xfId="422" xr:uid="{258ACE1C-8C37-43E9-8F9E-504F66369A2C}"/>
     <cellStyle name="Normal 19 9" xfId="443" xr:uid="{AED5C701-AD5D-4D29-BEA5-DC3E31B13CEA}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{C38414E3-CB2A-4D4E-8F45-0EDAF44A04EE}"/>
     <cellStyle name="Normal 2 10" xfId="58" xr:uid="{3CFE6032-8C71-4757-81CF-BC7BD4EDCEC3}"/>
+    <cellStyle name="Normal 2 100" xfId="3003" xr:uid="{1E0D4B34-B182-4479-B9FF-E2AD31E16DFC}"/>
     <cellStyle name="Normal 2 11" xfId="65" xr:uid="{1A4E0379-BAD1-46C4-84C4-3D89633D0D78}"/>
     <cellStyle name="Normal 2 12" xfId="72" xr:uid="{BED1FA71-FA51-484D-8A77-2D4E7B53F09C}"/>
     <cellStyle name="Normal 2 13" xfId="79" xr:uid="{0B0BE76B-92CC-41CE-B278-736F8DA2A6A8}"/>
@@ -4526,6 +5072,10 @@
     <cellStyle name="Normal 2 18" xfId="119" xr:uid="{A4F60C18-5727-4939-99F7-EDF8BF220A48}"/>
     <cellStyle name="Normal 2 19" xfId="127" xr:uid="{4CDBA938-FF61-4A4E-8A31-B3CF0151A1E8}"/>
     <cellStyle name="Normal 2 2" xfId="7" xr:uid="{0AC9A6C0-D26F-4899-B4DB-75E1982CE935}"/>
+    <cellStyle name="Normal 2 2 2" xfId="2715" xr:uid="{DF35F41C-5326-480A-B1B9-C77946F0B803}"/>
+    <cellStyle name="Normal 2 2 3" xfId="2828" xr:uid="{1771077B-CA3E-40FF-93A0-A3A4467DAB6B}"/>
+    <cellStyle name="Normal 2 2 4" xfId="2943" xr:uid="{9E896BD6-E9CA-4C79-832D-E582A9A5F29A}"/>
+    <cellStyle name="Normal 2 2 5" xfId="3058" xr:uid="{CA0EAA2C-6C3B-4978-B356-31AF804B644A}"/>
     <cellStyle name="Normal 2 20" xfId="135" xr:uid="{4D941A3B-78D7-41AC-BF2E-F2BDF7E165E2}"/>
     <cellStyle name="Normal 2 21" xfId="143" xr:uid="{C8541C4A-148D-4AA6-987A-E2E2C235C512}"/>
     <cellStyle name="Normal 2 22" xfId="151" xr:uid="{E8B9C67A-D8C8-4C43-A383-8E41400D2F6A}"/>
@@ -4610,6 +5160,9 @@
     <cellStyle name="Normal 2 94" xfId="2494" xr:uid="{77880587-4369-48CD-94BD-0D5381A5EBB1}"/>
     <cellStyle name="Normal 2 95" xfId="2549" xr:uid="{2F6F4E85-5134-450A-A2AE-91D593659995}"/>
     <cellStyle name="Normal 2 96" xfId="2604" xr:uid="{E68285F5-DDC2-443D-B366-0D48402A7849}"/>
+    <cellStyle name="Normal 2 97" xfId="2660" xr:uid="{0C5E9D3A-A91D-4C5D-9199-E7301D8F6E48}"/>
+    <cellStyle name="Normal 2 98" xfId="2773" xr:uid="{4A5E3067-BE1E-498F-B40B-05F88DE5B2F6}"/>
+    <cellStyle name="Normal 2 99" xfId="2888" xr:uid="{ECBE7BA2-D092-403F-A9FD-349962F0939F}"/>
     <cellStyle name="Normal 20" xfId="304" xr:uid="{46E9EC2A-F4CD-4474-8F1F-128DC22F7FEE}"/>
     <cellStyle name="Normal 20 10" xfId="487" xr:uid="{7BB6CDCC-D9F1-4CB0-A7DC-4C2435A3C632}"/>
     <cellStyle name="Normal 20 11" xfId="509" xr:uid="{BC3D68B8-B4B0-466B-88F8-0FB74407A0D0}"/>
@@ -4622,6 +5175,10 @@
     <cellStyle name="Normal 20 18" xfId="680" xr:uid="{AC4B4DEF-EB73-4CED-AEA7-291D273CAB51}"/>
     <cellStyle name="Normal 20 19" xfId="707" xr:uid="{DF8A02F6-E8B2-476A-8651-5E0AA94BA58B}"/>
     <cellStyle name="Normal 20 2" xfId="323" xr:uid="{2AE3D3B9-A114-4910-B515-447D827AC0C1}"/>
+    <cellStyle name="Normal 20 2 2" xfId="2733" xr:uid="{C31CF785-1C81-4750-8950-0817ACC7DA17}"/>
+    <cellStyle name="Normal 20 2 3" xfId="2846" xr:uid="{6B125987-BB52-4BA3-8714-5B0F5A94225E}"/>
+    <cellStyle name="Normal 20 2 4" xfId="2961" xr:uid="{AEB08130-7A80-4751-BDDE-B00DDC94E8D2}"/>
+    <cellStyle name="Normal 20 2 5" xfId="3076" xr:uid="{2A766B0E-1DE3-4B0A-AD70-7AD3F04452AD}"/>
     <cellStyle name="Normal 20 20" xfId="734" xr:uid="{9E400970-F340-41D5-A4F0-14B8875594D1}"/>
     <cellStyle name="Normal 20 21" xfId="761" xr:uid="{20BD6C2D-DF46-4B1D-80BD-8CF07E8DA94E}"/>
     <cellStyle name="Normal 20 22" xfId="788" xr:uid="{313BE505-C91B-4182-97A7-F5C890B7C9A6}"/>
@@ -4672,6 +5229,10 @@
     <cellStyle name="Normal 20 63" xfId="2512" xr:uid="{45A6C02A-AC02-4447-A552-6858B635C221}"/>
     <cellStyle name="Normal 20 64" xfId="2567" xr:uid="{4960C961-6572-4D98-9C70-EC5764237F0F}"/>
     <cellStyle name="Normal 20 65" xfId="2622" xr:uid="{5E2CFFB7-5EAD-4F04-8726-7E5FDEBB8548}"/>
+    <cellStyle name="Normal 20 66" xfId="2678" xr:uid="{8B114C5D-ECFD-4DEA-AD82-D87414559E6D}"/>
+    <cellStyle name="Normal 20 67" xfId="2791" xr:uid="{86FB79A3-0A84-4667-A73D-FB4869458D48}"/>
+    <cellStyle name="Normal 20 68" xfId="2906" xr:uid="{77AA8F7A-AEFE-45B2-8A40-917D42B1ADAD}"/>
+    <cellStyle name="Normal 20 69" xfId="3021" xr:uid="{650B7AC1-57F5-486D-BBCE-82167E60FEF0}"/>
     <cellStyle name="Normal 20 7" xfId="423" xr:uid="{086835B6-4345-4031-B11A-51B0C72CE8BF}"/>
     <cellStyle name="Normal 20 8" xfId="444" xr:uid="{AB563AA1-827B-4C23-99CE-81D8ACA1B263}"/>
     <cellStyle name="Normal 20 9" xfId="465" xr:uid="{8753642A-194D-4639-8E76-06C881170BFA}"/>
@@ -4687,6 +5248,10 @@
     <cellStyle name="Normal 21 18" xfId="708" xr:uid="{294C15D8-2891-4F35-8A2D-56C5A7E8E297}"/>
     <cellStyle name="Normal 21 19" xfId="735" xr:uid="{7F9236BD-8C5B-457B-B9C3-8E17647FFB7E}"/>
     <cellStyle name="Normal 21 2" xfId="344" xr:uid="{6FC6C4CF-76EB-4782-AADC-58E5DA41C718}"/>
+    <cellStyle name="Normal 21 2 2" xfId="2734" xr:uid="{B722E6BB-8707-47CA-8CBF-D805729A8601}"/>
+    <cellStyle name="Normal 21 2 3" xfId="2847" xr:uid="{AD59BB86-F709-4441-A6A8-0B728A6828EE}"/>
+    <cellStyle name="Normal 21 2 4" xfId="2962" xr:uid="{1209615C-26EF-49A7-8CCA-7E0B463787CC}"/>
+    <cellStyle name="Normal 21 2 5" xfId="3077" xr:uid="{7F903425-B93C-42EE-BB2A-71CFCAC9D222}"/>
     <cellStyle name="Normal 21 20" xfId="762" xr:uid="{8C275080-4934-459C-BC04-E7C117B2098C}"/>
     <cellStyle name="Normal 21 21" xfId="789" xr:uid="{303C5D0F-4B1B-45CD-BB29-C24C849E8E1B}"/>
     <cellStyle name="Normal 21 22" xfId="816" xr:uid="{20953B75-D116-467E-B53F-9AEF0B412C33}"/>
@@ -4736,6 +5301,10 @@
     <cellStyle name="Normal 21 62" xfId="2513" xr:uid="{73DE3A93-0B21-4690-9E41-0B93A8F62024}"/>
     <cellStyle name="Normal 21 63" xfId="2568" xr:uid="{4F7E2053-8815-4594-868A-2A89B2ABC360}"/>
     <cellStyle name="Normal 21 64" xfId="2623" xr:uid="{450C0F4B-1CFC-4ED9-944C-8E7EA9C3369D}"/>
+    <cellStyle name="Normal 21 65" xfId="2679" xr:uid="{32D3B287-53CE-4ED8-A0C9-D887BFDE8B9E}"/>
+    <cellStyle name="Normal 21 66" xfId="2792" xr:uid="{59B6B4E6-081B-4AB6-B35D-47509ADF993B}"/>
+    <cellStyle name="Normal 21 67" xfId="2907" xr:uid="{BCD688FF-D2C2-4858-901A-41BEB37A76B3}"/>
+    <cellStyle name="Normal 21 68" xfId="3022" xr:uid="{7F7FD6DB-D87E-4A0C-83C5-41FFF5EA8FC2}"/>
     <cellStyle name="Normal 21 7" xfId="445" xr:uid="{1C2BB24F-B439-48A3-AEEA-D7AB69CCFDC1}"/>
     <cellStyle name="Normal 21 8" xfId="466" xr:uid="{5E3619D4-D275-4EB0-A165-F875F480DB0E}"/>
     <cellStyle name="Normal 21 9" xfId="488" xr:uid="{B9BF371B-ACB6-4682-B3CB-DE98962B0D2B}"/>
@@ -4751,6 +5320,10 @@
     <cellStyle name="Normal 22 18" xfId="844" xr:uid="{E504B1D5-4C72-4DC2-9759-4B12A7E26A4C}"/>
     <cellStyle name="Normal 22 19" xfId="872" xr:uid="{DED9C921-729C-43E6-BF3E-CD3EA30F16D6}"/>
     <cellStyle name="Normal 22 2" xfId="446" xr:uid="{558AB8D8-F5AA-42C2-BC45-77F36FDC90E6}"/>
+    <cellStyle name="Normal 22 2 2" xfId="2735" xr:uid="{F0E71E6A-823A-4BA3-9E7D-A7F0972C1392}"/>
+    <cellStyle name="Normal 22 2 3" xfId="2848" xr:uid="{C7D0678B-348E-4171-81C3-977BCFB05444}"/>
+    <cellStyle name="Normal 22 2 4" xfId="2963" xr:uid="{5F0674EC-BB51-4168-8546-B6660F47B184}"/>
+    <cellStyle name="Normal 22 2 5" xfId="3078" xr:uid="{4309940F-CBF3-4AF4-AEE6-0A11EBF78E87}"/>
     <cellStyle name="Normal 22 20" xfId="900" xr:uid="{1078AF6C-9318-457B-AD9C-5C775E61924D}"/>
     <cellStyle name="Normal 22 21" xfId="929" xr:uid="{BE9E7ED9-2F14-49DC-A08D-5F554C1BD658}"/>
     <cellStyle name="Normal 22 22" xfId="958" xr:uid="{97C73FB3-1C4E-44A9-BF53-7489E0FD081B}"/>
@@ -4795,6 +5368,10 @@
     <cellStyle name="Normal 22 58" xfId="2569" xr:uid="{2BA44A11-0904-4BC4-BAE1-C39622B27FBB}"/>
     <cellStyle name="Normal 22 59" xfId="2624" xr:uid="{E3DC98DA-C070-41FE-9005-F32402B04C50}"/>
     <cellStyle name="Normal 22 6" xfId="533" xr:uid="{6D06BD98-20DD-45B0-8C60-88A9912CEF28}"/>
+    <cellStyle name="Normal 22 60" xfId="2680" xr:uid="{E4CB71D9-D8F0-4DAB-AADB-88EFF8B74674}"/>
+    <cellStyle name="Normal 22 61" xfId="2793" xr:uid="{77C91503-92BC-44C0-B209-8EFBC52A0AA8}"/>
+    <cellStyle name="Normal 22 62" xfId="2908" xr:uid="{6AAC8CF9-988A-4219-B559-46D4FDA5444F}"/>
+    <cellStyle name="Normal 22 63" xfId="3023" xr:uid="{9266AB89-BD18-4701-8058-FB5434EA113C}"/>
     <cellStyle name="Normal 22 7" xfId="556" xr:uid="{C4538170-DB37-479E-96ED-6FC8842F1A26}"/>
     <cellStyle name="Normal 22 8" xfId="579" xr:uid="{E69F69A2-D4D9-4555-B390-12901B969277}"/>
     <cellStyle name="Normal 22 9" xfId="603" xr:uid="{CC4AE523-7C4D-49B1-8390-4029AC553B3C}"/>
@@ -4810,6 +5387,10 @@
     <cellStyle name="Normal 23 18" xfId="901" xr:uid="{9A8C8E44-8CD5-4D3E-994F-90E856374CFD}"/>
     <cellStyle name="Normal 23 19" xfId="930" xr:uid="{54C1AF46-17FC-48D1-AE0D-BACE39FFB3C3}"/>
     <cellStyle name="Normal 23 2" xfId="490" xr:uid="{AF9C69B7-4D53-4082-98D8-CC3986A652BC}"/>
+    <cellStyle name="Normal 23 2 2" xfId="2736" xr:uid="{1FD72854-FAAE-48D9-8B8A-19594C9A26F0}"/>
+    <cellStyle name="Normal 23 2 3" xfId="2849" xr:uid="{3DC48B8C-B594-47C2-829B-030C21893C0E}"/>
+    <cellStyle name="Normal 23 2 4" xfId="2964" xr:uid="{D9489604-E9B4-4E32-90FF-317939EA31F1}"/>
+    <cellStyle name="Normal 23 2 5" xfId="3079" xr:uid="{D89B4D91-7E27-4147-B143-26481F3A31AD}"/>
     <cellStyle name="Normal 23 20" xfId="959" xr:uid="{9AAF16DE-3F39-4C5F-92F4-F7AD36E6AD49}"/>
     <cellStyle name="Normal 23 21" xfId="988" xr:uid="{2DDE8DE3-03B7-4AB8-91D3-36B223C80C73}"/>
     <cellStyle name="Normal 23 22" xfId="1018" xr:uid="{D5906C40-FCC5-47EC-BF5A-8B2579BC2E54}"/>
@@ -4851,7 +5432,11 @@
     <cellStyle name="Normal 23 55" xfId="2515" xr:uid="{7ABA03C1-736E-4214-B8AD-51A3A1E8A334}"/>
     <cellStyle name="Normal 23 56" xfId="2570" xr:uid="{3B7F3BE9-E1D7-4448-AEC2-CCB93619DD8D}"/>
     <cellStyle name="Normal 23 57" xfId="2625" xr:uid="{3C0C10A5-14DE-49C2-BD4E-FFA26EF15C55}"/>
+    <cellStyle name="Normal 23 58" xfId="2681" xr:uid="{8F968851-DCC1-4020-8B12-ECC8FB6BF1AD}"/>
+    <cellStyle name="Normal 23 59" xfId="2794" xr:uid="{18BD1B0C-500C-47DC-A27B-1C674E125663}"/>
     <cellStyle name="Normal 23 6" xfId="580" xr:uid="{AAB043AD-CE0D-40DF-9A63-8A4C5A6D4F58}"/>
+    <cellStyle name="Normal 23 60" xfId="2909" xr:uid="{92ADBC8C-4940-4326-90A2-D2DE01F9BAD9}"/>
+    <cellStyle name="Normal 23 61" xfId="3024" xr:uid="{D9EB5FFB-DE9B-4F05-98D7-BF6C3A98783C}"/>
     <cellStyle name="Normal 23 7" xfId="604" xr:uid="{34A3DB58-17AE-4BF6-9728-A09FFBA397E1}"/>
     <cellStyle name="Normal 23 8" xfId="629" xr:uid="{F434F633-2719-4E36-A0A3-945AC33697C3}"/>
     <cellStyle name="Normal 23 9" xfId="656" xr:uid="{A1B737CA-1989-4C15-BCE2-C92CAE075105}"/>
@@ -4867,6 +5452,10 @@
     <cellStyle name="Normal 24 18" xfId="989" xr:uid="{9528573C-AB38-42B4-BA8B-1A0C292AA107}"/>
     <cellStyle name="Normal 24 19" xfId="1019" xr:uid="{997F0AC7-DB4D-40E9-B207-9DE60F744E52}"/>
     <cellStyle name="Normal 24 2" xfId="558" xr:uid="{1853973C-1D62-4023-A0AD-CE47F79DDB51}"/>
+    <cellStyle name="Normal 24 2 2" xfId="2737" xr:uid="{FB851B99-E311-4646-98AE-FCFEDCEA4CC0}"/>
+    <cellStyle name="Normal 24 2 3" xfId="2850" xr:uid="{99FB707D-D3AB-4DD7-A8AB-8C522E38C458}"/>
+    <cellStyle name="Normal 24 2 4" xfId="2965" xr:uid="{CC15D493-8E4C-4EF6-823D-89FAD9832013}"/>
+    <cellStyle name="Normal 24 2 5" xfId="3080" xr:uid="{3D47AECC-5973-4737-A37D-77190FB1CFE3}"/>
     <cellStyle name="Normal 24 20" xfId="1050" xr:uid="{9A04BF62-40B8-455E-9F4B-C28EBBE865E9}"/>
     <cellStyle name="Normal 24 21" xfId="1082" xr:uid="{A03256FF-CC96-4B5E-AB78-FDAE678CB9D0}"/>
     <cellStyle name="Normal 24 22" xfId="1116" xr:uid="{37EF0EA7-2CE0-4F23-9C86-00DB391EFD92}"/>
@@ -4905,6 +5494,10 @@
     <cellStyle name="Normal 24 52" xfId="2516" xr:uid="{A82D1AB8-0B44-471A-A540-AABB5882FA4E}"/>
     <cellStyle name="Normal 24 53" xfId="2571" xr:uid="{E8BE0504-92AD-475D-8C93-438A762CC47D}"/>
     <cellStyle name="Normal 24 54" xfId="2626" xr:uid="{B6D35BBD-1EE9-46B4-958C-52F77CD36B82}"/>
+    <cellStyle name="Normal 24 55" xfId="2682" xr:uid="{F530836E-E329-4E2F-B596-68A059D9F1AC}"/>
+    <cellStyle name="Normal 24 56" xfId="2795" xr:uid="{8E322DA5-A283-4024-9EA4-645B0579445D}"/>
+    <cellStyle name="Normal 24 57" xfId="2910" xr:uid="{66A51D7F-4C3E-4002-9BA6-8FC5040AF81B}"/>
+    <cellStyle name="Normal 24 58" xfId="3025" xr:uid="{4B1E4086-C0F5-491E-B7D2-4B8BE55F0645}"/>
     <cellStyle name="Normal 24 6" xfId="657" xr:uid="{32CD1B47-986E-462F-9668-4C8456D8C1B2}"/>
     <cellStyle name="Normal 24 7" xfId="684" xr:uid="{4CA8DE0A-B4AD-4241-8614-A270B05E4B04}"/>
     <cellStyle name="Normal 24 8" xfId="711" xr:uid="{C4B81C6D-EA33-4229-A72E-E576757A69AA}"/>
@@ -4921,6 +5514,10 @@
     <cellStyle name="Normal 25 18" xfId="1051" xr:uid="{8449D374-B7A6-43BC-B1E7-5B351F0D4FBA}"/>
     <cellStyle name="Normal 25 19" xfId="1083" xr:uid="{9985FC9F-544B-4CBB-8808-D45C4EA35321}"/>
     <cellStyle name="Normal 25 2" xfId="606" xr:uid="{E7CEE723-8CBA-4F5D-A5B9-A0387D58B6AF}"/>
+    <cellStyle name="Normal 25 2 2" xfId="2738" xr:uid="{02A38A12-3BC0-4CA1-BAFC-557111AF3B63}"/>
+    <cellStyle name="Normal 25 2 3" xfId="2851" xr:uid="{C6A382DF-F4B4-4B6D-A975-9241604BB33C}"/>
+    <cellStyle name="Normal 25 2 4" xfId="2966" xr:uid="{49383454-7A72-484D-9733-4896CEB076B5}"/>
+    <cellStyle name="Normal 25 2 5" xfId="3081" xr:uid="{7DA95A6B-70AD-4DD7-9D14-B57EE1AD5395}"/>
     <cellStyle name="Normal 25 20" xfId="1117" xr:uid="{70B37F3A-4D8F-4EAC-B08C-161BE181923B}"/>
     <cellStyle name="Normal 25 21" xfId="1152" xr:uid="{5E752404-B4B6-4FAB-BC7D-82E51E72E1FC}"/>
     <cellStyle name="Normal 25 22" xfId="1189" xr:uid="{48358E42-9351-4CCB-B944-478741ADC8E7}"/>
@@ -4957,6 +5554,10 @@
     <cellStyle name="Normal 25 50" xfId="2517" xr:uid="{8F0BD65E-6C64-4635-922D-F44DF59A8FC7}"/>
     <cellStyle name="Normal 25 51" xfId="2572" xr:uid="{ED64F920-17F3-4E8C-8DF1-604C81AE3D9E}"/>
     <cellStyle name="Normal 25 52" xfId="2627" xr:uid="{420ADA81-9315-4993-9997-BF3BD07ADBE4}"/>
+    <cellStyle name="Normal 25 53" xfId="2683" xr:uid="{6341AC78-3BB2-4473-9866-3D0D9DE3B2FA}"/>
+    <cellStyle name="Normal 25 54" xfId="2796" xr:uid="{41EA7093-68D1-4B03-941A-5CF858E3C8A4}"/>
+    <cellStyle name="Normal 25 55" xfId="2911" xr:uid="{9546D54D-61EF-4E03-BAA1-DDFA1340F4F6}"/>
+    <cellStyle name="Normal 25 56" xfId="3026" xr:uid="{BF9B1745-A370-4590-B46B-69C53DE8C7E1}"/>
     <cellStyle name="Normal 25 6" xfId="712" xr:uid="{829BB221-C705-476D-A467-70C6FED9B8ED}"/>
     <cellStyle name="Normal 25 7" xfId="739" xr:uid="{B64EF1EB-9F92-4BEC-BEAD-2E23DE7EC71A}"/>
     <cellStyle name="Normal 25 8" xfId="766" xr:uid="{88AEE39D-1A12-41B0-AF55-E0D06D5E7B20}"/>
@@ -4973,6 +5574,10 @@
     <cellStyle name="Normal 26 18" xfId="1084" xr:uid="{9F06768A-2864-404D-94DE-53542AE8E6CD}"/>
     <cellStyle name="Normal 26 19" xfId="1118" xr:uid="{403EF579-6876-4604-B6E0-2F43F3859557}"/>
     <cellStyle name="Normal 26 2" xfId="632" xr:uid="{A584D364-7DB3-4806-998B-69D069EBCC9A}"/>
+    <cellStyle name="Normal 26 2 2" xfId="2739" xr:uid="{B52823FF-86F9-40E9-83C8-2F2013AA28FE}"/>
+    <cellStyle name="Normal 26 2 3" xfId="2852" xr:uid="{FB05A8FF-FACE-4246-A424-DB7670723B61}"/>
+    <cellStyle name="Normal 26 2 4" xfId="2967" xr:uid="{5D434ED8-C692-4F94-A116-95D7557EC96A}"/>
+    <cellStyle name="Normal 26 2 5" xfId="3082" xr:uid="{55FA7004-DBAB-44F5-BD51-1B307C815DBC}"/>
     <cellStyle name="Normal 26 20" xfId="1153" xr:uid="{825FD13E-22F2-414F-AC51-9B1DD1272442}"/>
     <cellStyle name="Normal 26 21" xfId="1190" xr:uid="{FDA097AA-B594-409E-91A8-4D7BCB6A37EB}"/>
     <cellStyle name="Normal 26 22" xfId="1229" xr:uid="{C416D535-B719-4700-94FB-F89F5C0E6512}"/>
@@ -5008,6 +5613,10 @@
     <cellStyle name="Normal 26 5" xfId="713" xr:uid="{D344AFEE-A03D-4DA9-BD02-29F7ABE09946}"/>
     <cellStyle name="Normal 26 50" xfId="2573" xr:uid="{B80F0946-702C-49C9-9827-5D854C2F8B97}"/>
     <cellStyle name="Normal 26 51" xfId="2628" xr:uid="{7480B03D-F904-42F4-9091-2815BE7B1725}"/>
+    <cellStyle name="Normal 26 52" xfId="2684" xr:uid="{EAE2BEB6-20B8-4798-8482-CC4F8F01AC6B}"/>
+    <cellStyle name="Normal 26 53" xfId="2797" xr:uid="{1A99664D-D89C-4077-BAE9-45C37AD3E941}"/>
+    <cellStyle name="Normal 26 54" xfId="2912" xr:uid="{AD0646CB-268D-4D10-A121-EBEE5ED70976}"/>
+    <cellStyle name="Normal 26 55" xfId="3027" xr:uid="{0AAA9E2E-37CF-4FC8-8AC8-BBCCB2823965}"/>
     <cellStyle name="Normal 26 6" xfId="740" xr:uid="{55099FE6-EF4A-4F80-A025-FC0681D4C856}"/>
     <cellStyle name="Normal 26 7" xfId="767" xr:uid="{E0D5D6CA-66CD-46E6-81F6-E5EF5A9B9699}"/>
     <cellStyle name="Normal 26 8" xfId="794" xr:uid="{8CA05745-9C12-4B23-8366-0110D6A2E67D}"/>
@@ -5024,6 +5633,10 @@
     <cellStyle name="Normal 27 18" xfId="1119" xr:uid="{7778DFC2-5E5D-4CAC-B579-86CCABBC6EC5}"/>
     <cellStyle name="Normal 27 19" xfId="1154" xr:uid="{259AE1D3-0C6C-41D8-971A-39472BB6A4F9}"/>
     <cellStyle name="Normal 27 2" xfId="660" xr:uid="{C51ED6B2-824E-43F9-B3ED-612C8F8CA640}"/>
+    <cellStyle name="Normal 27 2 2" xfId="2740" xr:uid="{1D8D88B5-AB2A-4A08-8FA6-71A26CBA7A91}"/>
+    <cellStyle name="Normal 27 2 3" xfId="2853" xr:uid="{3F4FD3E9-6A38-4993-B9FD-0FED5D27302C}"/>
+    <cellStyle name="Normal 27 2 4" xfId="2968" xr:uid="{E7CBEA15-8694-4BFA-B081-E821E4D23983}"/>
+    <cellStyle name="Normal 27 2 5" xfId="3083" xr:uid="{01326A2D-5906-44FE-BCA6-FC93C6388843}"/>
     <cellStyle name="Normal 27 20" xfId="1191" xr:uid="{6A3E9732-FF7C-424F-A537-AB914EB049FD}"/>
     <cellStyle name="Normal 27 21" xfId="1230" xr:uid="{4E944A0E-81F3-4500-A56A-BD32980D0557}"/>
     <cellStyle name="Normal 27 22" xfId="1270" xr:uid="{A12EB9B1-5D02-4308-B099-8CD42F299FFE}"/>
@@ -5058,6 +5671,10 @@
     <cellStyle name="Normal 27 49" xfId="2574" xr:uid="{E9404426-EF7E-45ED-B50A-733C111446F7}"/>
     <cellStyle name="Normal 27 5" xfId="741" xr:uid="{73F13B32-388D-4D89-9F01-E89AA863010F}"/>
     <cellStyle name="Normal 27 50" xfId="2629" xr:uid="{B2D9E922-308D-4610-B916-15EA96B9CF94}"/>
+    <cellStyle name="Normal 27 51" xfId="2685" xr:uid="{20411CDB-A7D8-4DAA-9634-D99CC5BD6CCD}"/>
+    <cellStyle name="Normal 27 52" xfId="2798" xr:uid="{A00C472A-06A3-41AE-AAFD-07FD813DAAD6}"/>
+    <cellStyle name="Normal 27 53" xfId="2913" xr:uid="{D61F03FE-2BB3-4ABC-8FFF-4D3D7F456CDA}"/>
+    <cellStyle name="Normal 27 54" xfId="3028" xr:uid="{0C68D4E2-6670-48D6-841D-118D120D31B9}"/>
     <cellStyle name="Normal 27 6" xfId="768" xr:uid="{C1FF1113-E4F1-409B-9342-01929F68ADCD}"/>
     <cellStyle name="Normal 27 7" xfId="795" xr:uid="{637C3645-B9B7-4559-9CFF-F3A6B8FF3C81}"/>
     <cellStyle name="Normal 27 8" xfId="822" xr:uid="{10EAD9CA-D6B3-4A76-91D8-4478130AB4E2}"/>
@@ -5074,6 +5691,10 @@
     <cellStyle name="Normal 28 18" xfId="1120" xr:uid="{2FE516CB-AA54-4357-BEAB-D5FE5BD951A1}"/>
     <cellStyle name="Normal 28 19" xfId="1155" xr:uid="{CCD28B53-E6F8-45FE-965E-AC1C8F68E5E2}"/>
     <cellStyle name="Normal 28 2" xfId="661" xr:uid="{57A94818-7A0C-48CE-A5E2-E690C4A53230}"/>
+    <cellStyle name="Normal 28 2 2" xfId="2741" xr:uid="{A225BE67-BADD-464E-BD9E-CEC7243E552C}"/>
+    <cellStyle name="Normal 28 2 3" xfId="2854" xr:uid="{DDFB9F25-7F35-466E-AF8C-BFE67D81E3BB}"/>
+    <cellStyle name="Normal 28 2 4" xfId="2969" xr:uid="{41AB104F-7AC5-4689-B452-B243B0A3B828}"/>
+    <cellStyle name="Normal 28 2 5" xfId="3084" xr:uid="{E64E8634-D566-455C-A049-4767DF77FBFC}"/>
     <cellStyle name="Normal 28 20" xfId="1192" xr:uid="{F37F71D1-C700-4480-BA81-3BF48D67C258}"/>
     <cellStyle name="Normal 28 21" xfId="1231" xr:uid="{312FC0C8-4731-44E5-A064-A618105660C2}"/>
     <cellStyle name="Normal 28 22" xfId="1271" xr:uid="{2204AB1B-909F-4DDD-A4DD-453C3350A278}"/>
@@ -5108,6 +5729,10 @@
     <cellStyle name="Normal 28 49" xfId="2575" xr:uid="{ABCA9612-907D-403E-AA90-787CD7FB4435}"/>
     <cellStyle name="Normal 28 5" xfId="742" xr:uid="{0E873815-9144-409F-9560-E3292F714AD5}"/>
     <cellStyle name="Normal 28 50" xfId="2630" xr:uid="{2FF253B9-A898-405E-83D6-E0778B761150}"/>
+    <cellStyle name="Normal 28 51" xfId="2686" xr:uid="{D49BA9DB-F4F8-4B6E-9D18-BE5281382985}"/>
+    <cellStyle name="Normal 28 52" xfId="2799" xr:uid="{CC549EDB-B34F-4FF8-BB74-608555ADE292}"/>
+    <cellStyle name="Normal 28 53" xfId="2914" xr:uid="{23719DB5-AEC3-4A01-8D00-5B56A03B0AFF}"/>
+    <cellStyle name="Normal 28 54" xfId="3029" xr:uid="{72441555-81B2-4C0E-8B2D-8625D7F4E6EB}"/>
     <cellStyle name="Normal 28 6" xfId="769" xr:uid="{E1B9D957-F371-47A0-AEBA-EB4390991517}"/>
     <cellStyle name="Normal 28 7" xfId="796" xr:uid="{CE95D840-1DED-4550-9B45-79BB1A30B661}"/>
     <cellStyle name="Normal 28 8" xfId="823" xr:uid="{75DAFBA6-27A3-47FE-B0FD-AC8663496528}"/>
@@ -5124,6 +5749,10 @@
     <cellStyle name="Normal 29 18" xfId="1440" xr:uid="{A94E8957-9E1B-4C94-9FB1-7C05F6A8C71E}"/>
     <cellStyle name="Normal 29 19" xfId="1484" xr:uid="{0C704CCB-CC42-483A-9370-25FB14740220}"/>
     <cellStyle name="Normal 29 2" xfId="879" xr:uid="{79A6075E-91D7-4C41-B44D-DF6758CB58C6}"/>
+    <cellStyle name="Normal 29 2 2" xfId="2742" xr:uid="{E8246056-E1E3-4E67-BA4D-C267125890D9}"/>
+    <cellStyle name="Normal 29 2 3" xfId="2855" xr:uid="{FAD2ADDF-D9DF-406E-A1B1-0472EB380495}"/>
+    <cellStyle name="Normal 29 2 4" xfId="2970" xr:uid="{674620B2-5E26-4190-8FDC-E37E40CE34CA}"/>
+    <cellStyle name="Normal 29 2 5" xfId="3085" xr:uid="{F6F0EE07-C237-482A-B1F7-C23213E0B81A}"/>
     <cellStyle name="Normal 29 20" xfId="1528" xr:uid="{6B2CC1B7-D9A1-4DB4-A643-F45251EBE48C}"/>
     <cellStyle name="Normal 29 21" xfId="1573" xr:uid="{745435DA-9464-4B29-8AFC-B7F19330BB60}"/>
     <cellStyle name="Normal 29 22" xfId="1617" xr:uid="{1D4817F6-3DDD-4917-938D-8C1B58745AA9}"/>
@@ -5149,6 +5778,10 @@
     <cellStyle name="Normal 29 40" xfId="2521" xr:uid="{7023392D-2709-4943-9C7A-0EA736D62434}"/>
     <cellStyle name="Normal 29 41" xfId="2576" xr:uid="{07E3A54A-6A39-4486-A4EC-C2F0E5CF5933}"/>
     <cellStyle name="Normal 29 42" xfId="2631" xr:uid="{663ACD19-5261-423E-A199-12144B535E20}"/>
+    <cellStyle name="Normal 29 43" xfId="2687" xr:uid="{E9AB5E4A-165D-4985-AB29-D5D3743A73E8}"/>
+    <cellStyle name="Normal 29 44" xfId="2800" xr:uid="{7E731D77-D693-41F6-BF4F-E061CD819F8A}"/>
+    <cellStyle name="Normal 29 45" xfId="2915" xr:uid="{D07AC9FF-0729-47E2-AA99-24799F1DBE28}"/>
+    <cellStyle name="Normal 29 46" xfId="3030" xr:uid="{D6FCD9B6-C6C4-43B9-8D1F-88E7D3B3F455}"/>
     <cellStyle name="Normal 29 5" xfId="965" xr:uid="{E4F2ED17-F04A-4AF1-A706-C14A73357E91}"/>
     <cellStyle name="Normal 29 6" xfId="994" xr:uid="{CAF38D46-8974-47D6-914C-330FB88EC9BB}"/>
     <cellStyle name="Normal 29 7" xfId="1024" xr:uid="{89E0CC64-087C-41A9-B0ED-A634EDD2A24E}"/>
@@ -5156,6 +5789,7 @@
     <cellStyle name="Normal 29 9" xfId="1087" xr:uid="{5EE8F91F-91C7-4176-A465-DCCBC879F43F}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{F50FA18E-7B72-456D-B8E9-6EB089AF9B03}"/>
     <cellStyle name="Normal 3 10" xfId="59" xr:uid="{D1CF1ACF-0DE0-4EF1-ADE7-19241CD0A4BB}"/>
+    <cellStyle name="Normal 3 100" xfId="3004" xr:uid="{1A192B61-B6EC-42D2-9A02-CD9D98DD9B2E}"/>
     <cellStyle name="Normal 3 11" xfId="66" xr:uid="{F07E7733-B7D0-4684-93D0-1BB1777E88C8}"/>
     <cellStyle name="Normal 3 12" xfId="73" xr:uid="{DD3B3D01-4611-4B64-B30F-7CA8C1E6CB19}"/>
     <cellStyle name="Normal 3 13" xfId="80" xr:uid="{51489280-DEDB-4995-B588-0D69213FFC63}"/>
@@ -5166,6 +5800,10 @@
     <cellStyle name="Normal 3 18" xfId="120" xr:uid="{0F6146BD-6815-4187-A222-3ACF8BC4350B}"/>
     <cellStyle name="Normal 3 19" xfId="128" xr:uid="{DDC3A0AF-6E23-43BB-8BD1-7FB710DBC75C}"/>
     <cellStyle name="Normal 3 2" xfId="8" xr:uid="{6151C0A1-5C68-47EC-9DAA-BA7F89F86D59}"/>
+    <cellStyle name="Normal 3 2 2" xfId="2716" xr:uid="{9C3A5FEE-B393-4F7D-BE67-C37511E77F14}"/>
+    <cellStyle name="Normal 3 2 3" xfId="2829" xr:uid="{B8481356-004B-4E93-BB2A-AAFA2A60668D}"/>
+    <cellStyle name="Normal 3 2 4" xfId="2944" xr:uid="{E2B5AF24-F2AC-4480-84D3-22A45EC0D6A8}"/>
+    <cellStyle name="Normal 3 2 5" xfId="3059" xr:uid="{B290F7B9-4318-4F18-97C7-F81EDB0B5C7B}"/>
     <cellStyle name="Normal 3 20" xfId="136" xr:uid="{0B1825F2-3C66-42DA-BB7D-021AEBDF6CC8}"/>
     <cellStyle name="Normal 3 21" xfId="144" xr:uid="{DDCB93E7-0420-4CF9-A693-B7B0A0E7C227}"/>
     <cellStyle name="Normal 3 22" xfId="152" xr:uid="{7C849DE9-914D-4AA4-8FD5-B428FA7A93A6}"/>
@@ -5250,6 +5888,9 @@
     <cellStyle name="Normal 3 94" xfId="2495" xr:uid="{861C0826-6EB8-4CDD-9449-B83DC31A913A}"/>
     <cellStyle name="Normal 3 95" xfId="2550" xr:uid="{58AA66E0-C1C7-4D30-B1E6-BF3992BDC85F}"/>
     <cellStyle name="Normal 3 96" xfId="2605" xr:uid="{528AA4E6-A7FF-48A6-9B0F-75BD4AA62468}"/>
+    <cellStyle name="Normal 3 97" xfId="2661" xr:uid="{270F3A86-2742-4B03-B327-748392D38918}"/>
+    <cellStyle name="Normal 3 98" xfId="2774" xr:uid="{BBC636C5-6D08-4B69-BEE5-48E4B748CEB3}"/>
+    <cellStyle name="Normal 3 99" xfId="2889" xr:uid="{00C5BA02-2FA1-44CF-86D6-EC062132E6DA}"/>
     <cellStyle name="Normal 30" xfId="908" xr:uid="{29060677-DDC7-44E4-9DB7-833832E2C2EF}"/>
     <cellStyle name="Normal 30 10" xfId="1194" xr:uid="{87CB8D63-90E2-489B-B2F1-CACD93DC026A}"/>
     <cellStyle name="Normal 30 11" xfId="1233" xr:uid="{BE9D1AC2-FA84-447C-980B-7C0F52813116}"/>
@@ -5262,6 +5903,10 @@
     <cellStyle name="Normal 30 18" xfId="1529" xr:uid="{B39C4654-DF2F-43D1-9D00-464168056BB5}"/>
     <cellStyle name="Normal 30 19" xfId="1574" xr:uid="{9F8AB992-BA25-48F7-A9A4-DAF5E2C40A28}"/>
     <cellStyle name="Normal 30 2" xfId="937" xr:uid="{041C6B12-60CB-41F4-83B3-75EFE68E9D81}"/>
+    <cellStyle name="Normal 30 2 2" xfId="2743" xr:uid="{2FF40563-0F4A-4DA0-A675-BA889998DD27}"/>
+    <cellStyle name="Normal 30 2 3" xfId="2856" xr:uid="{4500E837-418D-4BF6-AEF9-BE4825AC88DF}"/>
+    <cellStyle name="Normal 30 2 4" xfId="2971" xr:uid="{14EC1241-7A26-4C66-A446-894B9F122D8C}"/>
+    <cellStyle name="Normal 30 2 5" xfId="3086" xr:uid="{F84E2D77-2396-4DC1-80E4-66181385C466}"/>
     <cellStyle name="Normal 30 20" xfId="1618" xr:uid="{72D2A9D0-EAAF-4EE5-B66F-0D24EF30CCEA}"/>
     <cellStyle name="Normal 30 21" xfId="1662" xr:uid="{8E5EC0BF-3053-42C4-881B-76D2E7D68B40}"/>
     <cellStyle name="Normal 30 22" xfId="1706" xr:uid="{9A5E4208-916D-4859-A4CF-380FA4175BF7}"/>
@@ -5285,6 +5930,10 @@
     <cellStyle name="Normal 30 39" xfId="2577" xr:uid="{840D2EFC-978A-4345-92A2-B6E33B690D9A}"/>
     <cellStyle name="Normal 30 4" xfId="995" xr:uid="{8A471471-CC73-4677-8055-BF9B78704B15}"/>
     <cellStyle name="Normal 30 40" xfId="2632" xr:uid="{C6040655-0458-4CAF-B497-74DC85D9610D}"/>
+    <cellStyle name="Normal 30 41" xfId="2688" xr:uid="{EB1B5120-6F0F-4B1E-B16B-48F9EECBAA01}"/>
+    <cellStyle name="Normal 30 42" xfId="2801" xr:uid="{9EDE9EBF-F290-4512-B680-2D2EE20E203E}"/>
+    <cellStyle name="Normal 30 43" xfId="2916" xr:uid="{CE1D8E98-6C75-4566-9A85-6D722F2B9AD7}"/>
+    <cellStyle name="Normal 30 44" xfId="3031" xr:uid="{EA673834-25BB-4183-BB3D-92B34890278A}"/>
     <cellStyle name="Normal 30 5" xfId="1025" xr:uid="{8A88A566-55ED-4197-B3EC-34A2D6F4693C}"/>
     <cellStyle name="Normal 30 6" xfId="1056" xr:uid="{C7E13848-0B37-42F9-92EF-9D5A7F8289AC}"/>
     <cellStyle name="Normal 30 7" xfId="1088" xr:uid="{A17CA1F5-FE5F-4F1B-89F7-FE42660C5DC5}"/>
@@ -5302,6 +5951,10 @@
     <cellStyle name="Normal 31 18" xfId="1663" xr:uid="{00113A4E-98C9-49DD-9ECE-483407D32462}"/>
     <cellStyle name="Normal 31 19" xfId="1707" xr:uid="{AA1C5ADB-A5D9-4CAF-95AD-ECF60D2F3C79}"/>
     <cellStyle name="Normal 31 2" xfId="1026" xr:uid="{84B1F38F-096D-4E79-9E60-9ED4608D4714}"/>
+    <cellStyle name="Normal 31 2 2" xfId="2744" xr:uid="{AE5481C4-B662-4A9F-AD22-1B971BE245B7}"/>
+    <cellStyle name="Normal 31 2 3" xfId="2857" xr:uid="{94AD4ADC-CA41-4541-B88C-73414F34AACB}"/>
+    <cellStyle name="Normal 31 2 4" xfId="2972" xr:uid="{E50BBFF7-EDBE-4A30-81AB-975BF1439782}"/>
+    <cellStyle name="Normal 31 2 5" xfId="3087" xr:uid="{20DAA9E0-E862-4AA7-BE9E-EFA008640289}"/>
     <cellStyle name="Normal 31 20" xfId="1753" xr:uid="{7FC27BDF-534E-410C-AA0F-3B27CEA70ECA}"/>
     <cellStyle name="Normal 31 21" xfId="1797" xr:uid="{E2BAF1F5-540B-4B19-A359-DE8E3716A65F}"/>
     <cellStyle name="Normal 31 22" xfId="1843" xr:uid="{03A79503-D2A9-437F-BA02-E0BC1B95CD24}"/>
@@ -5321,7 +5974,11 @@
     <cellStyle name="Normal 31 35" xfId="2523" xr:uid="{41E38385-1124-44A7-8B1C-4EA87E2C2B69}"/>
     <cellStyle name="Normal 31 36" xfId="2578" xr:uid="{1BE42E08-24D8-41AD-A0A9-C39492ADD2DB}"/>
     <cellStyle name="Normal 31 37" xfId="2633" xr:uid="{B637D5AB-C4A9-4219-96D5-3677ECA6B10C}"/>
+    <cellStyle name="Normal 31 38" xfId="2689" xr:uid="{A27DB3EA-AB9A-4E8E-AD4B-F50C5871BDCA}"/>
+    <cellStyle name="Normal 31 39" xfId="2802" xr:uid="{177B83A4-10F8-4FBA-9DA6-12FF3F30FA6B}"/>
     <cellStyle name="Normal 31 4" xfId="1089" xr:uid="{115B4DBC-0A4B-43C2-8D38-B8E1346CA496}"/>
+    <cellStyle name="Normal 31 40" xfId="2917" xr:uid="{78C1A03C-5BD1-4EAB-8D3B-71EECE150E54}"/>
+    <cellStyle name="Normal 31 41" xfId="3032" xr:uid="{6DB55DF1-E58F-4353-86E9-39A5EBF072ED}"/>
     <cellStyle name="Normal 31 5" xfId="1123" xr:uid="{17785C55-2ED2-45EA-9422-1590CD144DCC}"/>
     <cellStyle name="Normal 31 6" xfId="1158" xr:uid="{5257BC80-708E-436F-B0A2-DE856F2C5DBA}"/>
     <cellStyle name="Normal 31 7" xfId="1195" xr:uid="{AF1E70AB-7FDE-4D6D-BA8B-CE7025620021}"/>
@@ -5339,6 +5996,10 @@
     <cellStyle name="Normal 32 18" xfId="1708" xr:uid="{B1147C14-8DB6-4A10-B59A-98A1B11F9F67}"/>
     <cellStyle name="Normal 32 19" xfId="1754" xr:uid="{4EBD2284-52BF-48D9-A812-B0C405726096}"/>
     <cellStyle name="Normal 32 2" xfId="1058" xr:uid="{650534B7-0F52-424E-A310-FEA20A034F13}"/>
+    <cellStyle name="Normal 32 2 2" xfId="2745" xr:uid="{9BEA67B9-08BB-41EA-B46C-059BC3996582}"/>
+    <cellStyle name="Normal 32 2 3" xfId="2858" xr:uid="{89BF775F-3C9B-41D0-875A-6E4213920B1E}"/>
+    <cellStyle name="Normal 32 2 4" xfId="2973" xr:uid="{8A6F80B4-A77A-43FF-8674-32EC388445DF}"/>
+    <cellStyle name="Normal 32 2 5" xfId="3088" xr:uid="{D2061E9C-381E-46B8-BD9A-71AE4FC309A9}"/>
     <cellStyle name="Normal 32 20" xfId="1798" xr:uid="{DCEF45B3-4CB0-48C2-80F2-0AC6ACB45618}"/>
     <cellStyle name="Normal 32 21" xfId="1844" xr:uid="{29BE3F56-E8BE-4401-A692-618E5E40FBE1}"/>
     <cellStyle name="Normal 32 22" xfId="1891" xr:uid="{6C745B56-9F6C-4B3D-9F44-6C0F4B129B91}"/>
@@ -5357,7 +6018,11 @@
     <cellStyle name="Normal 32 34" xfId="2524" xr:uid="{47A48D37-3155-4508-BC2A-2C06457875E7}"/>
     <cellStyle name="Normal 32 35" xfId="2579" xr:uid="{2AA15E46-370C-43A3-8935-26F782454E98}"/>
     <cellStyle name="Normal 32 36" xfId="2634" xr:uid="{80852F55-B1DC-4B2A-9E96-56F6F94B8D47}"/>
+    <cellStyle name="Normal 32 37" xfId="2690" xr:uid="{6BA0120C-3EE7-4876-9097-EC5949CDB137}"/>
+    <cellStyle name="Normal 32 38" xfId="2803" xr:uid="{DD921701-68DA-46EB-A403-3916CBBDAEF5}"/>
+    <cellStyle name="Normal 32 39" xfId="2918" xr:uid="{DC3CAB8D-82ED-4F05-887D-B9211D511633}"/>
     <cellStyle name="Normal 32 4" xfId="1124" xr:uid="{02CC8B8D-088C-499C-99A0-F631BCDD8473}"/>
+    <cellStyle name="Normal 32 40" xfId="3033" xr:uid="{3A527AC5-DB5C-4A73-AA3A-BA7FA9145DE5}"/>
     <cellStyle name="Normal 32 5" xfId="1159" xr:uid="{D2F78B05-994A-4DB4-A496-D9328EBBE67B}"/>
     <cellStyle name="Normal 32 6" xfId="1196" xr:uid="{2DCB929C-297C-4C53-82E4-0403B87AF2B1}"/>
     <cellStyle name="Normal 32 7" xfId="1235" xr:uid="{DE999473-AD5B-4096-AF2C-28DC856E4A08}"/>
@@ -5375,6 +6040,10 @@
     <cellStyle name="Normal 33 18" xfId="1755" xr:uid="{06C9CEB4-051D-41EC-BCB3-F1780C8941AD}"/>
     <cellStyle name="Normal 33 19" xfId="1799" xr:uid="{3909DBDD-B778-4600-BD15-5CEB8A68CE9F}"/>
     <cellStyle name="Normal 33 2" xfId="1091" xr:uid="{332739C9-E76F-4546-A54B-10E94BEDA71A}"/>
+    <cellStyle name="Normal 33 2 2" xfId="2746" xr:uid="{FFE2FF4D-FA79-44C0-A750-A5A52C8042E1}"/>
+    <cellStyle name="Normal 33 2 3" xfId="2859" xr:uid="{D506A3DE-4C6A-4BD9-9186-69887E9B6562}"/>
+    <cellStyle name="Normal 33 2 4" xfId="2974" xr:uid="{E4786A21-257C-4417-B46A-B7B4103D749F}"/>
+    <cellStyle name="Normal 33 2 5" xfId="3089" xr:uid="{ECAF7763-6BE1-4822-A9EA-D50DBB89D368}"/>
     <cellStyle name="Normal 33 20" xfId="1845" xr:uid="{4389BCC1-1FA6-4167-9FEE-6D970499D837}"/>
     <cellStyle name="Normal 33 21" xfId="1892" xr:uid="{5912A04E-55E9-4472-AD35-22A1973AEDFE}"/>
     <cellStyle name="Normal 33 22" xfId="1940" xr:uid="{BD9BC33B-1EAD-4A2C-9583-58EA15F502ED}"/>
@@ -5392,6 +6061,10 @@
     <cellStyle name="Normal 33 33" xfId="2525" xr:uid="{2FDCE2FA-E5C2-443C-ACB6-88B99FCD9A18}"/>
     <cellStyle name="Normal 33 34" xfId="2580" xr:uid="{5B5E38BD-E6E2-42A6-8E04-7225903D5289}"/>
     <cellStyle name="Normal 33 35" xfId="2635" xr:uid="{47DF46BC-9148-4BE0-AAB3-BA6F6681CBAD}"/>
+    <cellStyle name="Normal 33 36" xfId="2691" xr:uid="{1AC3EA5A-4894-4975-BFD0-4854238EBFE0}"/>
+    <cellStyle name="Normal 33 37" xfId="2804" xr:uid="{D00CC1E7-C0ED-4616-BB12-A2808C0E40DA}"/>
+    <cellStyle name="Normal 33 38" xfId="2919" xr:uid="{CF966835-5D6A-4F52-9CC1-6DABCE20C0C5}"/>
+    <cellStyle name="Normal 33 39" xfId="3034" xr:uid="{D569FC10-533B-4C18-B5E0-A990DB76D17E}"/>
     <cellStyle name="Normal 33 4" xfId="1160" xr:uid="{740C5F2E-4830-4E49-BDD6-9A5138A262C0}"/>
     <cellStyle name="Normal 33 5" xfId="1197" xr:uid="{63D7510F-076E-4560-907D-87441A3EC81D}"/>
     <cellStyle name="Normal 33 6" xfId="1236" xr:uid="{32588593-4A0B-46F3-8C61-023846E9132B}"/>
@@ -5410,6 +6083,10 @@
     <cellStyle name="Normal 34 18" xfId="1800" xr:uid="{FD5DB2A8-0062-4188-8E4D-74BBE3149761}"/>
     <cellStyle name="Normal 34 19" xfId="1846" xr:uid="{3912B41D-A64D-442B-AAFB-5502EC906127}"/>
     <cellStyle name="Normal 34 2" xfId="1126" xr:uid="{43B14C5F-4819-45D7-BE34-4F226C9FA9A6}"/>
+    <cellStyle name="Normal 34 2 2" xfId="2747" xr:uid="{5EE3A540-6C69-4A3B-AEAC-4A02A252CAC4}"/>
+    <cellStyle name="Normal 34 2 3" xfId="2860" xr:uid="{FD9E71AA-4E38-4502-80A1-B0FB970FD440}"/>
+    <cellStyle name="Normal 34 2 4" xfId="2975" xr:uid="{16570336-0060-4CA0-A94B-D78C983934EC}"/>
+    <cellStyle name="Normal 34 2 5" xfId="3090" xr:uid="{23C116FC-5E3A-404A-8641-E881C1D76297}"/>
     <cellStyle name="Normal 34 20" xfId="1893" xr:uid="{695D72A4-BE4B-400E-A13F-FC430413BE04}"/>
     <cellStyle name="Normal 34 21" xfId="1941" xr:uid="{D08E0B55-61F8-4471-9F68-04ECDBAEC174}"/>
     <cellStyle name="Normal 34 22" xfId="1990" xr:uid="{CA4D29B3-A182-408D-8A83-0CAB4F0AA283}"/>
@@ -5426,6 +6103,10 @@
     <cellStyle name="Normal 34 32" xfId="2526" xr:uid="{10A2FDA6-BFA6-4CFA-98B4-0A840EBB2E5A}"/>
     <cellStyle name="Normal 34 33" xfId="2581" xr:uid="{DD105E7E-441F-41E9-9408-B1E3C8521CD6}"/>
     <cellStyle name="Normal 34 34" xfId="2636" xr:uid="{DE36D422-D4D8-4B3B-B886-4669F4CC72DB}"/>
+    <cellStyle name="Normal 34 35" xfId="2692" xr:uid="{DD0CDA92-AC84-4FF8-A6F9-666959AC6A11}"/>
+    <cellStyle name="Normal 34 36" xfId="2805" xr:uid="{F646E706-D975-4F6F-B65E-04C25937B7FA}"/>
+    <cellStyle name="Normal 34 37" xfId="2920" xr:uid="{860D38AA-EF93-4820-9B71-AFFAFC61DD21}"/>
+    <cellStyle name="Normal 34 38" xfId="3035" xr:uid="{31DFF6DE-08FE-4CC4-9A68-3141F3A8614C}"/>
     <cellStyle name="Normal 34 4" xfId="1198" xr:uid="{8F856BAA-2847-43FC-BEA2-D1DAFE5D5C08}"/>
     <cellStyle name="Normal 34 5" xfId="1237" xr:uid="{E8D324D6-0564-42C7-A347-F071F77AD38C}"/>
     <cellStyle name="Normal 34 6" xfId="1277" xr:uid="{78E23A18-BA39-450B-AF6F-829AB866D556}"/>
@@ -5444,6 +6125,10 @@
     <cellStyle name="Normal 35 18" xfId="1801" xr:uid="{29C93CB9-7684-48BF-9DDA-DD6A30618ED6}"/>
     <cellStyle name="Normal 35 19" xfId="1847" xr:uid="{3B693393-6A44-46FF-87B2-1E4D08069F19}"/>
     <cellStyle name="Normal 35 2" xfId="1127" xr:uid="{B7265EF5-4F13-4822-BD22-F31E7C9EBED3}"/>
+    <cellStyle name="Normal 35 2 2" xfId="2748" xr:uid="{C3C10855-10E2-4C6A-B97B-DF20EFAB5F33}"/>
+    <cellStyle name="Normal 35 2 3" xfId="2861" xr:uid="{00646614-9616-4965-AB40-221A5608F633}"/>
+    <cellStyle name="Normal 35 2 4" xfId="2976" xr:uid="{BC20F40F-16FA-4257-979D-7C37DB326938}"/>
+    <cellStyle name="Normal 35 2 5" xfId="3091" xr:uid="{4DCA5CBB-D38D-41F4-86F0-FAE454A4A251}"/>
     <cellStyle name="Normal 35 20" xfId="1894" xr:uid="{F03C9F9A-857E-4131-A88C-49A4764621F7}"/>
     <cellStyle name="Normal 35 21" xfId="1942" xr:uid="{78799344-8DF5-4F1D-84C2-AC121645FE13}"/>
     <cellStyle name="Normal 35 22" xfId="1991" xr:uid="{AD502C56-D248-44D1-BF2F-904A6D6CC1A3}"/>
@@ -5460,6 +6145,10 @@
     <cellStyle name="Normal 35 32" xfId="2527" xr:uid="{E343B2F7-1F4F-41C7-BEA5-0687D0F8567E}"/>
     <cellStyle name="Normal 35 33" xfId="2582" xr:uid="{E3472DD8-BF44-4FAA-8F23-B0B259F2C546}"/>
     <cellStyle name="Normal 35 34" xfId="2637" xr:uid="{7375C592-CDC4-4E6E-9BDC-07152104C8FF}"/>
+    <cellStyle name="Normal 35 35" xfId="2693" xr:uid="{DD28D2DB-A758-459A-81B6-72630D0B1A7A}"/>
+    <cellStyle name="Normal 35 36" xfId="2806" xr:uid="{D4FF5BA0-4697-4643-96E4-1678E1D152E0}"/>
+    <cellStyle name="Normal 35 37" xfId="2921" xr:uid="{2FCF70F2-EBFA-4BF8-BDC3-8294B67DFFEC}"/>
+    <cellStyle name="Normal 35 38" xfId="3036" xr:uid="{F4F30DFA-6EEC-4F5D-9E6B-A2A25C60FB16}"/>
     <cellStyle name="Normal 35 4" xfId="1199" xr:uid="{5C6D934C-C084-456A-8378-EFEE061775E5}"/>
     <cellStyle name="Normal 35 5" xfId="1238" xr:uid="{7CB240F7-BDE4-4E7B-8875-63F971329466}"/>
     <cellStyle name="Normal 35 6" xfId="1278" xr:uid="{EF4981D6-3F62-4CEE-AFBB-7FAF9F704E25}"/>
@@ -5478,6 +6167,10 @@
     <cellStyle name="Normal 36 18" xfId="1848" xr:uid="{307E37AE-F216-485C-B6E6-FE3A0D702086}"/>
     <cellStyle name="Normal 36 19" xfId="1895" xr:uid="{9C5C376D-416C-4B50-B0E1-8F63B2663F7C}"/>
     <cellStyle name="Normal 36 2" xfId="1163" xr:uid="{5F031862-E9CA-4CC2-8414-CC83AEF61342}"/>
+    <cellStyle name="Normal 36 2 2" xfId="2749" xr:uid="{B492DE42-76EE-43E3-B620-5ADD4E7F58CD}"/>
+    <cellStyle name="Normal 36 2 3" xfId="2862" xr:uid="{0CA145A1-5EEF-4CDC-8C6D-12EC797F25CA}"/>
+    <cellStyle name="Normal 36 2 4" xfId="2977" xr:uid="{BA7006C2-1E53-4F0A-9F87-C213F444AE51}"/>
+    <cellStyle name="Normal 36 2 5" xfId="3092" xr:uid="{6102DE2F-88E2-44BD-9F76-B7E4C48FBCC2}"/>
     <cellStyle name="Normal 36 20" xfId="1943" xr:uid="{FD78705A-3630-44D0-BE45-22CA0C689418}"/>
     <cellStyle name="Normal 36 21" xfId="1992" xr:uid="{BC10B028-8187-4C59-A24A-74905A983715}"/>
     <cellStyle name="Normal 36 22" xfId="2042" xr:uid="{E31AE236-F51C-4104-AA39-0099594621DF}"/>
@@ -5493,6 +6186,10 @@
     <cellStyle name="Normal 36 31" xfId="2528" xr:uid="{A51D5C9B-C51F-45C7-8CB3-D186C51F1862}"/>
     <cellStyle name="Normal 36 32" xfId="2583" xr:uid="{903B5BA5-7C47-4979-983F-76E943151007}"/>
     <cellStyle name="Normal 36 33" xfId="2638" xr:uid="{DBE0A2AF-3F5E-4F68-AFC0-38D10F8A4990}"/>
+    <cellStyle name="Normal 36 34" xfId="2694" xr:uid="{1E40D692-3948-4262-8B99-54326A16D759}"/>
+    <cellStyle name="Normal 36 35" xfId="2807" xr:uid="{18877A70-FE87-486F-8A31-A3B164BF7E50}"/>
+    <cellStyle name="Normal 36 36" xfId="2922" xr:uid="{6B7C4611-F49B-4F67-B3B2-1087E6A11760}"/>
+    <cellStyle name="Normal 36 37" xfId="3037" xr:uid="{F50AD153-156A-4A16-AEDB-87C985174E8F}"/>
     <cellStyle name="Normal 36 4" xfId="1239" xr:uid="{D6071E2A-50A2-4D3C-9968-A1E3E4687B7E}"/>
     <cellStyle name="Normal 36 5" xfId="1279" xr:uid="{F643CB92-74BB-4F63-99A2-B010269425DF}"/>
     <cellStyle name="Normal 36 6" xfId="1320" xr:uid="{A54925E5-DBB1-4E4A-A7E8-D13C59949278}"/>
@@ -5511,6 +6208,10 @@
     <cellStyle name="Normal 37 18" xfId="1896" xr:uid="{B2FB34E9-83FA-40B8-83C7-07C470DED77F}"/>
     <cellStyle name="Normal 37 19" xfId="1944" xr:uid="{BC4977A6-0D69-48AE-90C0-63DCE5012FF4}"/>
     <cellStyle name="Normal 37 2" xfId="1201" xr:uid="{7C1A9B56-0357-4E4F-B0CC-D525D76EA19D}"/>
+    <cellStyle name="Normal 37 2 2" xfId="2750" xr:uid="{598E5B22-154A-4F90-9AD8-32B7F4CCAFDF}"/>
+    <cellStyle name="Normal 37 2 3" xfId="2863" xr:uid="{B41F314C-B34C-4150-83AA-45841D1D6DA2}"/>
+    <cellStyle name="Normal 37 2 4" xfId="2978" xr:uid="{01E498CE-D9B1-42E1-AF21-9A9413EACC54}"/>
+    <cellStyle name="Normal 37 2 5" xfId="3093" xr:uid="{CAC3FB43-7C11-4E05-A718-C91DB9D33ABD}"/>
     <cellStyle name="Normal 37 20" xfId="1993" xr:uid="{3C812CF5-0586-4E8E-9292-61DBFA26C1D5}"/>
     <cellStyle name="Normal 37 21" xfId="2043" xr:uid="{0FF7211A-CFF9-4C51-AC1E-81525E2FED96}"/>
     <cellStyle name="Normal 37 22" xfId="2096" xr:uid="{33DE0ACD-5338-4790-9EE7-E262F328E259}"/>
@@ -5525,6 +6226,10 @@
     <cellStyle name="Normal 37 30" xfId="2529" xr:uid="{3A652BB0-A70B-4BBD-B6BF-4DF249A443EA}"/>
     <cellStyle name="Normal 37 31" xfId="2584" xr:uid="{AA99344E-F1BB-406C-9284-8EC5BD558673}"/>
     <cellStyle name="Normal 37 32" xfId="2639" xr:uid="{DE962FA6-FAD7-498A-B3C7-F593975FD3F4}"/>
+    <cellStyle name="Normal 37 33" xfId="2695" xr:uid="{302AE904-97BC-47D3-89F6-206A16F55EDE}"/>
+    <cellStyle name="Normal 37 34" xfId="2808" xr:uid="{3F7644D1-BE3D-4C56-B8A9-B3DB64504B87}"/>
+    <cellStyle name="Normal 37 35" xfId="2923" xr:uid="{20DFBC0A-38F8-4943-9D29-DFFDE0CE6612}"/>
+    <cellStyle name="Normal 37 36" xfId="3038" xr:uid="{8D03A0C9-447C-4BC3-AEE3-5C0BDEC63480}"/>
     <cellStyle name="Normal 37 4" xfId="1280" xr:uid="{BB9F55A5-BDD5-4597-90A0-CF5B0C044934}"/>
     <cellStyle name="Normal 37 5" xfId="1321" xr:uid="{C233C0E3-A15F-40DD-88CA-205C74255FCE}"/>
     <cellStyle name="Normal 37 6" xfId="1363" xr:uid="{BF242644-0A31-474B-BA33-9B0FA600A6E1}"/>
@@ -5543,6 +6248,10 @@
     <cellStyle name="Normal 38 18" xfId="1897" xr:uid="{07F50D67-FB6D-480E-8124-B43C55776E86}"/>
     <cellStyle name="Normal 38 19" xfId="1945" xr:uid="{7F29CD14-A652-438D-A24C-574E85DA356E}"/>
     <cellStyle name="Normal 38 2" xfId="1202" xr:uid="{B0FAF236-5724-4CB6-B26D-8F90CC51297B}"/>
+    <cellStyle name="Normal 38 2 2" xfId="2751" xr:uid="{1FC655BB-DB79-4A00-9E51-3B3B61374038}"/>
+    <cellStyle name="Normal 38 2 3" xfId="2864" xr:uid="{AC62BC98-78A9-43AA-A156-2D156A95C534}"/>
+    <cellStyle name="Normal 38 2 4" xfId="2979" xr:uid="{D1D4A6B9-5922-4B55-96D4-AE46D072EC1E}"/>
+    <cellStyle name="Normal 38 2 5" xfId="3094" xr:uid="{5B76102A-6DF5-4705-BEE7-763C1096B5B8}"/>
     <cellStyle name="Normal 38 20" xfId="1994" xr:uid="{C59763F5-0850-4D08-A1D6-9FCDC99662EF}"/>
     <cellStyle name="Normal 38 21" xfId="2044" xr:uid="{225E38C2-C9D5-41B6-9B82-4A53AFAAA53A}"/>
     <cellStyle name="Normal 38 22" xfId="2097" xr:uid="{236F4960-ADDB-476D-82E5-2B62A733B5DE}"/>
@@ -5557,6 +6266,10 @@
     <cellStyle name="Normal 38 30" xfId="2530" xr:uid="{07BFE165-0C73-4794-ABD6-61BFC651DF7E}"/>
     <cellStyle name="Normal 38 31" xfId="2585" xr:uid="{3B7B97CB-CF69-4248-BA93-3793AF85C633}"/>
     <cellStyle name="Normal 38 32" xfId="2640" xr:uid="{32043AFA-59BD-4271-AA46-0306589BA734}"/>
+    <cellStyle name="Normal 38 33" xfId="2696" xr:uid="{81CDCD14-2B2F-4266-8E2C-6E927B5A16A9}"/>
+    <cellStyle name="Normal 38 34" xfId="2809" xr:uid="{6714592C-B892-4090-8CB0-73B238DF561F}"/>
+    <cellStyle name="Normal 38 35" xfId="2924" xr:uid="{E66B685B-91B6-4A08-9D4B-7B960D0BCB9B}"/>
+    <cellStyle name="Normal 38 36" xfId="3039" xr:uid="{BAA409E2-0395-4281-A40F-543D34641A06}"/>
     <cellStyle name="Normal 38 4" xfId="1281" xr:uid="{06B9E8CD-8E13-44D7-B4A2-3CCA5CF70BFC}"/>
     <cellStyle name="Normal 38 5" xfId="1322" xr:uid="{64D206D8-A195-42CA-8AFF-84B3F657D678}"/>
     <cellStyle name="Normal 38 6" xfId="1364" xr:uid="{A37FD0CC-7CC6-439F-9126-06B26282AAA9}"/>
@@ -5575,6 +6288,10 @@
     <cellStyle name="Normal 39 18" xfId="1946" xr:uid="{0D02DE3A-DCDF-46BF-B571-B325D62556E3}"/>
     <cellStyle name="Normal 39 19" xfId="1995" xr:uid="{2AC23D60-4A64-47F2-B477-6406B391D52B}"/>
     <cellStyle name="Normal 39 2" xfId="1242" xr:uid="{9B6D5D0B-E302-4B4C-93EB-E056A23BBE0F}"/>
+    <cellStyle name="Normal 39 2 2" xfId="2752" xr:uid="{8D8267D8-73CE-44B7-9056-BB12EB6FD4F9}"/>
+    <cellStyle name="Normal 39 2 3" xfId="2865" xr:uid="{A9D687FA-EC44-426E-A926-CC18ECEB5DA9}"/>
+    <cellStyle name="Normal 39 2 4" xfId="2980" xr:uid="{86E2A356-3F2D-4916-85C5-876C6F11096F}"/>
+    <cellStyle name="Normal 39 2 5" xfId="3095" xr:uid="{3A0C6936-4FD7-466A-94B4-83D9B8A98087}"/>
     <cellStyle name="Normal 39 20" xfId="2045" xr:uid="{E858B128-4FE0-45EF-A008-F5B1C468572B}"/>
     <cellStyle name="Normal 39 21" xfId="2098" xr:uid="{8A9F59CC-979E-448E-8536-BA76ED50CF50}"/>
     <cellStyle name="Normal 39 22" xfId="2151" xr:uid="{6F0F52DE-2CA3-4F41-8C47-59C581F959C3}"/>
@@ -5588,6 +6305,10 @@
     <cellStyle name="Normal 39 3" xfId="1282" xr:uid="{0296B16D-DA08-43E9-9663-8A88969E79F4}"/>
     <cellStyle name="Normal 39 30" xfId="2586" xr:uid="{6DFF16CF-67E4-4DD5-8603-E0CA064031AE}"/>
     <cellStyle name="Normal 39 31" xfId="2641" xr:uid="{A9F2DB4C-9778-49B9-B98D-A3F7D714FA5F}"/>
+    <cellStyle name="Normal 39 32" xfId="2697" xr:uid="{7A828D63-0888-4DC1-85F5-3A6E1E7ED047}"/>
+    <cellStyle name="Normal 39 33" xfId="2810" xr:uid="{F1A141D4-DC57-49BB-87FC-2C314F32A647}"/>
+    <cellStyle name="Normal 39 34" xfId="2925" xr:uid="{B2C29D08-7C4B-4107-BE94-FC0298B4A13E}"/>
+    <cellStyle name="Normal 39 35" xfId="3040" xr:uid="{E5E83F1B-CA9E-4D2B-A580-6A8D8C931FBF}"/>
     <cellStyle name="Normal 39 4" xfId="1323" xr:uid="{15831E53-2DBD-4A2E-B270-23C619CA089E}"/>
     <cellStyle name="Normal 39 5" xfId="1365" xr:uid="{F009ABEF-0BCE-4955-ADC3-3578DB39F7F8}"/>
     <cellStyle name="Normal 39 6" xfId="1407" xr:uid="{726EFD29-EDCE-49BC-825A-A138625D51CD}"/>
@@ -5596,6 +6317,7 @@
     <cellStyle name="Normal 39 9" xfId="1538" xr:uid="{DD4AA46F-DBE8-4550-B556-58288FDBB67B}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{CC068BAF-4114-41CE-974F-9AA5434E3A14}"/>
     <cellStyle name="Normal 4 10" xfId="60" xr:uid="{9242557F-1A56-4359-99FE-2C316F7701F5}"/>
+    <cellStyle name="Normal 4 100" xfId="3005" xr:uid="{F1E619EE-2B20-4039-AA4F-593582620CE9}"/>
     <cellStyle name="Normal 4 11" xfId="67" xr:uid="{0A2B4805-1128-483C-844B-2630CBFFFFA6}"/>
     <cellStyle name="Normal 4 12" xfId="74" xr:uid="{A2120A26-AB5C-41C4-A09A-B3E14213D25E}"/>
     <cellStyle name="Normal 4 13" xfId="81" xr:uid="{E3AF6016-CFB5-477F-8D8C-C14D02C3A171}"/>
@@ -5606,6 +6328,10 @@
     <cellStyle name="Normal 4 18" xfId="121" xr:uid="{05072892-1F23-4BE5-942A-B4F4C2E7800D}"/>
     <cellStyle name="Normal 4 19" xfId="129" xr:uid="{5AE30855-35A2-480B-98BA-4D921E828889}"/>
     <cellStyle name="Normal 4 2" xfId="9" xr:uid="{EDAA3683-05B6-4BC7-AD09-8DD7D2B9D9F9}"/>
+    <cellStyle name="Normal 4 2 2" xfId="2717" xr:uid="{2372B843-4F6E-45AE-8669-4B1CA3D6980B}"/>
+    <cellStyle name="Normal 4 2 3" xfId="2830" xr:uid="{C8B60490-FF61-4D00-A4AE-B1FC433CD75B}"/>
+    <cellStyle name="Normal 4 2 4" xfId="2945" xr:uid="{35A023AE-19B9-43F6-AEBD-36073D9FBA37}"/>
+    <cellStyle name="Normal 4 2 5" xfId="3060" xr:uid="{7BCF02FE-E071-4204-90FB-E2187241478E}"/>
     <cellStyle name="Normal 4 20" xfId="137" xr:uid="{8ECAF58F-6033-4FAE-8F6D-F69EFA4CFAC4}"/>
     <cellStyle name="Normal 4 21" xfId="145" xr:uid="{E849ED04-C446-4516-A1A4-6F0A529AF78B}"/>
     <cellStyle name="Normal 4 22" xfId="153" xr:uid="{343376C8-1273-4151-944F-9DB5E5D1EE75}"/>
@@ -5690,6 +6416,9 @@
     <cellStyle name="Normal 4 94" xfId="2496" xr:uid="{7AEC0261-4350-465C-8F83-41FF9454D6DE}"/>
     <cellStyle name="Normal 4 95" xfId="2551" xr:uid="{0521DAAF-579E-4EB5-A892-1824F512F272}"/>
     <cellStyle name="Normal 4 96" xfId="2606" xr:uid="{81B8554B-195D-41A4-B1CE-733020EA6D7B}"/>
+    <cellStyle name="Normal 4 97" xfId="2662" xr:uid="{EFF8DB05-6A10-4EF1-BE2D-69DE3A1DA7B9}"/>
+    <cellStyle name="Normal 4 98" xfId="2775" xr:uid="{A6439975-BEF7-42A4-AB8E-000077A87705}"/>
+    <cellStyle name="Normal 4 99" xfId="2890" xr:uid="{CE042ABD-8171-498C-824B-F6307383A9CF}"/>
     <cellStyle name="Normal 40" xfId="1204" xr:uid="{9A758E20-7263-44F0-A0A0-3D5D1FE88C83}"/>
     <cellStyle name="Normal 40 10" xfId="1584" xr:uid="{00514BDB-1937-4C34-97E1-6B15E53A4098}"/>
     <cellStyle name="Normal 40 11" xfId="1628" xr:uid="{858AF8D4-5153-4B46-93B1-00B25FF415FB}"/>
@@ -5702,6 +6431,10 @@
     <cellStyle name="Normal 40 18" xfId="1947" xr:uid="{3001DEC0-12AA-4308-A9B1-C5B3DB634459}"/>
     <cellStyle name="Normal 40 19" xfId="1996" xr:uid="{17D2B3B7-527E-4AF8-A44E-CD98CC306D06}"/>
     <cellStyle name="Normal 40 2" xfId="1243" xr:uid="{01DB0934-BA67-4920-BE40-65A1B85F7EF8}"/>
+    <cellStyle name="Normal 40 2 2" xfId="2753" xr:uid="{C9C75A4E-D2A0-448C-AF0A-8A58476F9F09}"/>
+    <cellStyle name="Normal 40 2 3" xfId="2866" xr:uid="{427BC04C-D661-4935-8476-BA3EB8660B73}"/>
+    <cellStyle name="Normal 40 2 4" xfId="2981" xr:uid="{7D6BC997-B675-4B76-A9BB-C873BA519A42}"/>
+    <cellStyle name="Normal 40 2 5" xfId="3096" xr:uid="{EC6248E0-0195-4DFA-A335-A7EA898F9927}"/>
     <cellStyle name="Normal 40 20" xfId="2046" xr:uid="{1AA8DCDC-3E38-4179-B5A8-A7C399016171}"/>
     <cellStyle name="Normal 40 21" xfId="2099" xr:uid="{B628178D-0F3A-474F-925E-07FA0BB612DA}"/>
     <cellStyle name="Normal 40 22" xfId="2152" xr:uid="{8D7B175A-5572-4CC6-9CC5-604A9FF6E594}"/>
@@ -5715,6 +6448,10 @@
     <cellStyle name="Normal 40 3" xfId="1283" xr:uid="{60DC833A-F031-4DBD-BC0B-B48ABCDE6533}"/>
     <cellStyle name="Normal 40 30" xfId="2587" xr:uid="{0E60E04E-AB8C-41D1-975C-2E5D4DAA9195}"/>
     <cellStyle name="Normal 40 31" xfId="2642" xr:uid="{E5EBFCBF-3FAB-4093-872F-65B412F95D30}"/>
+    <cellStyle name="Normal 40 32" xfId="2698" xr:uid="{E1C5D300-29D2-44DF-B09D-626BA0E887AA}"/>
+    <cellStyle name="Normal 40 33" xfId="2811" xr:uid="{21FE7F06-08B6-4894-963C-9B53555D5910}"/>
+    <cellStyle name="Normal 40 34" xfId="2926" xr:uid="{182E0D4A-6597-42BD-B490-3CB353CB95B2}"/>
+    <cellStyle name="Normal 40 35" xfId="3041" xr:uid="{0D3E011A-A6D4-46ED-8C81-C25A4B449685}"/>
     <cellStyle name="Normal 40 4" xfId="1324" xr:uid="{BC132578-6363-4D48-BB11-F90899981771}"/>
     <cellStyle name="Normal 40 5" xfId="1366" xr:uid="{CCB407F9-2940-4586-A2FB-F175B848303E}"/>
     <cellStyle name="Normal 40 6" xfId="1408" xr:uid="{7548B4F1-5CC1-4EA1-9223-B76BCC53A8BD}"/>
@@ -5733,6 +6470,10 @@
     <cellStyle name="Normal 41 18" xfId="1997" xr:uid="{4607E77B-CFB0-412B-AF45-790B42C55B28}"/>
     <cellStyle name="Normal 41 19" xfId="2047" xr:uid="{FA58CFA3-0CB6-4723-BA48-609EDE6195D5}"/>
     <cellStyle name="Normal 41 2" xfId="1284" xr:uid="{4D69E5D3-0AFE-413E-AFD0-14C4CB9DF0B1}"/>
+    <cellStyle name="Normal 41 2 2" xfId="2754" xr:uid="{DDA31F51-C264-4AF2-968A-F43C60623E7C}"/>
+    <cellStyle name="Normal 41 2 3" xfId="2867" xr:uid="{C6AC872A-B07D-40BF-84E4-5B6F25D0E104}"/>
+    <cellStyle name="Normal 41 2 4" xfId="2982" xr:uid="{C81D461F-EEBD-4EB9-9F36-0EF734A3EF1B}"/>
+    <cellStyle name="Normal 41 2 5" xfId="3097" xr:uid="{85B8B1E1-6F7F-45A5-A25D-4679B5D5A434}"/>
     <cellStyle name="Normal 41 20" xfId="2100" xr:uid="{9728B843-827F-43B7-A679-4FCCED5546FD}"/>
     <cellStyle name="Normal 41 21" xfId="2153" xr:uid="{F82C7E42-39AB-4328-9589-F26A236D3AF9}"/>
     <cellStyle name="Normal 41 22" xfId="2206" xr:uid="{3B44B64E-D9F1-44D2-9F8B-A2EF092534DB}"/>
@@ -5745,6 +6486,10 @@
     <cellStyle name="Normal 41 29" xfId="2588" xr:uid="{9EC65DA9-F820-4E50-AA99-FF308522A26D}"/>
     <cellStyle name="Normal 41 3" xfId="1325" xr:uid="{DB7266FD-DB20-4504-9181-FDAD4A49F920}"/>
     <cellStyle name="Normal 41 30" xfId="2643" xr:uid="{5A70FD02-EF28-4CB5-B20D-AF73372F3BCE}"/>
+    <cellStyle name="Normal 41 31" xfId="2699" xr:uid="{3588404C-B904-4AE0-92F5-75ECFB729F94}"/>
+    <cellStyle name="Normal 41 32" xfId="2812" xr:uid="{431840BA-29D4-4E29-8345-31B46E4A09F9}"/>
+    <cellStyle name="Normal 41 33" xfId="2927" xr:uid="{AB387AFE-B125-4A4B-BEC9-B1A6B8E6E264}"/>
+    <cellStyle name="Normal 41 34" xfId="3042" xr:uid="{4B8D4BDA-A28E-4AC2-ACDD-477A4370AB8B}"/>
     <cellStyle name="Normal 41 4" xfId="1367" xr:uid="{7EE95D5B-6BEF-49DA-8567-DB37D49C5ABE}"/>
     <cellStyle name="Normal 41 5" xfId="1409" xr:uid="{626DD975-DD53-4D9F-B777-AA700296E57B}"/>
     <cellStyle name="Normal 41 6" xfId="1452" xr:uid="{6CE0B273-A5D0-46F8-A408-8A59B910B884}"/>
@@ -5763,6 +6508,10 @@
     <cellStyle name="Normal 42 18" xfId="2048" xr:uid="{F9E95BFC-799F-4907-BE17-FD3426A2871C}"/>
     <cellStyle name="Normal 42 19" xfId="2101" xr:uid="{3F7D7D68-4882-4511-AA27-ED1EB091A09A}"/>
     <cellStyle name="Normal 42 2" xfId="1326" xr:uid="{C11F173C-8B23-4A8C-8AF5-B290CCCD5008}"/>
+    <cellStyle name="Normal 42 2 2" xfId="2755" xr:uid="{B810CB12-A510-4E6F-BBFE-28C335D3697D}"/>
+    <cellStyle name="Normal 42 2 3" xfId="2868" xr:uid="{5394BEC5-11C6-4443-960A-75D8CFAF0559}"/>
+    <cellStyle name="Normal 42 2 4" xfId="2983" xr:uid="{6A21E49D-0427-48A8-9E39-BFC53953FDB9}"/>
+    <cellStyle name="Normal 42 2 5" xfId="3098" xr:uid="{8E272D24-FA92-4C1E-BC16-2A944D50B61F}"/>
     <cellStyle name="Normal 42 20" xfId="2154" xr:uid="{5EDB87FE-E2CC-4CB1-8EFC-70B996934A91}"/>
     <cellStyle name="Normal 42 21" xfId="2207" xr:uid="{7FD2750E-290A-4D4C-B57F-BBF4E41B01FD}"/>
     <cellStyle name="Normal 42 22" xfId="2261" xr:uid="{0B62BB22-7FC0-43E8-9633-EE7CA43B1CED}"/>
@@ -5774,6 +6523,10 @@
     <cellStyle name="Normal 42 28" xfId="2589" xr:uid="{807D0CC8-9AB4-4E1F-829A-BA8CE8E1A61B}"/>
     <cellStyle name="Normal 42 29" xfId="2644" xr:uid="{82416638-6DDE-4130-B174-F4443FA4C084}"/>
     <cellStyle name="Normal 42 3" xfId="1368" xr:uid="{027F54D2-79FB-429D-8AF6-DC22C57389A3}"/>
+    <cellStyle name="Normal 42 30" xfId="2700" xr:uid="{56AC33E5-5EEA-47EA-8259-0949B3129A5A}"/>
+    <cellStyle name="Normal 42 31" xfId="2813" xr:uid="{2F5B48B8-3B5B-43BE-AE2C-EB3E5AC1C08E}"/>
+    <cellStyle name="Normal 42 32" xfId="2928" xr:uid="{DF2AD7D6-3AC5-4862-8C0E-F943CADC6AD6}"/>
+    <cellStyle name="Normal 42 33" xfId="3043" xr:uid="{2B298408-974C-4248-B82A-01E381E7BBB0}"/>
     <cellStyle name="Normal 42 4" xfId="1410" xr:uid="{04BC6829-1A0D-4655-BB18-979D575FAF18}"/>
     <cellStyle name="Normal 42 5" xfId="1453" xr:uid="{A41DFB52-1E5B-461C-8EE4-AB2538BAB5D4}"/>
     <cellStyle name="Normal 42 6" xfId="1497" xr:uid="{3B664C59-A8E2-4B39-9C29-9C1380064345}"/>
@@ -5792,6 +6545,10 @@
     <cellStyle name="Normal 43 18" xfId="2102" xr:uid="{412D1AC7-8964-462F-91B8-B920AC9F7C3C}"/>
     <cellStyle name="Normal 43 19" xfId="2155" xr:uid="{8647AF3E-D719-41B3-80E6-79EED38E4726}"/>
     <cellStyle name="Normal 43 2" xfId="1369" xr:uid="{ABE00B05-FBDD-472A-83B6-A905DBC59FFD}"/>
+    <cellStyle name="Normal 43 2 2" xfId="2756" xr:uid="{916C8810-B713-4072-8D5B-ED3A84769530}"/>
+    <cellStyle name="Normal 43 2 3" xfId="2869" xr:uid="{D9CD1E6B-6173-462D-802C-AB841BE74D4F}"/>
+    <cellStyle name="Normal 43 2 4" xfId="2984" xr:uid="{8100632C-ED2A-466F-ACD1-6121BE5F21C6}"/>
+    <cellStyle name="Normal 43 2 5" xfId="3099" xr:uid="{52FB432B-20D5-448D-96A5-D599024ECDA6}"/>
     <cellStyle name="Normal 43 20" xfId="2208" xr:uid="{863323DB-B25B-44E0-8AA0-507DCEFB5E27}"/>
     <cellStyle name="Normal 43 21" xfId="2262" xr:uid="{08000729-FCA7-447A-8293-2AE43813AF6E}"/>
     <cellStyle name="Normal 43 22" xfId="2316" xr:uid="{E6CC6AF2-7ACA-49DA-AA08-6B90ADEDDF35}"/>
@@ -5801,7 +6558,11 @@
     <cellStyle name="Normal 43 26" xfId="2535" xr:uid="{13849D65-AA3D-421C-9F10-23D08DCD8FE9}"/>
     <cellStyle name="Normal 43 27" xfId="2590" xr:uid="{BFB8FA52-F487-40E1-8D18-17137293FCBC}"/>
     <cellStyle name="Normal 43 28" xfId="2645" xr:uid="{86B6D99C-6592-46CC-BA91-E3DC06CFC223}"/>
+    <cellStyle name="Normal 43 29" xfId="2701" xr:uid="{73CA54A0-BCB8-487E-8615-3AD79B422B7A}"/>
     <cellStyle name="Normal 43 3" xfId="1411" xr:uid="{E9013BFE-34CD-4396-9801-740BE57E4C74}"/>
+    <cellStyle name="Normal 43 30" xfId="2814" xr:uid="{88154F93-A35F-4BA5-B330-B204CE3C45AE}"/>
+    <cellStyle name="Normal 43 31" xfId="2929" xr:uid="{D7ED0A32-7DFE-4697-A92D-F04DC5F32E72}"/>
+    <cellStyle name="Normal 43 32" xfId="3044" xr:uid="{149BC815-0288-4F19-B763-A5C080DB5C80}"/>
     <cellStyle name="Normal 43 4" xfId="1454" xr:uid="{8B718497-4D05-4283-B46C-590C40CCD3B5}"/>
     <cellStyle name="Normal 43 5" xfId="1498" xr:uid="{8E7273E6-D96E-4807-9FA4-FD3FAA93ABEC}"/>
     <cellStyle name="Normal 43 6" xfId="1542" xr:uid="{B31FB50A-76E8-4636-A18C-E05DFC7ADE17}"/>
@@ -5820,6 +6581,10 @@
     <cellStyle name="Normal 44 18" xfId="2209" xr:uid="{D30AF8B5-B9EA-48B9-961D-1F1FD6F9CE04}"/>
     <cellStyle name="Normal 44 19" xfId="2263" xr:uid="{166376C5-5132-4181-8CEE-C4540FB64AA3}"/>
     <cellStyle name="Normal 44 2" xfId="1455" xr:uid="{FB733BCC-778D-482A-8F7C-76DD90096D45}"/>
+    <cellStyle name="Normal 44 2 2" xfId="2757" xr:uid="{6163AEEF-986E-48CE-89BA-3907F3D7CB52}"/>
+    <cellStyle name="Normal 44 2 3" xfId="2870" xr:uid="{0A225940-6873-42DA-B6E1-AD9DDFEC46BC}"/>
+    <cellStyle name="Normal 44 2 4" xfId="2985" xr:uid="{666154C8-975D-4BD6-ADAC-EE6F5BA53CD8}"/>
+    <cellStyle name="Normal 44 2 5" xfId="3100" xr:uid="{88189171-1B20-4831-AC23-50052AC57FDC}"/>
     <cellStyle name="Normal 44 20" xfId="2317" xr:uid="{37A14A11-41D7-4793-9EB1-375B7C7BC519}"/>
     <cellStyle name="Normal 44 21" xfId="2371" xr:uid="{39BEE483-4692-476C-9313-D62EA4633326}"/>
     <cellStyle name="Normal 44 22" xfId="2426" xr:uid="{3BA62BB1-792D-45F3-8659-AF5C7965BF92}"/>
@@ -5827,7 +6592,11 @@
     <cellStyle name="Normal 44 24" xfId="2536" xr:uid="{BA975EB6-7634-44DC-B476-BFAAA0821F6E}"/>
     <cellStyle name="Normal 44 25" xfId="2591" xr:uid="{1F7DE00D-A6C1-4A9E-8BFB-7AA0C5B7FCF8}"/>
     <cellStyle name="Normal 44 26" xfId="2646" xr:uid="{9726AF58-BCBA-4D0A-A55F-A2E5B65F6CC9}"/>
+    <cellStyle name="Normal 44 27" xfId="2702" xr:uid="{847CD07D-D603-4D51-B00C-3491D09078B7}"/>
+    <cellStyle name="Normal 44 28" xfId="2815" xr:uid="{D27FD044-69EC-491F-9DDD-D0599D09D68A}"/>
+    <cellStyle name="Normal 44 29" xfId="2930" xr:uid="{DA160561-433F-497A-BAAD-CE027BC709EE}"/>
     <cellStyle name="Normal 44 3" xfId="1499" xr:uid="{19841630-1868-4129-AF65-9439A8362635}"/>
+    <cellStyle name="Normal 44 30" xfId="3045" xr:uid="{414F4DF4-B660-4624-9C24-4BE4CA5E4093}"/>
     <cellStyle name="Normal 44 4" xfId="1543" xr:uid="{B24CAFA4-F870-42C6-835A-841530B7459E}"/>
     <cellStyle name="Normal 44 5" xfId="1588" xr:uid="{F3149A38-5BF0-4CF4-92A1-CEBFBCA9E57B}"/>
     <cellStyle name="Normal 44 6" xfId="1632" xr:uid="{1852EA26-6C56-496C-93D7-FD09B509C57A}"/>
@@ -5846,12 +6615,20 @@
     <cellStyle name="Normal 45 18" xfId="2264" xr:uid="{DFD0FB7C-1F4D-4665-A7DC-5308508319F8}"/>
     <cellStyle name="Normal 45 19" xfId="2318" xr:uid="{35A59C85-A695-422D-9858-4CDF82238F16}"/>
     <cellStyle name="Normal 45 2" xfId="1500" xr:uid="{5027BECF-87E9-4D4B-9BEF-85E1909AE39A}"/>
+    <cellStyle name="Normal 45 2 2" xfId="2758" xr:uid="{51D14985-6D48-4636-81AF-6D9CE1576A8C}"/>
+    <cellStyle name="Normal 45 2 3" xfId="2871" xr:uid="{55C6F11C-5D72-4821-AACE-EE3A73831B5C}"/>
+    <cellStyle name="Normal 45 2 4" xfId="2986" xr:uid="{7652BF85-ED97-4921-844C-AF187B4CB45B}"/>
+    <cellStyle name="Normal 45 2 5" xfId="3101" xr:uid="{79E482AA-09DA-48D5-AA93-04363C69C5BD}"/>
     <cellStyle name="Normal 45 20" xfId="2372" xr:uid="{0E3AA70B-706E-422D-BA4C-6FFD45EF939A}"/>
     <cellStyle name="Normal 45 21" xfId="2427" xr:uid="{6B8EEB3E-EF73-45B8-A5A6-B1DEF269080F}"/>
     <cellStyle name="Normal 45 22" xfId="2482" xr:uid="{860D4BE7-897A-468C-87DC-248651837E59}"/>
     <cellStyle name="Normal 45 23" xfId="2537" xr:uid="{BFE2DAAA-B94B-40B0-94ED-BA82B45EF879}"/>
     <cellStyle name="Normal 45 24" xfId="2592" xr:uid="{B776F09F-482E-4A29-9779-68E1BC542E91}"/>
     <cellStyle name="Normal 45 25" xfId="2647" xr:uid="{76C85D64-BEC3-40E2-AF82-B27533CF7EAC}"/>
+    <cellStyle name="Normal 45 26" xfId="2703" xr:uid="{C318CA5C-C750-45A1-B748-E8AAF8A13D09}"/>
+    <cellStyle name="Normal 45 27" xfId="2816" xr:uid="{C83C5A88-59DE-45FC-A806-6D27D53B9C9F}"/>
+    <cellStyle name="Normal 45 28" xfId="2931" xr:uid="{0582439B-2B17-49CD-A694-E2E0A710B851}"/>
+    <cellStyle name="Normal 45 29" xfId="3046" xr:uid="{DEBF8B63-A14A-48A3-94DA-861B308A8DCC}"/>
     <cellStyle name="Normal 45 3" xfId="1544" xr:uid="{1787A129-1435-4B42-BEEC-006984305340}"/>
     <cellStyle name="Normal 45 4" xfId="1589" xr:uid="{D8955FBC-9811-4F2B-8AA5-1BB672F751BC}"/>
     <cellStyle name="Normal 45 5" xfId="1633" xr:uid="{282C9639-360C-473E-852D-2521B8E40B05}"/>
@@ -5871,6 +6648,14 @@
     <cellStyle name="Normal 46 18" xfId="2593" xr:uid="{66F26B5C-8E69-47D1-8428-45F31C6B4FC8}"/>
     <cellStyle name="Normal 46 19" xfId="2648" xr:uid="{0CCF7C06-7E7F-4698-904D-6FB64062790F}"/>
     <cellStyle name="Normal 46 2" xfId="1722" xr:uid="{A92ECEED-86A5-4AF8-A45B-3F5122E4A57C}"/>
+    <cellStyle name="Normal 46 2 2" xfId="2759" xr:uid="{010A2599-DC2A-4D59-BC06-10F6B9A28FB6}"/>
+    <cellStyle name="Normal 46 2 3" xfId="2872" xr:uid="{F3DB1F59-409B-4D1E-951C-4AEF9E69625E}"/>
+    <cellStyle name="Normal 46 2 4" xfId="2987" xr:uid="{43E52D82-36BA-446D-BC61-F33E1140C8F8}"/>
+    <cellStyle name="Normal 46 2 5" xfId="3102" xr:uid="{6B3B7659-CF2E-49A9-B482-0AE4CA59FEA4}"/>
+    <cellStyle name="Normal 46 20" xfId="2704" xr:uid="{7FD38751-90D0-47F1-9B82-7B7F87E4F4A1}"/>
+    <cellStyle name="Normal 46 21" xfId="2817" xr:uid="{D59DA624-4041-4F66-8653-E74CEF0B863E}"/>
+    <cellStyle name="Normal 46 22" xfId="2932" xr:uid="{676DF148-C10E-46B8-963B-04DB72F4FA98}"/>
+    <cellStyle name="Normal 46 23" xfId="3047" xr:uid="{0A7D6A00-BB2C-4C5D-9D08-41B1C42ADFEB}"/>
     <cellStyle name="Normal 46 3" xfId="1812" xr:uid="{9B7FD6F8-A2AE-4D9F-97CA-07164D6BFAED}"/>
     <cellStyle name="Normal 46 4" xfId="1858" xr:uid="{5099E28A-8E05-4821-9D0F-B6E84C8944BB}"/>
     <cellStyle name="Normal 46 5" xfId="1905" xr:uid="{5B92D1A3-9D58-433F-A2C1-47AD5097A2B3}"/>
@@ -5888,7 +6673,15 @@
     <cellStyle name="Normal 47 16" xfId="2539" xr:uid="{2FC79E6F-B9D4-48AD-B16C-3C3B6B31B74D}"/>
     <cellStyle name="Normal 47 17" xfId="2594" xr:uid="{0AEE451B-3F60-47D7-8640-887E17B22603}"/>
     <cellStyle name="Normal 47 18" xfId="2649" xr:uid="{EA7667C7-C1DD-40B6-A318-2C0C47212009}"/>
+    <cellStyle name="Normal 47 19" xfId="2705" xr:uid="{8B1E6270-1366-4D17-8D51-1DA9C398C200}"/>
     <cellStyle name="Normal 47 2" xfId="1813" xr:uid="{C2210DC9-C26B-4BF3-AF35-FBEBA6756BF6}"/>
+    <cellStyle name="Normal 47 2 2" xfId="2760" xr:uid="{1AF5987C-315C-4E08-9E66-D06C0461CC90}"/>
+    <cellStyle name="Normal 47 2 3" xfId="2873" xr:uid="{4F508B1E-DB8B-4990-BC9F-7F1C29EBEB1F}"/>
+    <cellStyle name="Normal 47 2 4" xfId="2988" xr:uid="{258A8FAF-22FA-4ABA-8A38-846EADEF780B}"/>
+    <cellStyle name="Normal 47 2 5" xfId="3103" xr:uid="{D75339CA-3587-4FCA-904F-51FED439ACD8}"/>
+    <cellStyle name="Normal 47 20" xfId="2818" xr:uid="{B9BBFC70-4E0C-4CAF-9B98-1BB2489C9D85}"/>
+    <cellStyle name="Normal 47 21" xfId="2933" xr:uid="{6A056758-BC3A-4B49-8865-6566BEF817B2}"/>
+    <cellStyle name="Normal 47 22" xfId="3048" xr:uid="{1FBA8C6D-D6EC-427A-8588-9F4888C99867}"/>
     <cellStyle name="Normal 47 3" xfId="1859" xr:uid="{68779769-7635-477C-A18C-EF4DCCAC4899}"/>
     <cellStyle name="Normal 47 4" xfId="1906" xr:uid="{2F6200A8-6C6E-4A93-87BA-36E965276181}"/>
     <cellStyle name="Normal 47 5" xfId="1954" xr:uid="{93F6DB6D-9F99-4F65-B61E-458354B3226D}"/>
@@ -5904,7 +6697,15 @@
     <cellStyle name="Normal 48 14" xfId="2540" xr:uid="{502A937D-F975-404A-AFA2-D58C2AB2303E}"/>
     <cellStyle name="Normal 48 15" xfId="2595" xr:uid="{4623B74F-9F0C-4AAA-B3F1-BAE059E5B8A9}"/>
     <cellStyle name="Normal 48 16" xfId="2650" xr:uid="{D0006705-DECE-4952-A764-E6ADDE980A8D}"/>
+    <cellStyle name="Normal 48 17" xfId="2706" xr:uid="{79F3BACE-46A6-49BF-80F8-C0997AF41F05}"/>
+    <cellStyle name="Normal 48 18" xfId="2819" xr:uid="{2839EC71-24D0-41C6-9DD8-A4CF4D1199EF}"/>
+    <cellStyle name="Normal 48 19" xfId="2934" xr:uid="{7463D7D2-29C6-48F2-BBBF-08864FE0C328}"/>
     <cellStyle name="Normal 48 2" xfId="1907" xr:uid="{CB91C6DC-62B0-4992-A8A4-FEC63EC908A5}"/>
+    <cellStyle name="Normal 48 2 2" xfId="2761" xr:uid="{514247BF-DA86-49F9-9D37-BCB7A6E46930}"/>
+    <cellStyle name="Normal 48 2 3" xfId="2874" xr:uid="{783976CF-6972-41B4-AE6D-8EA47D535105}"/>
+    <cellStyle name="Normal 48 2 4" xfId="2989" xr:uid="{FC9131FD-EB1F-40ED-8F6A-FDC5963AB685}"/>
+    <cellStyle name="Normal 48 2 5" xfId="3104" xr:uid="{14E4599A-1B09-4490-9387-B0F4302459DD}"/>
+    <cellStyle name="Normal 48 20" xfId="3049" xr:uid="{FAA8F4EA-ED8A-4714-86DC-28878EDF7940}"/>
     <cellStyle name="Normal 48 3" xfId="1955" xr:uid="{9140C7D6-0A03-4AEF-AB80-301C7410CF0E}"/>
     <cellStyle name="Normal 48 4" xfId="2004" xr:uid="{4958E27D-47B3-4CE5-9C94-AA09930271BA}"/>
     <cellStyle name="Normal 48 5" xfId="2054" xr:uid="{B7DE59F7-3166-451B-A667-D798A94434CF}"/>
@@ -5919,7 +6720,15 @@
     <cellStyle name="Normal 49 13" xfId="2541" xr:uid="{02F45A4E-86FD-4BB1-BEC6-FEE9F7C27D78}"/>
     <cellStyle name="Normal 49 14" xfId="2596" xr:uid="{AD88EABD-127C-45C5-AB5B-FCFF698F0AAF}"/>
     <cellStyle name="Normal 49 15" xfId="2651" xr:uid="{9D6D2683-4B16-4C7E-AA58-5678DAC277C2}"/>
+    <cellStyle name="Normal 49 16" xfId="2707" xr:uid="{E941AF5A-BEDA-48ED-B298-1C776B1080FF}"/>
+    <cellStyle name="Normal 49 17" xfId="2820" xr:uid="{2D093F96-C612-4EFA-BA5E-32E71A39A260}"/>
+    <cellStyle name="Normal 49 18" xfId="2935" xr:uid="{EE66896D-5CF2-42F8-8113-9B2A5F2A1FAE}"/>
+    <cellStyle name="Normal 49 19" xfId="3050" xr:uid="{84F9638C-B2F7-487A-B207-5EB150F85C8C}"/>
     <cellStyle name="Normal 49 2" xfId="1956" xr:uid="{AB9E1C32-A524-46A2-A8BF-A94BB89130A2}"/>
+    <cellStyle name="Normal 49 2 2" xfId="2762" xr:uid="{C104C047-D2EB-4E3E-8024-E24530F736BC}"/>
+    <cellStyle name="Normal 49 2 3" xfId="2875" xr:uid="{E2EDE42C-E445-4675-BFCE-216C747698C1}"/>
+    <cellStyle name="Normal 49 2 4" xfId="2990" xr:uid="{C394AEE7-A1E6-4B1C-9966-C3FFBCA81A1A}"/>
+    <cellStyle name="Normal 49 2 5" xfId="3105" xr:uid="{4DFF73C0-070A-4F6B-8928-5052FFFBD5DC}"/>
     <cellStyle name="Normal 49 3" xfId="2005" xr:uid="{049F4BEA-0C06-4129-947B-575F3F21ED78}"/>
     <cellStyle name="Normal 49 4" xfId="2055" xr:uid="{17958B43-E79B-4901-9FE3-F7F09DD6273F}"/>
     <cellStyle name="Normal 49 5" xfId="2108" xr:uid="{A039EBD6-D478-4119-94DE-4D03095F9375}"/>
@@ -5929,6 +6738,7 @@
     <cellStyle name="Normal 49 9" xfId="2322" xr:uid="{659BD9E2-9C06-4FA7-9BDD-7ED36884121B}"/>
     <cellStyle name="Normal 5" xfId="4" xr:uid="{7CC83B24-7AF4-4FD2-A509-1D73B7789011}"/>
     <cellStyle name="Normal 5 10" xfId="61" xr:uid="{9BCEDEA2-EBC7-4796-B33B-893EE691F6D3}"/>
+    <cellStyle name="Normal 5 100" xfId="3006" xr:uid="{882276C7-3481-4064-8DFC-4FE3E6CA35F8}"/>
     <cellStyle name="Normal 5 11" xfId="68" xr:uid="{1EB49392-9FFB-4FE5-BEC3-36B4D724CB67}"/>
     <cellStyle name="Normal 5 12" xfId="75" xr:uid="{7F2BA834-8382-417A-8BD1-1E7DB9E58142}"/>
     <cellStyle name="Normal 5 13" xfId="82" xr:uid="{7CC06B99-66EF-4592-8DEE-868837D8130E}"/>
@@ -5939,6 +6749,10 @@
     <cellStyle name="Normal 5 18" xfId="122" xr:uid="{1C2C2CC4-B1D0-4DE4-8503-C311716CF589}"/>
     <cellStyle name="Normal 5 19" xfId="130" xr:uid="{8B2F3349-F907-433D-8169-7629FEDE2CBA}"/>
     <cellStyle name="Normal 5 2" xfId="10" xr:uid="{FEF54BC1-F973-4B57-ABAF-38B83C725C7A}"/>
+    <cellStyle name="Normal 5 2 2" xfId="2718" xr:uid="{B6FC7524-8081-48C5-81F6-B513286704D5}"/>
+    <cellStyle name="Normal 5 2 3" xfId="2831" xr:uid="{5DD48EF6-FA17-40FC-97F0-53492476FEDD}"/>
+    <cellStyle name="Normal 5 2 4" xfId="2946" xr:uid="{11866CB4-2E95-483C-A0BD-EC5496ABC3DC}"/>
+    <cellStyle name="Normal 5 2 5" xfId="3061" xr:uid="{7ED7F035-4FB9-4AF9-AFF4-D2934E5E5356}"/>
     <cellStyle name="Normal 5 20" xfId="138" xr:uid="{593752D1-AC28-42B3-B6F6-704861D0CF96}"/>
     <cellStyle name="Normal 5 21" xfId="146" xr:uid="{8BE94E7C-4AED-45FC-8DE4-35D57B374544}"/>
     <cellStyle name="Normal 5 22" xfId="154" xr:uid="{60FB101F-006C-4D48-B5E6-E393EEA112B5}"/>
@@ -6023,13 +6837,24 @@
     <cellStyle name="Normal 5 94" xfId="2497" xr:uid="{BAA3D145-A84A-4E03-94FC-05B9F720FD9A}"/>
     <cellStyle name="Normal 5 95" xfId="2552" xr:uid="{4FE77182-375F-4D42-A41A-846285BFB9D6}"/>
     <cellStyle name="Normal 5 96" xfId="2607" xr:uid="{6F37AC54-F363-49A4-B837-9005DB98231B}"/>
+    <cellStyle name="Normal 5 97" xfId="2663" xr:uid="{B7899055-0AA6-4FCB-977B-7990A6AAAF7B}"/>
+    <cellStyle name="Normal 5 98" xfId="2776" xr:uid="{822710BA-CC7B-44C7-94E7-5D95D6717F37}"/>
+    <cellStyle name="Normal 5 99" xfId="2891" xr:uid="{01D25773-EE12-408E-8F36-33B10C412458}"/>
     <cellStyle name="Normal 50" xfId="1957" xr:uid="{F694FC52-4B0F-47E1-92DF-CD4D0A8F23AF}"/>
     <cellStyle name="Normal 50 10" xfId="2432" xr:uid="{2354729D-8ABA-4246-92CA-A3C324BC2D2A}"/>
     <cellStyle name="Normal 50 11" xfId="2487" xr:uid="{138B7319-971A-4BFF-B9A2-4FB00311A37F}"/>
     <cellStyle name="Normal 50 12" xfId="2542" xr:uid="{673A2782-1DD1-4B34-AA50-A418268828F0}"/>
     <cellStyle name="Normal 50 13" xfId="2597" xr:uid="{52EB8DB8-D289-4C7F-A347-25BFF8F032C9}"/>
     <cellStyle name="Normal 50 14" xfId="2652" xr:uid="{5B1EBE0D-4CBF-453E-B54A-8B3C3A213A70}"/>
+    <cellStyle name="Normal 50 15" xfId="2708" xr:uid="{7066061F-24CE-4E05-8038-F1474F6755C5}"/>
+    <cellStyle name="Normal 50 16" xfId="2821" xr:uid="{62B22B05-CFE7-42D9-A2E8-9636174DEBBC}"/>
+    <cellStyle name="Normal 50 17" xfId="2936" xr:uid="{BFE64B27-6C8D-49CF-B030-BD80ED1E888C}"/>
+    <cellStyle name="Normal 50 18" xfId="3051" xr:uid="{ED2839E2-8109-4056-82A9-7B182CDAF907}"/>
     <cellStyle name="Normal 50 2" xfId="2006" xr:uid="{5EA267D6-8E66-4747-B152-4678861E6E9C}"/>
+    <cellStyle name="Normal 50 2 2" xfId="2763" xr:uid="{81B28D78-2EFC-4C02-AC32-E97105C5EA5D}"/>
+    <cellStyle name="Normal 50 2 3" xfId="2876" xr:uid="{5DFD9FEA-4AA0-4DA1-BBAD-D9DF6089D6C4}"/>
+    <cellStyle name="Normal 50 2 4" xfId="2991" xr:uid="{A1A56CCF-E53B-495D-A999-70DAFDC92038}"/>
+    <cellStyle name="Normal 50 2 5" xfId="3106" xr:uid="{31B569FA-0B69-4084-8954-54D7F347DCBA}"/>
     <cellStyle name="Normal 50 3" xfId="2056" xr:uid="{94B7053D-F0C4-43EA-8BBD-E8EEE51A73B1}"/>
     <cellStyle name="Normal 50 4" xfId="2109" xr:uid="{27280868-ECF2-4D7D-8DEB-75C7CAA06413}"/>
     <cellStyle name="Normal 50 5" xfId="2162" xr:uid="{11026A6B-D9F7-4300-B399-08FDCE95969F}"/>
@@ -6042,7 +6867,15 @@
     <cellStyle name="Normal 51 11" xfId="2543" xr:uid="{602C832C-1E0E-4C8B-A86E-DFCC7C206A00}"/>
     <cellStyle name="Normal 51 12" xfId="2598" xr:uid="{3411D145-5D70-4277-9C19-98C1E7FBD1D2}"/>
     <cellStyle name="Normal 51 13" xfId="2653" xr:uid="{01F34818-BD22-4F8A-9D1A-DFADC559C11D}"/>
+    <cellStyle name="Normal 51 14" xfId="2709" xr:uid="{4D92EA6B-A907-42B8-8A4D-1CE09471FFEA}"/>
+    <cellStyle name="Normal 51 15" xfId="2822" xr:uid="{5CCC7DA3-7B45-49D8-9123-203847AB9D15}"/>
+    <cellStyle name="Normal 51 16" xfId="2937" xr:uid="{4B6DE4FC-961E-491A-973F-C426E9F7942F}"/>
+    <cellStyle name="Normal 51 17" xfId="3052" xr:uid="{1F110AF6-B890-49DA-89AF-C0062706DECF}"/>
     <cellStyle name="Normal 51 2" xfId="2057" xr:uid="{05B9550F-EDC2-4B34-8448-0CE71335699D}"/>
+    <cellStyle name="Normal 51 2 2" xfId="2764" xr:uid="{4C9CFF4E-CEA4-4DC5-81EF-A249B150FA92}"/>
+    <cellStyle name="Normal 51 2 3" xfId="2877" xr:uid="{D9CD33F3-1BBB-4F2D-AC48-C5D6E46AC13A}"/>
+    <cellStyle name="Normal 51 2 4" xfId="2992" xr:uid="{CD07054E-0F59-4B4A-A703-E49CFA1C4217}"/>
+    <cellStyle name="Normal 51 2 5" xfId="3107" xr:uid="{8EC80105-7902-41D3-9315-07CCA57D8557}"/>
     <cellStyle name="Normal 51 3" xfId="2110" xr:uid="{EEADDD94-46EB-4534-81FD-415BB9146977}"/>
     <cellStyle name="Normal 51 4" xfId="2163" xr:uid="{D49AB824-E1AD-412A-B267-FD7C3B6A5F1D}"/>
     <cellStyle name="Normal 51 5" xfId="2216" xr:uid="{D17E7BA8-3116-4F5F-8179-74E08399A4EF}"/>
@@ -6054,7 +6887,15 @@
     <cellStyle name="Normal 52 10" xfId="2544" xr:uid="{BA2FE816-9D57-4C39-8C1D-8FFD9462F1A2}"/>
     <cellStyle name="Normal 52 11" xfId="2599" xr:uid="{48869502-3B3C-4D2E-A9D4-F18D8144C2A4}"/>
     <cellStyle name="Normal 52 12" xfId="2654" xr:uid="{C87CF75B-EF7C-45CB-9521-97307C655F76}"/>
+    <cellStyle name="Normal 52 13" xfId="2710" xr:uid="{EC5DBB74-722A-4017-AB71-243D46BEEE2D}"/>
+    <cellStyle name="Normal 52 14" xfId="2823" xr:uid="{62D6C938-0F0F-45F1-8795-884EC5CCC403}"/>
+    <cellStyle name="Normal 52 15" xfId="2938" xr:uid="{26978246-7240-440A-B7DD-B0D6B688975C}"/>
+    <cellStyle name="Normal 52 16" xfId="3053" xr:uid="{FE7F4830-6CC6-4C3A-85EA-FA84ECDEAA75}"/>
     <cellStyle name="Normal 52 2" xfId="2111" xr:uid="{2C609632-C4ED-40F2-8062-2BB9333D71A1}"/>
+    <cellStyle name="Normal 52 2 2" xfId="2765" xr:uid="{47551841-98A6-4862-AEC0-0B141E853C18}"/>
+    <cellStyle name="Normal 52 2 3" xfId="2878" xr:uid="{E00952A2-B560-4D26-8483-ED5EA4AF645F}"/>
+    <cellStyle name="Normal 52 2 4" xfId="2993" xr:uid="{60DC0D07-4FA9-40D4-B555-618169F885C4}"/>
+    <cellStyle name="Normal 52 2 5" xfId="3108" xr:uid="{3E0318B7-3D23-4086-893A-EC9A8BFE83A2}"/>
     <cellStyle name="Normal 52 3" xfId="2164" xr:uid="{38502271-BE6F-47FA-9158-64F5F05DCB08}"/>
     <cellStyle name="Normal 52 4" xfId="2217" xr:uid="{BB0FA74F-2845-479E-940A-6418FF10EDEA}"/>
     <cellStyle name="Normal 52 5" xfId="2271" xr:uid="{7EDE6A6E-6245-40E0-AAE7-27AB621DE21E}"/>
@@ -6066,7 +6907,15 @@
     <cellStyle name="Normal 53 10" xfId="2545" xr:uid="{8C6530DA-41F7-4571-80BF-CE550551732B}"/>
     <cellStyle name="Normal 53 11" xfId="2600" xr:uid="{63BC088F-798F-4007-A069-AB104C765385}"/>
     <cellStyle name="Normal 53 12" xfId="2655" xr:uid="{2CAF221B-D2F4-4F52-AAA8-12F076279079}"/>
+    <cellStyle name="Normal 53 13" xfId="2711" xr:uid="{F53458BF-836A-43AD-89E0-D71A6FEF91B6}"/>
+    <cellStyle name="Normal 53 14" xfId="2824" xr:uid="{D60D9C08-84AE-4D95-A611-0A469D061D7D}"/>
+    <cellStyle name="Normal 53 15" xfId="2939" xr:uid="{FAD9E380-9D95-4B2C-A0FD-3E02EDA380FC}"/>
+    <cellStyle name="Normal 53 16" xfId="3054" xr:uid="{FBB03957-08D9-48E8-B57B-FFE291511DCE}"/>
     <cellStyle name="Normal 53 2" xfId="2112" xr:uid="{16C62648-6EA8-4037-9ED8-095F822FF00A}"/>
+    <cellStyle name="Normal 53 2 2" xfId="2766" xr:uid="{0F621B8D-7BC2-496E-8C38-A20F2CB1D093}"/>
+    <cellStyle name="Normal 53 2 3" xfId="2879" xr:uid="{D5B7CFD1-B94C-405B-B0E7-C383323491DB}"/>
+    <cellStyle name="Normal 53 2 4" xfId="2994" xr:uid="{E6C531F0-F0C9-4F22-BCA8-BC5C4F5C9C55}"/>
+    <cellStyle name="Normal 53 2 5" xfId="3109" xr:uid="{AF98381E-76D2-41D7-901D-62644DEAA200}"/>
     <cellStyle name="Normal 53 3" xfId="2165" xr:uid="{06B1AB3E-FD03-476B-ABB1-E3CA9C13FD86}"/>
     <cellStyle name="Normal 53 4" xfId="2218" xr:uid="{3C01CD0D-BB46-489D-BB4D-0F40A7561659}"/>
     <cellStyle name="Normal 53 5" xfId="2272" xr:uid="{9A948023-87A5-454D-B748-B968765580AB}"/>
@@ -6078,7 +6927,15 @@
     <cellStyle name="Normal 54 10" xfId="2546" xr:uid="{506FFD66-3A0A-4238-96D3-4AFFA4C56879}"/>
     <cellStyle name="Normal 54 11" xfId="2601" xr:uid="{1EBEAD19-BB8E-4118-A3D6-E322867DDD06}"/>
     <cellStyle name="Normal 54 12" xfId="2656" xr:uid="{6237C52D-F099-4572-9D05-82FB1661022A}"/>
+    <cellStyle name="Normal 54 13" xfId="2712" xr:uid="{BFEC8FE3-E64E-4FD2-B6FD-0D26CDAB1723}"/>
+    <cellStyle name="Normal 54 14" xfId="2825" xr:uid="{D61D4DBB-A5C9-49D8-BD30-65A369D0E93C}"/>
+    <cellStyle name="Normal 54 15" xfId="2940" xr:uid="{FFC46046-2659-4254-B361-DD02A8A455FF}"/>
+    <cellStyle name="Normal 54 16" xfId="3055" xr:uid="{A3FA7369-2FBA-4628-8C1F-32EBD79830A2}"/>
     <cellStyle name="Normal 54 2" xfId="2113" xr:uid="{52C4B073-4C53-40E7-A256-18B3D9AD7A02}"/>
+    <cellStyle name="Normal 54 2 2" xfId="2767" xr:uid="{6919D4F1-EDD6-4982-A32C-B1BF7D60770E}"/>
+    <cellStyle name="Normal 54 2 3" xfId="2880" xr:uid="{A44C0C1A-9E33-4423-BB85-940DA0D39668}"/>
+    <cellStyle name="Normal 54 2 4" xfId="2995" xr:uid="{1444F21B-92EE-4AEE-91E7-9B974546AF1D}"/>
+    <cellStyle name="Normal 54 2 5" xfId="3110" xr:uid="{9BCD3E9F-F37F-42D0-B2EA-E059C8CD8CAA}"/>
     <cellStyle name="Normal 54 3" xfId="2166" xr:uid="{5464CF50-21BE-4C16-B689-EB526957E877}"/>
     <cellStyle name="Normal 54 4" xfId="2219" xr:uid="{DFDA0EC6-330A-4F76-B02D-67ECB9E2963B}"/>
     <cellStyle name="Normal 54 5" xfId="2273" xr:uid="{644BA510-66C4-42CC-A3EC-7F9DAFD552F7}"/>
@@ -6087,7 +6944,15 @@
     <cellStyle name="Normal 54 8" xfId="2436" xr:uid="{B7883CF5-9F52-4891-BAA2-505887CBE3B9}"/>
     <cellStyle name="Normal 54 9" xfId="2491" xr:uid="{CE13531C-89CA-4088-A71C-09946268A9C5}"/>
     <cellStyle name="Normal 55" xfId="2220" xr:uid="{F2DBE977-3055-4B8C-8DB1-9063802CB3CE}"/>
+    <cellStyle name="Normal 55 10" xfId="2713" xr:uid="{F24B3582-21FD-4D7C-864A-3BA728F5F670}"/>
+    <cellStyle name="Normal 55 11" xfId="2826" xr:uid="{3DADC277-9263-43AE-9171-059F2FCCE580}"/>
+    <cellStyle name="Normal 55 12" xfId="2941" xr:uid="{1B8E9511-C145-4B6F-8874-487E5798F01D}"/>
+    <cellStyle name="Normal 55 13" xfId="3056" xr:uid="{4751B14E-4D7F-4EAD-B1F0-ECBDD4BF153F}"/>
     <cellStyle name="Normal 55 2" xfId="2274" xr:uid="{2AFC1409-514C-44F8-A16A-009B4AAA5942}"/>
+    <cellStyle name="Normal 55 2 2" xfId="2768" xr:uid="{BB3F96DF-C660-45E6-A748-212719977B74}"/>
+    <cellStyle name="Normal 55 2 3" xfId="2881" xr:uid="{21F533F1-5BB2-4550-AC04-658780E8C2F0}"/>
+    <cellStyle name="Normal 55 2 4" xfId="2996" xr:uid="{369CA73A-0D1A-4064-94F1-83A71F244D47}"/>
+    <cellStyle name="Normal 55 2 5" xfId="3111" xr:uid="{947FDDEA-BB62-4F5B-947C-FB9322CA11D2}"/>
     <cellStyle name="Normal 55 3" xfId="2328" xr:uid="{1779E91A-B6EE-4CCD-A0AA-3104AAC79AD1}"/>
     <cellStyle name="Normal 55 4" xfId="2382" xr:uid="{82A622E9-AAF1-4266-998C-63CC070A21C0}"/>
     <cellStyle name="Normal 55 5" xfId="2437" xr:uid="{A3132FCE-3118-4D83-BD66-780B5BB8B4B9}"/>
@@ -6096,13 +6961,35 @@
     <cellStyle name="Normal 55 8" xfId="2602" xr:uid="{3F7D91E9-8E15-4C2B-AD8B-54544E42ED39}"/>
     <cellStyle name="Normal 55 9" xfId="2657" xr:uid="{2332CC96-CAB7-4C4F-AB22-1982EB42FB84}"/>
     <cellStyle name="Normal 56" xfId="2383" xr:uid="{A9CCEEB6-8E80-47DA-918C-160799DDECFE}"/>
+    <cellStyle name="Normal 56 10" xfId="3057" xr:uid="{4ABDAC8C-9ED1-4008-9251-69117E6053A2}"/>
     <cellStyle name="Normal 56 2" xfId="2438" xr:uid="{EA476B24-9472-4541-8F5A-FCAE56DDBF2E}"/>
+    <cellStyle name="Normal 56 2 2" xfId="2769" xr:uid="{3817D2A4-2133-4B7D-9F80-F26F5A537FD5}"/>
+    <cellStyle name="Normal 56 2 3" xfId="2882" xr:uid="{46F0EA8A-82C1-4D67-AA61-36E901EB20D4}"/>
+    <cellStyle name="Normal 56 2 4" xfId="2997" xr:uid="{27CA23FE-DDFB-46A8-8CDC-D05BE071439D}"/>
+    <cellStyle name="Normal 56 2 5" xfId="3112" xr:uid="{B5B20243-AB44-4D03-8952-7056E375D117}"/>
     <cellStyle name="Normal 56 3" xfId="2493" xr:uid="{6EB1B442-4D38-4DA0-BE5C-8BDA89B86CB0}"/>
     <cellStyle name="Normal 56 4" xfId="2548" xr:uid="{C4EF64E2-6B10-47A6-AC84-1B2E1223A04A}"/>
     <cellStyle name="Normal 56 5" xfId="2603" xr:uid="{3A0B3AB3-F81A-4C14-8937-2F0F8CBDCCCB}"/>
     <cellStyle name="Normal 56 6" xfId="2658" xr:uid="{E700C0E4-3C35-479B-B321-E16FD5A757F6}"/>
+    <cellStyle name="Normal 56 7" xfId="2714" xr:uid="{19720FFA-9187-4EF0-AFF9-770A6DA0A23B}"/>
+    <cellStyle name="Normal 56 8" xfId="2827" xr:uid="{FFB364F3-F264-40D2-B2F1-CB1AC57490E5}"/>
+    <cellStyle name="Normal 56 9" xfId="2942" xr:uid="{08FBC483-7A0C-48A4-8065-0E7931C0300C}"/>
+    <cellStyle name="Normal 57" xfId="2659" xr:uid="{69F06C49-2B52-4C63-80D0-59334892E300}"/>
+    <cellStyle name="Normal 57 2" xfId="2770" xr:uid="{FF9E013C-0864-4C29-AAC2-A9F605BA4622}"/>
+    <cellStyle name="Normal 57 3" xfId="2883" xr:uid="{7365D6CE-51D2-4A58-B665-4E342F0C3813}"/>
+    <cellStyle name="Normal 57 4" xfId="2998" xr:uid="{010973C8-A721-4F1F-8A66-CF41A6A21771}"/>
+    <cellStyle name="Normal 57 5" xfId="3113" xr:uid="{95BEC7D6-4B56-4E4A-9243-687D8ECC158A}"/>
+    <cellStyle name="Normal 58" xfId="2771" xr:uid="{6D64905C-C3A3-4F15-93FB-6C06332B37FC}"/>
+    <cellStyle name="Normal 58 2" xfId="2884" xr:uid="{E52A950C-97D4-46A5-85F8-48BBCF45C741}"/>
+    <cellStyle name="Normal 58 3" xfId="2999" xr:uid="{9BFD70A9-300C-471C-8693-C9C097D8024A}"/>
+    <cellStyle name="Normal 58 4" xfId="3114" xr:uid="{1AC950F1-FD75-4511-891B-E50B9D738FF9}"/>
+    <cellStyle name="Normal 59" xfId="2772" xr:uid="{41D40870-0752-4240-AA2C-97D6E713F61A}"/>
+    <cellStyle name="Normal 59 2" xfId="2885" xr:uid="{2B3A650E-3D45-4836-85E5-408B126A8D49}"/>
+    <cellStyle name="Normal 59 3" xfId="3000" xr:uid="{4AD9557B-3727-409F-A7E2-CEFD068F8B2A}"/>
+    <cellStyle name="Normal 59 4" xfId="3115" xr:uid="{BFD73127-522F-4348-816C-6772594DC5DC}"/>
     <cellStyle name="Normal 6" xfId="5" xr:uid="{31BE2080-B222-435D-8A48-DEEADDEF6488}"/>
     <cellStyle name="Normal 6 10" xfId="62" xr:uid="{F76AEC00-2B15-423C-8653-788DAF9DBB9C}"/>
+    <cellStyle name="Normal 6 100" xfId="3007" xr:uid="{43CD87CB-663B-4165-9AC1-B50B2A163F84}"/>
     <cellStyle name="Normal 6 11" xfId="69" xr:uid="{69EF0E4C-7EAA-4CE4-BF59-7EC105A17AD6}"/>
     <cellStyle name="Normal 6 12" xfId="76" xr:uid="{51E53339-1CE3-41E8-B360-5327A09FCEEF}"/>
     <cellStyle name="Normal 6 13" xfId="83" xr:uid="{46C044AC-8612-44BB-B270-978285A0DB33}"/>
@@ -6113,6 +7000,10 @@
     <cellStyle name="Normal 6 18" xfId="123" xr:uid="{8C66F3E6-B6A4-4416-8CBC-269F13AFACAD}"/>
     <cellStyle name="Normal 6 19" xfId="131" xr:uid="{13957F89-95C6-41D0-8BD7-53CCC2BC7F9F}"/>
     <cellStyle name="Normal 6 2" xfId="11" xr:uid="{EE7A43B0-A7DC-4E32-8BB1-1015A418FBC2}"/>
+    <cellStyle name="Normal 6 2 2" xfId="2719" xr:uid="{8D8F23EF-A909-4F7C-A950-2524AA6B0FE7}"/>
+    <cellStyle name="Normal 6 2 3" xfId="2832" xr:uid="{AC1C4E3E-366C-4557-9C08-747A74435E93}"/>
+    <cellStyle name="Normal 6 2 4" xfId="2947" xr:uid="{12911D3B-7636-4EBF-AC19-C3868227E78D}"/>
+    <cellStyle name="Normal 6 2 5" xfId="3062" xr:uid="{411BFA69-322E-4376-AAC5-90B98D07C0C0}"/>
     <cellStyle name="Normal 6 20" xfId="139" xr:uid="{83F55AAD-0832-49CB-AA11-0C67B1415416}"/>
     <cellStyle name="Normal 6 21" xfId="147" xr:uid="{7BE834A1-F5A4-487E-9EE4-A360DAEF9B02}"/>
     <cellStyle name="Normal 6 22" xfId="155" xr:uid="{DEB52F5D-4671-4504-8B9C-992037572D14}"/>
@@ -6197,8 +7088,18 @@
     <cellStyle name="Normal 6 94" xfId="2498" xr:uid="{47FD3778-BDE7-4B81-85DC-C40989C808B6}"/>
     <cellStyle name="Normal 6 95" xfId="2553" xr:uid="{2D64A2C1-ACA0-46A6-8978-38AE9C3F0541}"/>
     <cellStyle name="Normal 6 96" xfId="2608" xr:uid="{DD4C3072-729B-4CDD-B99B-CC3C38B280EA}"/>
+    <cellStyle name="Normal 6 97" xfId="2664" xr:uid="{FCD124A4-C326-4B8D-A68E-7F837B6DC57B}"/>
+    <cellStyle name="Normal 6 98" xfId="2777" xr:uid="{31700988-83D3-4251-920C-08301E638EEF}"/>
+    <cellStyle name="Normal 6 99" xfId="2892" xr:uid="{D35873D3-BE9A-46D2-B412-E97198CE0B21}"/>
+    <cellStyle name="Normal 60" xfId="2886" xr:uid="{231DD928-CDC8-4186-BDC6-65C7A86A95F0}"/>
+    <cellStyle name="Normal 60 2" xfId="3001" xr:uid="{768CAF8E-526A-460A-ABDC-40FC598FE120}"/>
+    <cellStyle name="Normal 60 3" xfId="3116" xr:uid="{CFA19106-0817-4FF6-BEDF-7B6AAAB93D91}"/>
+    <cellStyle name="Normal 61" xfId="2887" xr:uid="{09E504F5-62E4-4475-B42C-6E495D277A70}"/>
+    <cellStyle name="Normal 61 2" xfId="3002" xr:uid="{6A2E9478-A057-45F4-9CB7-DA82F6C45B2C}"/>
+    <cellStyle name="Normal 61 3" xfId="3117" xr:uid="{B1B3B667-3668-4498-B628-B9DDC56CFAE0}"/>
     <cellStyle name="Normal 7" xfId="6" xr:uid="{8FDF4D0E-5067-42C1-8AB6-21A2DD8B8199}"/>
     <cellStyle name="Normal 7 10" xfId="63" xr:uid="{076EEBFE-E343-48C7-AD51-40C5F37875B2}"/>
+    <cellStyle name="Normal 7 100" xfId="3008" xr:uid="{2D210E16-B1D0-4A19-9809-7615CFFCA901}"/>
     <cellStyle name="Normal 7 11" xfId="70" xr:uid="{C92A195D-1E83-4EB3-9856-15A82899A737}"/>
     <cellStyle name="Normal 7 12" xfId="77" xr:uid="{B7ABE029-148A-4F51-8D74-38CBB930BB27}"/>
     <cellStyle name="Normal 7 13" xfId="84" xr:uid="{80BAE901-0CCF-4E94-9A96-E850985EEF4A}"/>
@@ -6209,6 +7110,10 @@
     <cellStyle name="Normal 7 18" xfId="124" xr:uid="{1184332C-C894-4211-8FC0-4ABAB48A0F64}"/>
     <cellStyle name="Normal 7 19" xfId="132" xr:uid="{C26E41C3-8A45-4F8E-B61D-007CE8B88A3A}"/>
     <cellStyle name="Normal 7 2" xfId="12" xr:uid="{92B06EF3-B29D-4105-BC3E-CA07D1A85031}"/>
+    <cellStyle name="Normal 7 2 2" xfId="2720" xr:uid="{42D0122C-6DCA-4B2C-985F-FA86975B8E6F}"/>
+    <cellStyle name="Normal 7 2 3" xfId="2833" xr:uid="{E93C05B3-3A76-427C-9F3F-20439CE6ED1F}"/>
+    <cellStyle name="Normal 7 2 4" xfId="2948" xr:uid="{A84A458F-32A7-4B52-AF28-01F00C145A57}"/>
+    <cellStyle name="Normal 7 2 5" xfId="3063" xr:uid="{A852DAAA-4490-4F35-BACF-009A3F667B0B}"/>
     <cellStyle name="Normal 7 20" xfId="140" xr:uid="{6586C4A1-177E-4E42-9EDF-AC67397DFB64}"/>
     <cellStyle name="Normal 7 21" xfId="148" xr:uid="{B512CF68-AA41-4DA0-B8CB-C4FA006BAE0F}"/>
     <cellStyle name="Normal 7 22" xfId="156" xr:uid="{0D823CEF-5D1C-47F8-AB46-63A1A6FEF837}"/>
@@ -6293,6 +7198,9 @@
     <cellStyle name="Normal 7 94" xfId="2499" xr:uid="{C123C8E0-A08F-4E26-9A73-77BA00C8621B}"/>
     <cellStyle name="Normal 7 95" xfId="2554" xr:uid="{DE55F490-1530-4336-9520-0F427D50F2C5}"/>
     <cellStyle name="Normal 7 96" xfId="2609" xr:uid="{016B4DC6-8175-41FB-88EE-1C6A602C4928}"/>
+    <cellStyle name="Normal 7 97" xfId="2665" xr:uid="{AEDD4587-9602-4575-93C9-B3035959340E}"/>
+    <cellStyle name="Normal 7 98" xfId="2778" xr:uid="{4C893E68-3907-4721-B998-210003BD0CE6}"/>
+    <cellStyle name="Normal 7 99" xfId="2893" xr:uid="{74C3B876-6659-495A-B5D8-DD55AD43D21D}"/>
     <cellStyle name="Normal 8" xfId="43" xr:uid="{B3C5BFDC-2A95-4E6A-803F-B149318E48CC}"/>
     <cellStyle name="Normal 8 10" xfId="109" xr:uid="{2C5F0F9A-3251-494A-998A-DF2DB5E1065F}"/>
     <cellStyle name="Normal 8 11" xfId="117" xr:uid="{A66804B5-EC5B-4C85-82CD-D00400FFCA77}"/>
@@ -6305,6 +7213,10 @@
     <cellStyle name="Normal 8 18" xfId="176" xr:uid="{5998FFEB-065A-4BC0-8B7A-A1918DF653F6}"/>
     <cellStyle name="Normal 8 19" xfId="187" xr:uid="{0F99986F-5A9F-4C64-8635-A44C2DDE7695}"/>
     <cellStyle name="Normal 8 2" xfId="50" xr:uid="{5B471B36-FCA9-4C5F-A59A-4945AE0E7C2E}"/>
+    <cellStyle name="Normal 8 2 2" xfId="2721" xr:uid="{C093AEF2-A1A2-407C-9632-1FF5FC0E9C31}"/>
+    <cellStyle name="Normal 8 2 3" xfId="2834" xr:uid="{32F52DB6-D8C7-4675-B57D-79454A58E416}"/>
+    <cellStyle name="Normal 8 2 4" xfId="2949" xr:uid="{AFC62757-4B45-413B-9237-D2C455F37438}"/>
+    <cellStyle name="Normal 8 2 5" xfId="3064" xr:uid="{0EDC1BD9-7D0C-4C87-BD61-E3E8C6A59480}"/>
     <cellStyle name="Normal 8 20" xfId="199" xr:uid="{6C4AD662-49D3-4EEB-99F5-FE3AE08EF33B}"/>
     <cellStyle name="Normal 8 21" xfId="212" xr:uid="{4B287179-427A-4EE3-8500-50FC7926EAD3}"/>
     <cellStyle name="Normal 8 22" xfId="226" xr:uid="{EF1D0439-8208-4AC0-BA51-E4573BA4D5C6}"/>
@@ -6383,6 +7295,10 @@
     <cellStyle name="Normal 8 89" xfId="2555" xr:uid="{F6C155A5-4017-4361-8DB6-AF51C97C6BB4}"/>
     <cellStyle name="Normal 8 9" xfId="101" xr:uid="{EF361D85-BD7F-4E58-9FE7-65473E5583EE}"/>
     <cellStyle name="Normal 8 90" xfId="2610" xr:uid="{B10BCBE7-C417-4176-B770-6D4AF5496FDE}"/>
+    <cellStyle name="Normal 8 91" xfId="2666" xr:uid="{62C7ADEB-2011-46EB-B115-53FC7779FA87}"/>
+    <cellStyle name="Normal 8 92" xfId="2779" xr:uid="{FAFC4743-91B5-4402-95DB-808CCB159EAB}"/>
+    <cellStyle name="Normal 8 93" xfId="2894" xr:uid="{3C748DED-802C-480A-9A50-BB5877D69462}"/>
+    <cellStyle name="Normal 8 94" xfId="3009" xr:uid="{BCA7A4B8-C5A7-42C2-A1B9-95585425A2D3}"/>
     <cellStyle name="Normal 9" xfId="86" xr:uid="{63C162E7-EB2C-460C-8F1B-D9BC4CBB1C65}"/>
     <cellStyle name="Normal 9 10" xfId="158" xr:uid="{EA44C88E-C9B8-4EDC-99A4-D9EF32DAD79D}"/>
     <cellStyle name="Normal 9 11" xfId="167" xr:uid="{361119E1-3FCE-4102-8A43-24B6D72873F7}"/>
@@ -6395,6 +7311,10 @@
     <cellStyle name="Normal 9 18" xfId="258" xr:uid="{8042C5AC-6E40-4E60-A5C4-4DE15BDE8C6D}"/>
     <cellStyle name="Normal 9 19" xfId="275" xr:uid="{956C79FE-7B8F-4A97-A621-05D42593E9CD}"/>
     <cellStyle name="Normal 9 2" xfId="94" xr:uid="{9ED2EE7C-53E9-4653-AC47-18DB6F004BB3}"/>
+    <cellStyle name="Normal 9 2 2" xfId="2722" xr:uid="{1356CC68-60FF-45DE-933C-D60DFD22B41C}"/>
+    <cellStyle name="Normal 9 2 3" xfId="2835" xr:uid="{905FF622-8A3F-433C-AD3B-C91469B8B36F}"/>
+    <cellStyle name="Normal 9 2 4" xfId="2950" xr:uid="{C72CA34D-6C99-4395-8812-9FB62FE5AE86}"/>
+    <cellStyle name="Normal 9 2 5" xfId="3065" xr:uid="{9F55F413-4A10-4EE9-9324-F71349501F45}"/>
     <cellStyle name="Normal 9 20" xfId="293" xr:uid="{5994B785-D88C-4C07-9D30-95B3E54405FB}"/>
     <cellStyle name="Normal 9 21" xfId="312" xr:uid="{E2690F61-2E76-4BEB-91D4-55F120CAF545}"/>
     <cellStyle name="Normal 9 22" xfId="332" xr:uid="{13ACC2A3-59E3-450A-9E75-F0E8590D8BF8}"/>
@@ -6466,6 +7386,10 @@
     <cellStyle name="Normal 9 82" xfId="2501" xr:uid="{9C379A32-672A-4123-9C85-292B6C63FB20}"/>
     <cellStyle name="Normal 9 83" xfId="2556" xr:uid="{4058EEFE-43E1-4197-B4FE-D2D046E6A8B2}"/>
     <cellStyle name="Normal 9 84" xfId="2611" xr:uid="{516B1A08-7F68-4A1B-BB56-F4DAAE27CD74}"/>
+    <cellStyle name="Normal 9 85" xfId="2667" xr:uid="{0786D930-F29A-40A0-A43D-81817C0B34F7}"/>
+    <cellStyle name="Normal 9 86" xfId="2780" xr:uid="{AC421633-824E-4DAF-AE32-BC88808046A7}"/>
+    <cellStyle name="Normal 9 87" xfId="2895" xr:uid="{A7AF6B67-2D48-4A4C-9D6A-7B452CCC2B29}"/>
+    <cellStyle name="Normal 9 88" xfId="3010" xr:uid="{93985147-5550-48E3-A801-C0CC8A7F5E93}"/>
     <cellStyle name="Normal 9 9" xfId="150" xr:uid="{5810B583-F0FF-4873-A2AE-BF7471C0EA6E}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6769,7 +7693,7 @@
   <dimension ref="A1:CD16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7055,7 +7979,7 @@
       </c>
     </row>
     <row r="2" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C2" t="s">
@@ -7068,7 +7992,7 @@
         <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
         <v>87</v>
@@ -7083,215 +8007,156 @@
         <v>90</v>
       </c>
       <c r="T2" s="3">
-        <v>5610</v>
-      </c>
-      <c r="V2" s="2">
-        <v>44562</v>
-      </c>
-      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="AB2" t="s">
         <v>91</v>
       </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>92</v>
       </c>
       <c r="AH2" t="s">
         <v>93</v>
       </c>
+      <c r="AI2" t="s">
+        <v>94</v>
+      </c>
       <c r="AK2" s="2">
-        <v>33136</v>
-      </c>
-      <c r="AL2" s="2"/>
-      <c r="AT2" s="7"/>
+        <v>29589</v>
+      </c>
+      <c r="AL2" s="2">
+        <v>31011</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>89</v>
+      </c>
       <c r="AV2" t="s">
         <v>82</v>
       </c>
-      <c r="AX2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ2"/>
-      <c r="BA2"/>
       <c r="BD2" t="s">
         <v>87</v>
       </c>
       <c r="BE2" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>97</v>
       </c>
       <c r="BQ2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="BY2" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>99</v>
       </c>
       <c r="CD2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>96</v>
+      <c r="A3" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
         <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="N3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="P3" t="s">
+        <v>105</v>
       </c>
       <c r="T3" s="3">
-        <v>497</v>
-      </c>
-      <c r="V3" s="2">
-        <v>44713</v>
-      </c>
-      <c r="W3" t="s">
-        <v>102</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
+        <v>17497</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3"/>
+      <c r="X3"/>
       <c r="AB3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="AC3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>30658</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>34769</v>
+      </c>
+      <c r="AT3" t="s">
         <v>104</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK3" s="2">
-        <v>28183</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>29090</v>
       </c>
       <c r="AV3" t="s">
         <v>82</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>100</v>
       </c>
       <c r="AZ3"/>
       <c r="BA3"/>
       <c r="BD3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="BE3" t="s">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>111</v>
       </c>
       <c r="BQ3" t="s">
         <v>82</v>
       </c>
-      <c r="BY3" t="s">
-        <v>107</v>
+      <c r="BY3" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="BZ3" t="s">
-        <v>108</v>
-      </c>
-      <c r="CD3" t="s">
-        <v>107</v>
+        <v>113</v>
+      </c>
+      <c r="CD3" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" t="s">
-        <v>111</v>
-      </c>
-      <c r="N4" t="s">
-        <v>112</v>
-      </c>
-      <c r="O4" t="s">
-        <v>113</v>
-      </c>
-      <c r="P4" t="s">
-        <v>114</v>
-      </c>
-      <c r="T4" s="3">
-        <v>1750</v>
-      </c>
-      <c r="V4" t="s">
-        <v>115</v>
-      </c>
-      <c r="W4" t="s">
-        <v>116</v>
-      </c>
-      <c r="X4">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK4" s="2">
-        <v>32902</v>
-      </c>
+      <c r="T4" s="3"/>
+      <c r="V4" s="2"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="AK4" s="2"/>
       <c r="AL4" s="2"/>
-      <c r="AV4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>113</v>
-      </c>
       <c r="AZ4"/>
       <c r="BA4"/>
-      <c r="BD4" t="s">
-        <v>111</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>119</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>83</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>120</v>
-      </c>
-      <c r="CD4" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="T5" s="3"/>
-      <c r="V5"/>
+      <c r="V5" s="2"/>
       <c r="W5"/>
       <c r="X5"/>
       <c r="AK5" s="2"/>
@@ -7313,6 +8178,9 @@
     <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="T7" s="3"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
       <c r="AZ7"/>
@@ -7353,17 +8221,20 @@
     </row>
     <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="T11" s="5"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
+      <c r="T11" s="3"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
       <c r="AZ11"/>
       <c r="BA11"/>
     </row>
     <row r="12" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
       <c r="T12" s="3"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
       <c r="AZ12"/>
       <c r="BA12"/>
     </row>
@@ -7401,5 +8272,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>